<commit_message>
Fixed East FoCo result
</commit_message>
<xml_diff>
--- a/database_working.xlsx
+++ b/database_working.xlsx
@@ -3249,9 +3249,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BL188"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AP1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V70" sqref="V70"/>
+      <selection pane="bottomLeft" activeCell="BF2" sqref="BF2:BF187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3271,7 +3271,8 @@
     <col min="53" max="53" width="10.140625" style="1" customWidth="1"/>
     <col min="54" max="56" width="9.140625" style="1"/>
     <col min="57" max="57" width="53.5703125" style="1" customWidth="1"/>
-    <col min="58" max="16384" width="9.140625" style="1"/>
+    <col min="58" max="58" width="19.42578125" style="1" customWidth="1"/>
+    <col min="59" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3633,7 +3634,7 @@
         <v>easy med sfoco kid</v>
       </c>
       <c r="BF2" s="1" t="str">
-        <f>IF(C2="old","Old Town",IF(C2="campus","Near Campus",IF(C2="sfoco","South Foco",IF(C2="nfoco","North Foco",IF(C2="midtown","Midtown",IF(C2="cwest","Campus West",IF(C2="efoco","East FoCo,""")))))))</f>
+        <f>IF(C2="old","Old Town",IF(C2="campus","Near Campus",IF(C2="sfoco","South Foco",IF(C2="nfoco","North Foco",IF(C2="midtown","Midtown",IF(C2="cwest","Campus West",IF(C2="efoco","East FoCo","")))))))</f>
         <v>South Foco</v>
       </c>
       <c r="BG2" s="1">
@@ -3851,7 +3852,7 @@
         <v>hard med old</v>
       </c>
       <c r="BF3" s="1" t="str">
-        <f t="shared" ref="BF3:BF66" si="50">IF(C3="old","Old Town",IF(C3="campus","Near Campus",IF(C3="sfoco","South Foco",IF(C3="nfoco","North Foco",IF(C3="midtown","Midtown",IF(C3="cwest","Campus West",IF(C3="efoco","East FoCo,""")))))))</f>
+        <f t="shared" ref="BF3:BF66" si="50">IF(C3="old","Old Town",IF(C3="campus","Near Campus",IF(C3="sfoco","South Foco",IF(C3="nfoco","North Foco",IF(C3="midtown","Midtown",IF(C3="cwest","Campus West",IF(C3="efoco","East FoCo","")))))))</f>
         <v>Old Town</v>
       </c>
       <c r="BG3" s="1">
@@ -15629,7 +15630,7 @@
         <v>drink food easy low sfoco</v>
       </c>
       <c r="BF67" s="1" t="str">
-        <f t="shared" ref="BF67:BF130" si="114">IF(C67="old","Old Town",IF(C67="campus","Near Campus",IF(C67="sfoco","South Foco",IF(C67="nfoco","North Foco",IF(C67="midtown","Midtown",IF(C67="cwest","Campus West",IF(C67="efoco","East FoCo,""")))))))</f>
+        <f t="shared" ref="BF67:BF130" si="114">IF(C67="old","Old Town",IF(C67="campus","Near Campus",IF(C67="sfoco","South Foco",IF(C67="nfoco","North Foco",IF(C67="midtown","Midtown",IF(C67="cwest","Campus West",IF(C67="efoco","East FoCo","")))))))</f>
         <v>South Foco</v>
       </c>
       <c r="BG67" s="1">
@@ -16333,7 +16334,7 @@
       </c>
       <c r="BF71" s="1" t="str">
         <f t="shared" si="114"/>
-        <v>East FoCo,"</v>
+        <v>East FoCo</v>
       </c>
       <c r="BG71" s="1">
         <v>40.581789000000001</v>
@@ -27246,7 +27247,7 @@
         <v>outdoor hard med old</v>
       </c>
       <c r="BF131" s="1" t="str">
-        <f t="shared" ref="BF131:BF187" si="157">IF(C131="old","Old Town",IF(C131="campus","Near Campus",IF(C131="sfoco","South Foco",IF(C131="nfoco","North Foco",IF(C131="midtown","Midtown",IF(C131="cwest","Campus West",IF(C131="efoco","East FoCo,""")))))))</f>
+        <f t="shared" ref="BF131:BF187" si="157">IF(C131="old","Old Town",IF(C131="campus","Near Campus",IF(C131="sfoco","South Foco",IF(C131="nfoco","North Foco",IF(C131="midtown","Midtown",IF(C131="cwest","Campus West",IF(C131="efoco","East FoCo","")))))))</f>
         <v>Old Town</v>
       </c>
       <c r="BG131" s="1">
@@ -30871,9 +30872,9 @@
         <f t="shared" si="154"/>
         <v xml:space="preserve">easy med </v>
       </c>
-      <c r="BF151" s="1" t="b">
+      <c r="BF151" s="1" t="str">
         <f t="shared" si="157"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BG151" s="1">
         <v>40.582129999999999</v>
@@ -35985,9 +35986,9 @@
         <f t="shared" si="154"/>
         <v xml:space="preserve">easy med </v>
       </c>
-      <c r="BF180" s="1" t="b">
+      <c r="BF180" s="1" t="str">
         <f t="shared" si="157"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="BG180" s="1">
         <v>40.552579999999999</v>

</xml_diff>

<commit_message>
Updated content. Revised CSS to better display on iPads. Fixed Amenties spelling
</commit_message>
<xml_diff>
--- a/database_working.xlsx
+++ b/database_working.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clorange\Dropbox\CLD\Orange House\Happy Hour\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Dropbox\CLD\Orange House\Happy Hour\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DD5802-5A7C-4F84-82AE-012287BB011D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14390" windowHeight="3500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$C$189</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2297,7 +2298,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2877,12 +2878,12 @@
     <cellStyle name="40% - Accent4" xfId="28" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent5" xfId="31" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent6" xfId="34" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="37"/>
-    <cellStyle name="60% - Accent2" xfId="38"/>
-    <cellStyle name="60% - Accent3" xfId="39"/>
-    <cellStyle name="60% - Accent4" xfId="40"/>
-    <cellStyle name="60% - Accent5" xfId="41"/>
-    <cellStyle name="60% - Accent6" xfId="42"/>
+    <cellStyle name="60% - Accent1" xfId="37" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60% - Accent2" xfId="38" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - Accent3" xfId="39" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent4" xfId="40" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent5" xfId="41" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent6" xfId="42" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Accent1" xfId="17" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="23" builtinId="37" customBuiltin="1"/>
@@ -2901,11 +2902,11 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Input" xfId="8" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="11" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36"/>
+    <cellStyle name="Neutral" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="14" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="9" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="35"/>
+    <cellStyle name="Title" xfId="35" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="13" builtinId="11" customBuiltin="1"/>
   </cellStyles>
@@ -2934,7 +2935,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -3246,36 +3247,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BL188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BF2" sqref="BF2:BF187"/>
+      <selection pane="bottomLeft" activeCell="U54" sqref="U54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="19.85546875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.1796875" style="1"/>
+    <col min="3" max="3" width="19.81640625" style="1" customWidth="1"/>
     <col min="4" max="36" width="6" style="1" customWidth="1"/>
-    <col min="37" max="37" width="10.85546875" style="1" customWidth="1"/>
-    <col min="38" max="38" width="13.5703125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="10.81640625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="13.54296875" style="1" customWidth="1"/>
     <col min="39" max="39" width="13" style="1" customWidth="1"/>
-    <col min="40" max="42" width="10.28515625" style="1" customWidth="1"/>
-    <col min="43" max="43" width="15.85546875" style="1" customWidth="1"/>
-    <col min="44" max="49" width="9.140625" style="1"/>
-    <col min="50" max="50" width="90.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.140625" style="1"/>
-    <col min="53" max="53" width="10.140625" style="1" customWidth="1"/>
-    <col min="54" max="56" width="9.140625" style="1"/>
-    <col min="57" max="57" width="53.5703125" style="1" customWidth="1"/>
-    <col min="58" max="58" width="19.42578125" style="1" customWidth="1"/>
-    <col min="59" max="16384" width="9.140625" style="1"/>
+    <col min="40" max="42" width="10.26953125" style="1" customWidth="1"/>
+    <col min="43" max="43" width="15.81640625" style="1" customWidth="1"/>
+    <col min="44" max="49" width="9.1796875" style="1"/>
+    <col min="50" max="50" width="90.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.1796875" style="1"/>
+    <col min="53" max="53" width="10.1796875" style="1" customWidth="1"/>
+    <col min="54" max="56" width="9.1796875" style="1"/>
+    <col min="57" max="57" width="53.54296875" style="1" customWidth="1"/>
+    <col min="58" max="58" width="19.453125" style="1" customWidth="1"/>
+    <col min="59" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3443,7 +3444,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="2" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>462</v>
       </c>
@@ -3658,7 +3659,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="3" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>140</v>
       </c>
@@ -3870,7 +3871,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>690</v>
       </c>
@@ -4029,7 +4030,7 @@
         <v>[40.58526,-105.07653],</v>
       </c>
     </row>
-    <row r="5" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>146</v>
       </c>
@@ -4195,7 +4196,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>520</v>
       </c>
@@ -4359,7 +4360,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>149</v>
       </c>
@@ -4531,7 +4532,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>65</v>
       </c>
@@ -4745,7 +4746,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>524</v>
       </c>
@@ -4959,7 +4960,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>109</v>
       </c>
@@ -5173,7 +5174,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>583</v>
       </c>
@@ -5335,7 +5336,7 @@
         <v>[40.57561,-105.07659],</v>
       </c>
     </row>
-    <row r="12" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>527</v>
       </c>
@@ -5499,7 +5500,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>529</v>
       </c>
@@ -5660,7 +5661,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>742</v>
       </c>
@@ -5871,7 +5872,7 @@
         <v>[40.543718,-105.074853],</v>
       </c>
     </row>
-    <row r="15" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>134</v>
       </c>
@@ -6038,7 +6039,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
@@ -6240,7 +6241,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>594</v>
       </c>
@@ -6402,7 +6403,7 @@
         <v>[40.56626,-105.07835],</v>
       </c>
     </row>
-    <row r="18" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
@@ -6622,7 +6623,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="19" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>249</v>
       </c>
@@ -6833,7 +6834,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>52</v>
       </c>
@@ -6999,7 +7000,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>307</v>
       </c>
@@ -7198,7 +7199,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>151</v>
       </c>
@@ -7418,7 +7419,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="23" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>269</v>
       </c>
@@ -7629,7 +7630,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="24" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>180</v>
       </c>
@@ -7831,7 +7832,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
         <v>678</v>
       </c>
@@ -8011,7 +8012,7 @@
         <v>[40.58814,-105.07477],</v>
       </c>
     </row>
-    <row r="26" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
         <v>270</v>
       </c>
@@ -8195,7 +8196,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
         <v>532</v>
       </c>
@@ -8358,7 +8359,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
         <v>182</v>
       </c>
@@ -8530,7 +8531,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="29" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
         <v>667</v>
       </c>
@@ -8686,7 +8687,7 @@
         <v>[40.562466,-105.037963],</v>
       </c>
     </row>
-    <row r="30" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>535</v>
       </c>
@@ -8847,7 +8848,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>537</v>
       </c>
@@ -9008,7 +9009,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
         <v>597</v>
       </c>
@@ -9164,7 +9165,7 @@
         <v>[40.57515,-105.09912],</v>
       </c>
     </row>
-    <row r="33" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>600</v>
       </c>
@@ -9330,7 +9331,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="34" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
         <v>374</v>
       </c>
@@ -9532,7 +9533,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="1" t="s">
         <v>603</v>
       </c>
@@ -9688,7 +9689,7 @@
         <v>[40.57951,-105.07766],</v>
       </c>
     </row>
-    <row r="36" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
         <v>395</v>
       </c>
@@ -9902,7 +9903,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
         <v>278</v>
       </c>
@@ -10119,7 +10120,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="38" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
         <v>277</v>
       </c>
@@ -10321,7 +10322,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
         <v>606</v>
       </c>
@@ -10477,7 +10478,7 @@
         <v>[40.58152,-105.04595],</v>
       </c>
     </row>
-    <row r="40" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="1" t="s">
         <v>126</v>
       </c>
@@ -10646,7 +10647,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
         <v>30</v>
       </c>
@@ -10824,7 +10825,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="1" t="s">
         <v>153</v>
       </c>
@@ -10990,7 +10991,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
         <v>26</v>
       </c>
@@ -11195,7 +11196,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
         <v>156</v>
       </c>
@@ -11385,7 +11386,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>77</v>
       </c>
@@ -11599,7 +11600,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B46" s="1" t="s">
         <v>452</v>
       </c>
@@ -11801,7 +11802,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="47" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="1" t="s">
         <v>453</v>
       </c>
@@ -11967,7 +11968,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="48" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="1" t="s">
         <v>555</v>
       </c>
@@ -12166,7 +12167,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" s="1" t="s">
         <v>680</v>
       </c>
@@ -12325,7 +12326,7 @@
         <v>[40.58875,-105.07418],</v>
       </c>
     </row>
-    <row r="50" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="1" t="s">
         <v>677</v>
       </c>
@@ -12487,7 +12488,7 @@
         <v>[40.58587,-105.07762],</v>
       </c>
     </row>
-    <row r="51" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
         <v>675</v>
       </c>
@@ -12679,7 +12680,7 @@
         <v>[40.5666,-105.05774],</v>
       </c>
     </row>
-    <row r="52" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
         <v>86</v>
       </c>
@@ -12845,7 +12846,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
         <v>68</v>
       </c>
@@ -13011,7 +13012,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
         <v>668</v>
       </c>
@@ -13024,18 +13025,6 @@
       <c r="G54" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="H54" s="1">
-        <v>1600</v>
-      </c>
-      <c r="I54" s="1">
-        <v>1800</v>
-      </c>
-      <c r="J54" s="1">
-        <v>1600</v>
-      </c>
-      <c r="K54" s="1">
-        <v>1800</v>
-      </c>
       <c r="L54" s="1">
         <v>1600</v>
       </c>
@@ -13069,21 +13058,21 @@
       <c r="V54" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="W54" s="1">
+      <c r="W54" s="1" t="str">
         <f t="shared" si="21"/>
-        <v>16</v>
-      </c>
-      <c r="X54" s="1">
+        <v/>
+      </c>
+      <c r="X54" s="1" t="str">
         <f t="shared" si="22"/>
-        <v>18</v>
-      </c>
-      <c r="Y54" s="1">
+        <v/>
+      </c>
+      <c r="Y54" s="1" t="str">
         <f t="shared" si="23"/>
-        <v>16</v>
-      </c>
-      <c r="Z54" s="1">
+        <v/>
+      </c>
+      <c r="Z54" s="1" t="str">
         <f t="shared" si="24"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AA54" s="1">
         <f t="shared" si="25"/>
@@ -13127,11 +13116,11 @@
       </c>
       <c r="AK54" s="1" t="str">
         <f t="shared" si="35"/>
-        <v>4pm-6pm</v>
+        <v/>
       </c>
       <c r="AL54" s="1" t="str">
         <f t="shared" si="36"/>
-        <v>4pm-6pm</v>
+        <v/>
       </c>
       <c r="AM54" s="1" t="str">
         <f t="shared" si="37"/>
@@ -13170,7 +13159,7 @@
         <v>{
     'name': "Elevated Sandwiches",
     'area': "nfoco",'hours': {
-      'sunday-start':"1600", 'sunday-end':"1800", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1600", 'saturday-end':"1800"},  'description': "$2.00 off Draft Beers&lt;br&gt; $5.00 House Wines&lt;br&gt;$1.00 off wines by the glass&lt;br&gt;$3-8 food specials including flatbread pizza", 'link':"http://www.elevatedsandwiches.com/menu/", 'pricing':"med",   'phone-number': "", 'address': "1612 N College Ave Fort Collins CO", 'other-amenities': ['','','easy'], 'has-drink':true, 'has-food':true},</v>
+      'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"1600", 'saturday-end':"1800"},  'description': "$2.00 off Draft Beers&lt;br&gt; $5.00 House Wines&lt;br&gt;$1.00 off wines by the glass&lt;br&gt;$3-8 food specials including flatbread pizza", 'link':"http://www.elevatedsandwiches.com/menu/", 'pricing':"med",   'phone-number': "", 'address': "1612 N College Ave Fort Collins CO", 'other-amenities': ['','','easy'], 'has-drink':true, 'has-food':true},</v>
       </c>
       <c r="AY54" s="1" t="str">
         <f t="shared" si="43"/>
@@ -13215,7 +13204,7 @@
         <v>[40.60892,-105.0743],</v>
       </c>
     </row>
-    <row r="55" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B55" s="1" t="s">
         <v>159</v>
       </c>
@@ -13384,7 +13373,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B56" s="1" t="s">
         <v>272</v>
       </c>
@@ -13583,7 +13572,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B57" s="7" t="s">
         <v>375</v>
       </c>
@@ -13794,7 +13783,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B58" s="1" t="s">
         <v>689</v>
       </c>
@@ -13953,7 +13942,7 @@
         <v>[40.58602,-105.07859],</v>
       </c>
     </row>
-    <row r="59" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B59" s="1" t="s">
         <v>454</v>
       </c>
@@ -14119,7 +14108,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="60" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B60" s="1" t="s">
         <v>260</v>
       </c>
@@ -14285,7 +14274,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B61" s="1" t="s">
         <v>98</v>
       </c>
@@ -14496,7 +14485,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" s="1" t="s">
         <v>73</v>
       </c>
@@ -14662,7 +14651,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B63" s="1" t="s">
         <v>273</v>
       </c>
@@ -14876,7 +14865,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B64" s="1" t="s">
         <v>281</v>
       </c>
@@ -15075,7 +15064,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B65" s="1" t="s">
         <v>542</v>
       </c>
@@ -15233,7 +15222,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B66" s="1" t="s">
         <v>189</v>
       </c>
@@ -15439,7 +15428,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B67" s="1" t="s">
         <v>191</v>
       </c>
@@ -15648,7 +15637,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B68" s="1" t="s">
         <v>455</v>
       </c>
@@ -15814,7 +15803,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="69" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="1" t="s">
         <v>193</v>
       </c>
@@ -15983,7 +15972,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="1" t="s">
         <v>609</v>
       </c>
@@ -16190,7 +16179,7 @@
         <v>[40.59003,-105.07363],</v>
       </c>
     </row>
-    <row r="71" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="1" t="s">
         <v>545</v>
       </c>
@@ -16351,7 +16340,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B72" s="1" t="s">
         <v>283</v>
       </c>
@@ -16556,7 +16545,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B73" s="1" t="s">
         <v>687</v>
       </c>
@@ -16715,7 +16704,7 @@
         <v>[40.58839,-105.0776],</v>
       </c>
     </row>
-    <row r="74" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B74" s="1" t="s">
         <v>387</v>
       </c>
@@ -16926,7 +16915,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="75" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B75" s="1" t="s">
         <v>195</v>
       </c>
@@ -17098,7 +17087,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="1" t="s">
         <v>46</v>
       </c>
@@ -17264,7 +17253,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B77" s="1" t="s">
         <v>162</v>
       </c>
@@ -17478,7 +17467,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="1" t="s">
         <v>456</v>
       </c>
@@ -17644,7 +17633,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="79" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="1" t="s">
         <v>197</v>
       </c>
@@ -17810,7 +17799,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B80" s="1" t="s">
         <v>24</v>
       </c>
@@ -18027,7 +18016,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="81" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B81" s="1" t="s">
         <v>688</v>
       </c>
@@ -18183,7 +18172,7 @@
         <v>[40.5315,-105.11594],</v>
       </c>
     </row>
-    <row r="82" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B82" s="1" t="s">
         <v>612</v>
       </c>
@@ -18387,7 +18376,7 @@
         <v>[40.57428,-105.09835],</v>
       </c>
     </row>
-    <row r="83" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B83" s="1" t="s">
         <v>92</v>
       </c>
@@ -18601,7 +18590,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B84" s="1" t="s">
         <v>33</v>
       </c>
@@ -18815,7 +18804,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="1" t="s">
         <v>115</v>
       </c>
@@ -18987,7 +18976,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B86" s="1" t="s">
         <v>739</v>
       </c>
@@ -19069,7 +19058,7 @@
         <v>[40.562046,-105.038001],</v>
       </c>
     </row>
-    <row r="87" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B87" s="1" t="s">
         <v>131</v>
       </c>
@@ -19235,7 +19224,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B88" s="1" t="s">
         <v>95</v>
       </c>
@@ -19401,7 +19390,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B89" s="1" t="s">
         <v>561</v>
       </c>
@@ -19615,7 +19604,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B90" s="1" t="s">
         <v>164</v>
       </c>
@@ -19811,7 +19800,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B91" s="1" t="s">
         <v>616</v>
       </c>
@@ -20012,7 +20001,7 @@
         <v>[40.52366,-105.03402],</v>
       </c>
     </row>
-    <row r="92" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B92" s="1" t="s">
         <v>384</v>
       </c>
@@ -20217,7 +20206,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B93" s="1" t="s">
         <v>199</v>
       </c>
@@ -20431,7 +20420,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B94" s="1" t="s">
         <v>620</v>
       </c>
@@ -20587,7 +20576,7 @@
         <v>[40.5831,-105.08285],</v>
       </c>
     </row>
-    <row r="95" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B95" s="1" t="s">
         <v>285</v>
       </c>
@@ -20798,7 +20787,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B96" s="1" t="s">
         <v>623</v>
       </c>
@@ -20954,7 +20943,7 @@
         <v>[40.58653,-105.07751],</v>
       </c>
     </row>
-    <row r="97" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B97" s="1" t="s">
         <v>626</v>
       </c>
@@ -21107,7 +21096,7 @@
         <v>[40.58231,-105.10714],</v>
       </c>
     </row>
-    <row r="98" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B98" s="1" t="s">
         <v>379</v>
       </c>
@@ -21276,7 +21265,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B99" s="1" t="s">
         <v>288</v>
       </c>
@@ -21487,7 +21476,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B100" s="1" t="s">
         <v>684</v>
       </c>
@@ -21646,7 +21635,7 @@
         <v>[40.57914,-105.07946],</v>
       </c>
     </row>
-    <row r="101" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B101" s="1" t="s">
         <v>166</v>
       </c>
@@ -21818,7 +21807,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B102" s="1" t="s">
         <v>628</v>
       </c>
@@ -21974,7 +21963,7 @@
         <v>[40.55511,-105.07836],</v>
       </c>
     </row>
-    <row r="103" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B103" s="1" t="s">
         <v>574</v>
       </c>
@@ -22181,7 +22170,7 @@
         <v>[40.57291,-105.1154],</v>
       </c>
     </row>
-    <row r="104" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B104" s="1" t="s">
         <v>62</v>
       </c>
@@ -22347,7 +22336,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B105" s="1" t="s">
         <v>200</v>
       </c>
@@ -22513,7 +22502,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B106" s="1" t="s">
         <v>402</v>
       </c>
@@ -22688,7 +22677,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="107" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B107" s="1" t="s">
         <v>676</v>
       </c>
@@ -22896,7 +22885,7 @@
         <v>[40.57532,-105.10038],</v>
       </c>
     </row>
-    <row r="108" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B108" s="1" t="s">
         <v>121</v>
       </c>
@@ -23110,7 +23099,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B109" s="1" t="s">
         <v>168</v>
       </c>
@@ -23321,7 +23310,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B110" s="1" t="s">
         <v>202</v>
       </c>
@@ -23493,7 +23482,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="1" t="s">
         <v>170</v>
       </c>
@@ -23701,7 +23690,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="112" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B112" s="1" t="s">
         <v>674</v>
       </c>
@@ -23860,7 +23849,7 @@
         <v>[40.58358,-105.04801],</v>
       </c>
     </row>
-    <row r="113" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B113" s="1" t="s">
         <v>123</v>
       </c>
@@ -24026,7 +24015,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B114" s="1" t="s">
         <v>123</v>
       </c>
@@ -24182,7 +24171,7 @@
         <v>[40.5491,-105.07603],</v>
       </c>
     </row>
-    <row r="115" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B115" s="1" t="s">
         <v>672</v>
       </c>
@@ -24341,7 +24330,7 @@
         <v>[40.55065,-105.04275],</v>
       </c>
     </row>
-    <row r="116" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B116" s="1" t="s">
         <v>204</v>
       </c>
@@ -24513,7 +24502,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B117" s="1" t="s">
         <v>143</v>
       </c>
@@ -24679,7 +24668,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B118" s="1" t="s">
         <v>457</v>
       </c>
@@ -24845,7 +24834,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="119" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B119" s="1" t="s">
         <v>633</v>
       </c>
@@ -25049,7 +25038,7 @@
         <v>[40.52143,-105.05755],</v>
       </c>
     </row>
-    <row r="120" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B120" s="1" t="s">
         <v>637</v>
       </c>
@@ -25250,7 +25239,7 @@
         <v>[40.56741,-105.08268],</v>
       </c>
     </row>
-    <row r="121" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B121" s="1" t="s">
         <v>89</v>
       </c>
@@ -25464,7 +25453,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B122" s="1" t="s">
         <v>589</v>
       </c>
@@ -25659,7 +25648,7 @@
         <v>[40.58998,-105.0731],</v>
       </c>
     </row>
-    <row r="123" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B123" s="1" t="s">
         <v>206</v>
       </c>
@@ -25870,7 +25859,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B124" s="1" t="s">
         <v>208</v>
       </c>
@@ -26039,7 +26028,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B125" s="1" t="s">
         <v>458</v>
       </c>
@@ -26205,7 +26194,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="126" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B126" s="1" t="s">
         <v>673</v>
       </c>
@@ -26364,7 +26353,7 @@
         <v>[40.57789,-105.0766],</v>
       </c>
     </row>
-    <row r="127" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B127" s="1" t="s">
         <v>669</v>
       </c>
@@ -26526,7 +26515,7 @@
         <v>[40.57855,-105.07975],</v>
       </c>
     </row>
-    <row r="128" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B128" s="1" t="s">
         <v>210</v>
       </c>
@@ -26698,7 +26687,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B129" s="1" t="s">
         <v>681</v>
       </c>
@@ -26857,7 +26846,7 @@
         <v>[40.573785,-105.0833606],</v>
       </c>
     </row>
-    <row r="130" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B130" s="1" t="s">
         <v>172</v>
       </c>
@@ -27066,7 +27055,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B131" s="1" t="s">
         <v>43</v>
       </c>
@@ -27265,7 +27254,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B132" s="1" t="s">
         <v>212</v>
       </c>
@@ -27479,7 +27468,7 @@
         <v/>
       </c>
     </row>
-    <row r="133" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B133" s="1" t="s">
         <v>59</v>
       </c>
@@ -27645,7 +27634,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B134" s="1" t="s">
         <v>59</v>
       </c>
@@ -27806,7 +27795,7 @@
       </c>
       <c r="BL134" s="12"/>
     </row>
-    <row r="135" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B135" s="1" t="s">
         <v>459</v>
       </c>
@@ -27972,7 +27961,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="136" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B136" s="1" t="s">
         <v>682</v>
       </c>
@@ -28128,7 +28117,7 @@
         <v>[40.55258,-105.09673],</v>
       </c>
     </row>
-    <row r="137" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B137" s="1" t="s">
         <v>215</v>
       </c>
@@ -28294,7 +28283,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B138" s="1" t="s">
         <v>486</v>
       </c>
@@ -28460,7 +28449,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="139" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B139" s="1" t="s">
         <v>670</v>
       </c>
@@ -28664,7 +28653,7 @@
         <v>[40.55475,-105.09774],</v>
       </c>
     </row>
-    <row r="140" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B140" s="1" t="s">
         <v>405</v>
       </c>
@@ -28830,7 +28819,7 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B141" s="1" t="s">
         <v>386</v>
       </c>
@@ -29038,7 +29027,7 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B142" s="1" t="s">
         <v>671</v>
       </c>
@@ -29227,7 +29216,7 @@
         <v>[40.5635177,-105.077318],</v>
       </c>
     </row>
-    <row r="143" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B143" s="1" t="s">
         <v>218</v>
       </c>
@@ -29438,7 +29427,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B144" s="1" t="s">
         <v>290</v>
       </c>
@@ -29649,7 +29638,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B145" s="1" t="s">
         <v>103</v>
       </c>
@@ -29854,7 +29843,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B146" s="1" t="s">
         <v>137</v>
       </c>
@@ -30026,7 +30015,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="147" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B147" s="1" t="s">
         <v>118</v>
       </c>
@@ -30192,7 +30181,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B148" s="1" t="s">
         <v>642</v>
       </c>
@@ -30348,7 +30337,7 @@
         <v>[40.58742,-105.0784],</v>
       </c>
     </row>
-    <row r="149" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B149" s="1" t="s">
         <v>40</v>
       </c>
@@ -30523,7 +30512,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="150" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B150" s="1" t="s">
         <v>37</v>
       </c>
@@ -30734,7 +30723,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B151" s="1" t="s">
         <v>683</v>
       </c>
@@ -30887,7 +30876,7 @@
         <v>[40.58213,-105.02703],</v>
       </c>
     </row>
-    <row r="152" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B152" s="1" t="s">
         <v>383</v>
       </c>
@@ -31053,7 +31042,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B153" s="1" t="s">
         <v>550</v>
       </c>
@@ -31258,7 +31247,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B154" s="1" t="s">
         <v>685</v>
       </c>
@@ -31417,7 +31406,7 @@
         <v>[40.62701,-105.13785],</v>
       </c>
     </row>
-    <row r="155" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B155" s="1" t="s">
         <v>112</v>
       </c>
@@ -31613,7 +31602,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B156" s="1" t="s">
         <v>557</v>
       </c>
@@ -31815,7 +31804,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B157" s="1" t="s">
         <v>80</v>
       </c>
@@ -31984,7 +31973,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B158" s="1" t="s">
         <v>686</v>
       </c>
@@ -32140,7 +32129,7 @@
         <v>[40.66018,-105.161719],</v>
       </c>
     </row>
-    <row r="159" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B159" s="1" t="s">
         <v>460</v>
       </c>
@@ -32306,7 +32295,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="160" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B160" s="1" t="s">
         <v>100</v>
       </c>
@@ -32472,7 +32461,7 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B161" s="1" t="s">
         <v>645</v>
       </c>
@@ -32625,7 +32614,7 @@
         <v>[40.57906,-105.07656],</v>
       </c>
     </row>
-    <row r="162" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B162" s="1" t="s">
         <v>83</v>
       </c>
@@ -32794,7 +32783,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B163" s="1" t="s">
         <v>220</v>
       </c>
@@ -32993,7 +32982,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B164" s="1" t="s">
         <v>647</v>
       </c>
@@ -33173,7 +33162,7 @@
         <v>[40.56208,-105.03864],</v>
       </c>
     </row>
-    <row r="165" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B165" s="1" t="s">
         <v>175</v>
       </c>
@@ -33372,7 +33361,7 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B166" s="1" t="s">
         <v>586</v>
       </c>
@@ -33537,7 +33526,7 @@
         <v>[40.57891,-105.07843],</v>
       </c>
     </row>
-    <row r="167" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B167" s="1" t="s">
         <v>719</v>
       </c>
@@ -33738,7 +33727,7 @@
         <v>[40.58815,-105.07761],</v>
       </c>
     </row>
-    <row r="168" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B168" s="1" t="s">
         <v>650</v>
       </c>
@@ -33894,7 +33883,7 @@
         <v>[40.58899,-105.07637],</v>
       </c>
     </row>
-    <row r="169" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B169" s="1" t="s">
         <v>579</v>
       </c>
@@ -34056,7 +34045,7 @@
         <v>[40.58487,-105.0765],</v>
       </c>
     </row>
-    <row r="170" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B170" s="1" t="s">
         <v>653</v>
       </c>
@@ -34215,7 +34204,7 @@
         <v>[40.58758,-105.07636],</v>
       </c>
     </row>
-    <row r="171" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B171" s="1" t="s">
         <v>461</v>
       </c>
@@ -34381,7 +34370,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="172" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B172" s="1" t="s">
         <v>222</v>
       </c>
@@ -34595,7 +34584,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B173" s="1" t="s">
         <v>388</v>
       </c>
@@ -34797,7 +34786,7 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B174" s="1" t="s">
         <v>225</v>
       </c>
@@ -34963,7 +34952,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B175" s="1" t="s">
         <v>568</v>
       </c>
@@ -35159,7 +35148,7 @@
         <v>[40.58741,-105.07661],</v>
       </c>
     </row>
-    <row r="176" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B176" s="1" t="s">
         <v>655</v>
       </c>
@@ -35312,7 +35301,7 @@
         <v>[40.57844,-105.07856],</v>
       </c>
     </row>
-    <row r="177" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B177" s="1" t="s">
         <v>292</v>
       </c>
@@ -35523,7 +35512,7 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B178" s="1" t="s">
         <v>409</v>
       </c>
@@ -35692,7 +35681,7 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B179" s="1" t="s">
         <v>657</v>
       </c>
@@ -35848,7 +35837,7 @@
         <v>[40.57429,-105.0971],</v>
       </c>
     </row>
-    <row r="180" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B180" s="1" t="s">
         <v>679</v>
       </c>
@@ -36001,7 +35990,7 @@
         <v>[40.55258,-105.09673],</v>
       </c>
     </row>
-    <row r="181" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B181" s="1" t="s">
         <v>128</v>
       </c>
@@ -36173,7 +36162,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B182" s="1" t="s">
         <v>565</v>
       </c>
@@ -36338,7 +36327,7 @@
         <v>[40.55197,-105.03718],</v>
       </c>
     </row>
-    <row r="183" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B183" s="1" t="s">
         <v>660</v>
       </c>
@@ -36515,7 +36504,7 @@
         <v>[40.57358,-105.05826],</v>
       </c>
     </row>
-    <row r="184" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B184" s="1" t="s">
         <v>227</v>
       </c>
@@ -36681,7 +36670,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B185" s="17" t="s">
         <v>49</v>
       </c>
@@ -36847,7 +36836,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B186" s="1" t="s">
         <v>664</v>
       </c>
@@ -37006,7 +36995,7 @@
         <v>[40.57488,-105.10039],</v>
       </c>
     </row>
-    <row r="187" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B187" s="1" t="s">
         <v>229</v>
       </c>
@@ -37178,84 +37167,84 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AV188" s="5"/>
       <c r="AW188" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="C2:C189"/>
+  <autoFilter ref="C2:C189" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState ref="B2:BL188">
     <sortCondition ref="B3"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G130" r:id="rId1" display="https://www.google.com/maps/dir/Current+Location/101 S. College Avenue, Fort Collins, CO 80524"/>
-    <hyperlink ref="AR41" r:id="rId2"/>
-    <hyperlink ref="AR93" r:id="rId3"/>
-    <hyperlink ref="AR28" r:id="rId4"/>
-    <hyperlink ref="AR110" r:id="rId5"/>
-    <hyperlink ref="AR20" r:id="rId6"/>
-    <hyperlink ref="AR8" r:id="rId7"/>
-    <hyperlink ref="AR53" r:id="rId8"/>
-    <hyperlink ref="AR34" r:id="rId9"/>
-    <hyperlink ref="AR62" r:id="rId10"/>
-    <hyperlink ref="AR45" r:id="rId11"/>
-    <hyperlink ref="AR157" r:id="rId12"/>
-    <hyperlink ref="AR52" r:id="rId13"/>
-    <hyperlink ref="AR121" r:id="rId14"/>
-    <hyperlink ref="AR88" r:id="rId15"/>
-    <hyperlink ref="AR61" r:id="rId16"/>
-    <hyperlink ref="AR160" r:id="rId17"/>
-    <hyperlink ref="AR145" r:id="rId18"/>
-    <hyperlink ref="AR19" r:id="rId19"/>
-    <hyperlink ref="AR10" r:id="rId20"/>
-    <hyperlink ref="AR155" r:id="rId21"/>
-    <hyperlink ref="AR85" r:id="rId22"/>
-    <hyperlink ref="AR147" r:id="rId23"/>
-    <hyperlink ref="AR108" r:id="rId24"/>
-    <hyperlink ref="AR181" r:id="rId25"/>
-    <hyperlink ref="AR87" r:id="rId26"/>
-    <hyperlink ref="AR15" r:id="rId27"/>
-    <hyperlink ref="AR80" r:id="rId28"/>
-    <hyperlink ref="AR5" r:id="rId29"/>
-    <hyperlink ref="AR7" r:id="rId30"/>
-    <hyperlink ref="AR42" r:id="rId31"/>
-    <hyperlink ref="AR44" r:id="rId32"/>
-    <hyperlink ref="AR55" r:id="rId33"/>
-    <hyperlink ref="AR77" r:id="rId34"/>
-    <hyperlink ref="AR90" r:id="rId35"/>
-    <hyperlink ref="AR101" r:id="rId36"/>
-    <hyperlink ref="AR109" r:id="rId37"/>
-    <hyperlink ref="AR111" r:id="rId38"/>
-    <hyperlink ref="AR130" r:id="rId39"/>
-    <hyperlink ref="AR16" r:id="rId40"/>
-    <hyperlink ref="AR24" r:id="rId41"/>
-    <hyperlink ref="AR60" r:id="rId42"/>
-    <hyperlink ref="AR75" r:id="rId43"/>
-    <hyperlink ref="AR79" r:id="rId44"/>
-    <hyperlink ref="AR105" r:id="rId45"/>
-    <hyperlink ref="AR123" r:id="rId46"/>
-    <hyperlink ref="AR132" r:id="rId47"/>
-    <hyperlink ref="AR137" r:id="rId48"/>
-    <hyperlink ref="AR143" r:id="rId49"/>
-    <hyperlink ref="AR163" r:id="rId50"/>
-    <hyperlink ref="AR174" r:id="rId51"/>
-    <hyperlink ref="AR187" r:id="rId52"/>
-    <hyperlink ref="AR23" r:id="rId53"/>
-    <hyperlink ref="AR56" r:id="rId54"/>
-    <hyperlink ref="AR63" r:id="rId55"/>
-    <hyperlink ref="AR64" r:id="rId56"/>
-    <hyperlink ref="AR72" r:id="rId57"/>
-    <hyperlink ref="AR95" r:id="rId58"/>
-    <hyperlink ref="AR99" r:id="rId59"/>
-    <hyperlink ref="AR144" r:id="rId60"/>
-    <hyperlink ref="AR177" r:id="rId61"/>
-    <hyperlink ref="AR57" r:id="rId62"/>
-    <hyperlink ref="AR74" r:id="rId63"/>
-    <hyperlink ref="AR46" r:id="rId64"/>
-    <hyperlink ref="AR9" r:id="rId65"/>
-    <hyperlink ref="AR167" r:id="rId66"/>
-    <hyperlink ref="B11" r:id="rId67" display="https://www.yelp.com/biz/avuncular-bobs-beerhouse-fort-collins"/>
-    <hyperlink ref="AR166" r:id="rId68"/>
+    <hyperlink ref="G130" r:id="rId1" display="https://www.google.com/maps/dir/Current+Location/101 S. College Avenue, Fort Collins, CO 80524" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="AR41" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="AR93" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="AR28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="AR110" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="AR20" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="AR8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="AR53" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="AR34" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="AR62" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="AR45" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="AR157" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="AR52" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="AR121" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="AR88" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="AR61" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="AR160" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="AR145" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="AR19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="AR10" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="AR155" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="AR85" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="AR147" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="AR108" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="AR181" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="AR87" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="AR15" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="AR80" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="AR5" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="AR7" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="AR42" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="AR44" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="AR55" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="AR77" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="AR90" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="AR101" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="AR109" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="AR111" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="AR130" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="AR16" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="AR24" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="AR60" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="AR75" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="AR79" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="AR105" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="AR123" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="AR132" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="AR137" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="AR143" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="AR163" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="AR174" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="AR187" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="AR23" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="AR56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="AR63" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="AR64" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="AR72" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="AR95" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="AR99" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="AR144" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="AR177" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="AR57" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="AR74" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="AR46" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="AR9" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="AR167" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B11" r:id="rId67" display="https://www.yelp.com/biz/avuncular-bobs-beerhouse-fort-collins" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="AR166" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId69"/>
@@ -37263,19 +37252,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B1" s="11">
         <v>40.588749999999997</v>
       </c>
@@ -37289,7 +37278,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" s="11">
         <v>40.58587</v>
       </c>
@@ -37303,7 +37292,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="11">
         <v>40.566600000000001</v>
       </c>
@@ -37315,35 +37304,35 @@
       </c>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -37357,14 +37346,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <customProperties>

</xml_diff>

<commit_message>
Fixed minor mistake in one venue
</commit_message>
<xml_diff>
--- a/database_working.xlsx
+++ b/database_working.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Dropbox\CLD\Orange House\Happy Hour\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clorange\Dropbox\CLD\Orange House\Happy Hour\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B93326-36EF-483D-BED7-473A2809C5DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$C$191</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="799">
   <si>
     <t>Name</t>
   </si>
@@ -2420,9 +2419,6 @@
   </si>
   <si>
     <t>234 N College Ave #3a, Fort Collins, CO 80524</t>
-  </si>
-  <si>
-    <t>!600</t>
   </si>
   <si>
     <t>$5 Glasses of Wine</t>
@@ -2440,7 +2436,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3023,12 +3019,12 @@
     <cellStyle name="40% - Accent4" xfId="28" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent5" xfId="31" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent6" xfId="34" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="37" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2" xfId="38" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3" xfId="39" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4" xfId="40" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5" xfId="41" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6" xfId="42" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="60% - Accent1" xfId="37"/>
+    <cellStyle name="60% - Accent2" xfId="38"/>
+    <cellStyle name="60% - Accent3" xfId="39"/>
+    <cellStyle name="60% - Accent4" xfId="40"/>
+    <cellStyle name="60% - Accent5" xfId="41"/>
+    <cellStyle name="60% - Accent6" xfId="42"/>
     <cellStyle name="Accent1" xfId="17" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="23" builtinId="37" customBuiltin="1"/>
@@ -3047,11 +3043,11 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Input" xfId="8" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="11" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Neutral" xfId="36"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="14" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="9" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="35" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Title" xfId="35"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="13" builtinId="11" customBuiltin="1"/>
   </cellStyles>
@@ -3080,7 +3076,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -3392,33 +3388,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BL196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="BB38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AE74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="U86" sqref="U86"/>
-      <selection pane="bottomRight" activeCell="BG48" sqref="BG48"/>
+      <selection pane="bottomRight" activeCell="AU85" sqref="AU85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="36" width="6" customWidth="1"/>
-    <col min="37" max="37" width="10.81640625" customWidth="1"/>
-    <col min="38" max="38" width="13.54296875" customWidth="1"/>
+    <col min="37" max="37" width="10.85546875" customWidth="1"/>
+    <col min="38" max="38" width="13.5703125" customWidth="1"/>
     <col min="39" max="39" width="13" customWidth="1"/>
-    <col min="40" max="42" width="10.26953125" customWidth="1"/>
-    <col min="43" max="43" width="15.81640625" customWidth="1"/>
-    <col min="50" max="50" width="90.54296875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.1796875" customWidth="1"/>
-    <col min="57" max="57" width="53.54296875" customWidth="1"/>
-    <col min="58" max="58" width="19.453125" customWidth="1"/>
+    <col min="40" max="42" width="10.28515625" customWidth="1"/>
+    <col min="43" max="43" width="15.85546875" customWidth="1"/>
+    <col min="50" max="50" width="90.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.140625" customWidth="1"/>
+    <col min="57" max="57" width="53.5703125" customWidth="1"/>
+    <col min="58" max="58" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3586,7 +3582,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="2" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>454</v>
       </c>
@@ -3801,7 +3797,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="3" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>140</v>
       </c>
@@ -4009,7 +4005,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>671</v>
       </c>
@@ -4168,7 +4164,7 @@
         <v>[40.58526,-105.07653],</v>
       </c>
     </row>
-    <row r="5" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>146</v>
       </c>
@@ -4334,7 +4330,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>509</v>
       </c>
@@ -4498,7 +4494,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>149</v>
       </c>
@@ -4670,7 +4666,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>65</v>
       </c>
@@ -4884,7 +4880,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>513</v>
       </c>
@@ -5098,7 +5094,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>109</v>
       </c>
@@ -5312,7 +5308,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>568</v>
       </c>
@@ -5474,7 +5470,7 @@
         <v>[40.57561,-105.07659],</v>
       </c>
     </row>
-    <row r="12" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>516</v>
       </c>
@@ -5638,7 +5634,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>518</v>
       </c>
@@ -5799,7 +5795,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>720</v>
       </c>
@@ -6006,7 +6002,7 @@
         <v>[40.543718,-105.074853],</v>
       </c>
     </row>
-    <row r="15" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>134</v>
       </c>
@@ -6173,7 +6169,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -6375,7 +6371,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>579</v>
       </c>
@@ -6537,7 +6533,7 @@
         <v>[40.56626,-105.07835],</v>
       </c>
     </row>
-    <row r="18" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>56</v>
       </c>
@@ -6757,7 +6753,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="19" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>246</v>
       </c>
@@ -6968,7 +6964,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>52</v>
       </c>
@@ -7134,7 +7130,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>301</v>
       </c>
@@ -7333,7 +7329,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>151</v>
       </c>
@@ -7553,7 +7549,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="23" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>266</v>
       </c>
@@ -7764,7 +7760,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="24" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>178</v>
       </c>
@@ -7966,7 +7962,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>659</v>
       </c>
@@ -8146,7 +8142,7 @@
         <v>[40.58814,-105.07477],</v>
       </c>
     </row>
-    <row r="26" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>267</v>
       </c>
@@ -8330,7 +8326,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>520</v>
       </c>
@@ -8493,7 +8489,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>180</v>
       </c>
@@ -8665,7 +8661,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="29" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>648</v>
       </c>
@@ -8821,7 +8817,7 @@
         <v>[40.562466,-105.037963],</v>
       </c>
     </row>
-    <row r="30" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>523</v>
       </c>
@@ -8982,7 +8978,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>525</v>
       </c>
@@ -9143,7 +9139,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>582</v>
       </c>
@@ -9299,7 +9295,7 @@
         <v>[40.57515,-105.09912],</v>
       </c>
     </row>
-    <row r="33" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>585</v>
       </c>
@@ -9465,7 +9461,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="34" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>366</v>
       </c>
@@ -9671,7 +9667,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>588</v>
       </c>
@@ -9827,7 +9823,7 @@
         <v>[40.57951,-105.07766],</v>
       </c>
     </row>
-    <row r="36" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>387</v>
       </c>
@@ -10041,7 +10037,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>275</v>
       </c>
@@ -10258,7 +10254,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="38" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>274</v>
       </c>
@@ -10460,7 +10456,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>591</v>
       </c>
@@ -10616,7 +10612,7 @@
         <v>[40.58152,-105.04595],</v>
       </c>
     </row>
-    <row r="40" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>126</v>
       </c>
@@ -10785,7 +10781,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>731</v>
       </c>
@@ -10993,7 +10989,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>30</v>
       </c>
@@ -11171,7 +11167,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>153</v>
       </c>
@@ -11337,7 +11333,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>26</v>
       </c>
@@ -11542,7 +11538,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>156</v>
       </c>
@@ -11732,7 +11728,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>77</v>
       </c>
@@ -11946,9 +11942,9 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C47" t="s">
         <v>426</v>
@@ -11957,7 +11953,7 @@
         <v>431</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="W47" t="str">
         <f t="shared" ref="W47" si="59">IF(H47&gt;0,H47/100,"")</f>
@@ -12048,7 +12044,7 @@
         <v>295</v>
       </c>
       <c r="AT47" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="AU47" t="s">
         <v>298</v>
@@ -12113,7 +12109,7 @@
         <v>[40.589825,-105.076497],</v>
       </c>
     </row>
-    <row r="48" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>444</v>
       </c>
@@ -12315,7 +12311,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="49" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>445</v>
       </c>
@@ -12481,7 +12477,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="50" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>540</v>
       </c>
@@ -12680,7 +12676,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>661</v>
       </c>
@@ -12839,7 +12835,7 @@
         <v>[40.58875,-105.07418],</v>
       </c>
     </row>
-    <row r="52" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>658</v>
       </c>
@@ -13001,7 +12997,7 @@
         <v>[40.58587,-105.07762],</v>
       </c>
     </row>
-    <row r="53" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>656</v>
       </c>
@@ -13193,7 +13189,7 @@
         <v>[40.5666,-105.05774],</v>
       </c>
     </row>
-    <row r="54" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>86</v>
       </c>
@@ -13359,7 +13355,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>68</v>
       </c>
@@ -13525,7 +13521,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>649</v>
       </c>
@@ -13717,7 +13713,7 @@
         <v>[40.60892,-105.0743],</v>
       </c>
     </row>
-    <row r="57" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>159</v>
       </c>
@@ -13901,7 +13897,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>269</v>
       </c>
@@ -14100,7 +14096,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B59" s="5" t="s">
         <v>367</v>
       </c>
@@ -14311,7 +14307,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>670</v>
       </c>
@@ -14470,7 +14466,7 @@
         <v>[40.58602,-105.07859],</v>
       </c>
     </row>
-    <row r="61" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>446</v>
       </c>
@@ -14636,7 +14632,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="62" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>257</v>
       </c>
@@ -14802,7 +14798,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>98</v>
       </c>
@@ -15013,7 +15009,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>73</v>
       </c>
@@ -15179,7 +15175,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>749</v>
       </c>
@@ -15333,7 +15329,7 @@
         <v>[40.58976,-105.076497],</v>
       </c>
     </row>
-    <row r="66" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>270</v>
       </c>
@@ -15547,7 +15543,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>278</v>
       </c>
@@ -15750,7 +15746,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>751</v>
       </c>
@@ -15901,7 +15897,7 @@
         <v>[40.551049,-105.05831],</v>
       </c>
     </row>
-    <row r="69" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>530</v>
       </c>
@@ -16059,7 +16055,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>187</v>
       </c>
@@ -16265,7 +16261,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>189</v>
       </c>
@@ -16470,7 +16466,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>447</v>
       </c>
@@ -16636,7 +16632,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="73" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>191</v>
       </c>
@@ -16805,7 +16801,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>594</v>
       </c>
@@ -17012,7 +17008,7 @@
         <v>[40.59003,-105.07363],</v>
       </c>
     </row>
-    <row r="75" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>532</v>
       </c>
@@ -17173,7 +17169,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>736</v>
       </c>
@@ -17377,7 +17373,7 @@
         <v>[40.47964,-104.90192],</v>
       </c>
     </row>
-    <row r="77" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>280</v>
       </c>
@@ -17582,7 +17578,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>668</v>
       </c>
@@ -17741,7 +17737,7 @@
         <v>[40.58839,-105.0776],</v>
       </c>
     </row>
-    <row r="79" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>379</v>
       </c>
@@ -17952,7 +17948,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="80" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>193</v>
       </c>
@@ -18124,7 +18120,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>46</v>
       </c>
@@ -18290,7 +18286,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>162</v>
       </c>
@@ -18504,7 +18500,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>448</v>
       </c>
@@ -18670,7 +18666,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="84" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>793</v>
       </c>
@@ -18683,78 +18679,78 @@
       <c r="G84" s="7" t="s">
         <v>794</v>
       </c>
-      <c r="J84" t="s">
-        <v>795</v>
+      <c r="J84">
+        <v>1600</v>
       </c>
       <c r="K84">
         <v>1800</v>
       </c>
-      <c r="L84" t="s">
-        <v>795</v>
+      <c r="L84">
+        <v>1600</v>
       </c>
       <c r="M84">
         <v>1800</v>
       </c>
-      <c r="N84" t="s">
-        <v>795</v>
+      <c r="N84">
+        <v>1600</v>
       </c>
       <c r="O84">
         <v>1800</v>
       </c>
-      <c r="P84" t="s">
-        <v>795</v>
+      <c r="P84">
+        <v>1600</v>
       </c>
       <c r="Q84">
         <v>1800</v>
       </c>
-      <c r="R84" t="s">
-        <v>795</v>
+      <c r="R84">
+        <v>1600</v>
       </c>
       <c r="S84">
         <v>1800</v>
       </c>
       <c r="V84" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="X84" t="str">
         <f t="shared" ref="X84" si="121">IF(I84&gt;0,I84/100,"")</f>
         <v/>
       </c>
-      <c r="Y84" t="e">
+      <c r="Y84">
         <f t="shared" ref="Y84" si="122">IF(J84&gt;0,J84/100,"")</f>
-        <v>#VALUE!</v>
+        <v>16</v>
       </c>
       <c r="Z84">
         <f t="shared" ref="Z84" si="123">IF(K84&gt;0,K84/100,"")</f>
         <v>18</v>
       </c>
-      <c r="AA84" t="e">
+      <c r="AA84">
         <f t="shared" ref="AA84" si="124">IF(L84&gt;0,L84/100,"")</f>
-        <v>#VALUE!</v>
+        <v>16</v>
       </c>
       <c r="AB84">
         <f t="shared" ref="AB84" si="125">IF(M84&gt;0,M84/100,"")</f>
         <v>18</v>
       </c>
-      <c r="AC84" t="e">
+      <c r="AC84">
         <f t="shared" ref="AC84" si="126">IF(N84&gt;0,N84/100,"")</f>
-        <v>#VALUE!</v>
+        <v>16</v>
       </c>
       <c r="AD84">
         <f t="shared" ref="AD84" si="127">IF(O84&gt;0,O84/100,"")</f>
         <v>18</v>
       </c>
-      <c r="AE84" t="e">
+      <c r="AE84">
         <f t="shared" ref="AE84" si="128">IF(P84&gt;0,P84/100,"")</f>
-        <v>#VALUE!</v>
+        <v>16</v>
       </c>
       <c r="AF84">
         <f t="shared" ref="AF84" si="129">IF(Q84&gt;0,Q84/100,"")</f>
         <v>18</v>
       </c>
-      <c r="AG84" t="e">
+      <c r="AG84">
         <f t="shared" ref="AG84" si="130">IF(R84&gt;0,R84/100,"")</f>
-        <v>#VALUE!</v>
+        <v>16</v>
       </c>
       <c r="AH84">
         <f t="shared" ref="AH84" si="131">IF(S84&gt;0,S84/100,"")</f>
@@ -18772,25 +18768,25 @@
         <f t="shared" ref="AK84" si="134">IF(H84&gt;0,CONCATENATE(IF(W84&lt;=12,W84,W84-12),IF(OR(W84&lt;12,W84=24),"am","pm"),"-",IF(X84&lt;=12,X84,X84-12),IF(OR(X84&lt;12,X84=24),"am","pm")),"")</f>
         <v/>
       </c>
-      <c r="AL84" t="e">
+      <c r="AL84" t="str">
         <f t="shared" ref="AL84" si="135">IF(J84&gt;0,CONCATENATE(IF(Y84&lt;=12,Y84,Y84-12),IF(OR(Y84&lt;12,Y84=24),"am","pm"),"-",IF(Z84&lt;=12,Z84,Z84-12),IF(OR(Z84&lt;12,Z84=24),"am","pm")),"")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AM84" t="e">
+        <v>4pm-6pm</v>
+      </c>
+      <c r="AM84" t="str">
         <f t="shared" ref="AM84" si="136">IF(L84&gt;0,CONCATENATE(IF(AA84&lt;=12,AA84,AA84-12),IF(OR(AA84&lt;12,AA84=24),"am","pm"),"-",IF(AB84&lt;=12,AB84,AB84-12),IF(OR(AB84&lt;12,AB84=24),"am","pm")),"")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AN84" t="e">
+        <v>4pm-6pm</v>
+      </c>
+      <c r="AN84" t="str">
         <f t="shared" ref="AN84" si="137">IF(N84&gt;0,CONCATENATE(IF(AC84&lt;=12,AC84,AC84-12),IF(OR(AC84&lt;12,AC84=24),"am","pm"),"-",IF(AD84&lt;=12,AD84,AD84-12),IF(OR(AD84&lt;12,AD84=24),"am","pm")),"")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AO84" t="e">
+        <v>4pm-6pm</v>
+      </c>
+      <c r="AO84" t="str">
         <f t="shared" ref="AO84" si="138">IF(P84&gt;0,CONCATENATE(IF(AE84&lt;=12,AE84,AE84-12),IF(OR(AE84&lt;12,AE84=24),"am","pm"),"-",IF(AF84&lt;=12,AF84,AF84-12),IF(OR(AF84&lt;12,AF84=24),"am","pm")),"")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AP84" t="e">
+        <v>4pm-6pm</v>
+      </c>
+      <c r="AP84" t="str">
         <f t="shared" ref="AP84" si="139">IF(R84&gt;0,CONCATENATE(IF(AG84&lt;=12,AG84,AG84-12),IF(OR(AG84&lt;12,AG84=24),"am","pm"),"-",IF(AH84&lt;=12,AH84,AH84-12),IF(OR(AH84&lt;12,AH84=24),"am","pm")),"")</f>
-        <v>#VALUE!</v>
+        <v>4pm-6pm</v>
       </c>
       <c r="AQ84" t="str">
         <f t="shared" ref="AQ84" si="140">IF(T84&gt;0,CONCATENATE(IF(AI84&lt;=12,AI84,AI84-12),IF(OR(AI84&lt;12,AI84=24),"am","pm"),"-",IF(AJ84&lt;=12,AJ84,AJ84-12),IF(OR(AJ84&lt;12,AJ84=24),"am","pm")),"")</f>
@@ -18798,6 +18794,9 @@
       </c>
       <c r="AS84" t="s">
         <v>295</v>
+      </c>
+      <c r="AU84" t="s">
+        <v>28</v>
       </c>
       <c r="AV84" s="3" t="s">
         <v>306</v>
@@ -18814,7 +18813,7 @@
         <v>{
     'name': "Infinite Monkey Theorem",
     'area': "old",'hours': {
-      'sunday-start':"", 'sunday-end':"", 'monday-start':"!600", 'monday-end':"1800", 'tuesday-start':"!600", 'tuesday-end':"1800", 'wednesday-start':"!600", 'wednesday-end':"1800", 'thursday-start':"!600", 'thursday-end':"1800", 'friday-start':"!600", 'friday-end':"1800", 'saturday-start':"", 'saturday-end':""},  'description': "$5 Glasses of Wine", 'link':"", 'pricing':"med",   'phone-number': "", 'address': "234 N College Ave #3a, Fort Collins, CO 80524", 'other-amenities': ['outdoor','',''], 'has-drink':true, 'has-food':false},</v>
+      'sunday-start':"", 'sunday-end':"", 'monday-start':"1600", 'monday-end':"1800", 'tuesday-start':"1600", 'tuesday-end':"1800", 'wednesday-start':"1600", 'wednesday-end':"1800", 'thursday-start':"1600", 'thursday-end':"1800", 'friday-start':"1600", 'friday-end':"1800", 'saturday-start':"", 'saturday-end':""},  'description': "$5 Glasses of Wine", 'link':"", 'pricing':"med",   'phone-number': "", 'address': "234 N College Ave #3a, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':true, 'has-food':false},</v>
       </c>
       <c r="AY84" t="str">
         <f t="shared" ref="AY84" si="142">IF(AS84&gt;0,"&lt;img src=@img/outdoor.png@&gt;","")</f>
@@ -18826,7 +18825,7 @@
       </c>
       <c r="BA84" t="str">
         <f t="shared" ref="BA84" si="144">IF(AU84="hard","&lt;img src=@img/hard.png@&gt;",IF(AU84="medium","&lt;img src=@img/medium.png@&gt;",IF(AU84="easy","&lt;img src=@img/easy.png@&gt;","")))</f>
-        <v/>
+        <v>&lt;img src=@img/medium.png@&gt;</v>
       </c>
       <c r="BB84" t="str">
         <f t="shared" ref="BB84" si="145">IF(AV84="true","&lt;img src=@img/drinkicon.png@&gt;","")</f>
@@ -18838,11 +18837,11 @@
       </c>
       <c r="BD84" t="str">
         <f t="shared" ref="BD84" si="147">CONCATENATE(AY84,AZ84,BA84,BB84,BC84,BK84)</f>
-        <v>&lt;img src=@img/outdoor.png@&gt;&lt;img src=@img/drinkicon.png@&gt;</v>
+        <v>&lt;img src=@img/outdoor.png@&gt;&lt;img src=@img/medium.png@&gt;&lt;img src=@img/drinkicon.png@&gt;</v>
       </c>
       <c r="BE84" t="str">
         <f t="shared" ref="BE84" si="148">CONCATENATE(IF(AS84&gt;0,"outdoor ",""),IF(AT84&gt;0,"pet ",""),IF(AV84="true","drink ",""),IF(AW84="true","food ",""),AU84," ",E84," ",C84,IF(BJ84=TRUE," kid",""))</f>
-        <v>outdoor drink  med old</v>
+        <v>outdoor drink medium med old</v>
       </c>
       <c r="BF84" t="str">
         <f t="shared" ref="BF84" si="149">IF(C84="old","Old Town",IF(C84="campus","Near Campus",IF(C84="sfoco","South Foco",IF(C84="nfoco","North Foco",IF(C84="midtown","Midtown",IF(C84="cwest","Campus West",IF(C84="efoco","East FoCo",IF(C84="windsor","Windsor",""))))))))</f>
@@ -18863,7 +18862,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>195</v>
       </c>
@@ -19029,7 +19028,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>24</v>
       </c>
@@ -19246,7 +19245,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="87" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>669</v>
       </c>
@@ -19402,7 +19401,7 @@
         <v>[40.5315,-105.11594],</v>
       </c>
     </row>
-    <row r="88" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>597</v>
       </c>
@@ -19606,7 +19605,7 @@
         <v>[40.57428,-105.09835],</v>
       </c>
     </row>
-    <row r="89" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>92</v>
       </c>
@@ -19820,7 +19819,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>33</v>
       </c>
@@ -20034,7 +20033,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>115</v>
       </c>
@@ -20206,7 +20205,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>717</v>
       </c>
@@ -20312,7 +20311,7 @@
         <v>[40.562046,-105.038001],</v>
       </c>
     </row>
-    <row r="93" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>131</v>
       </c>
@@ -20478,7 +20477,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>785</v>
       </c>
@@ -20672,7 +20671,7 @@
         <v>[40.5738693,-105.1169419],</v>
       </c>
     </row>
-    <row r="95" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>95</v>
       </c>
@@ -20838,7 +20837,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>546</v>
       </c>
@@ -21052,7 +21051,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>601</v>
       </c>
@@ -21253,7 +21252,7 @@
         <v>[40.52366,-105.03402],</v>
       </c>
     </row>
-    <row r="98" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>376</v>
       </c>
@@ -21452,7 +21451,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>197</v>
       </c>
@@ -21666,7 +21665,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>605</v>
       </c>
@@ -21822,7 +21821,7 @@
         <v>[40.5831,-105.08285],</v>
       </c>
     </row>
-    <row r="101" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>282</v>
       </c>
@@ -22037,7 +22036,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>608</v>
       </c>
@@ -22193,7 +22192,7 @@
         <v>[40.58653,-105.07751],</v>
       </c>
     </row>
-    <row r="103" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>611</v>
       </c>
@@ -22346,7 +22345,7 @@
         <v>[40.58231,-105.10714],</v>
       </c>
     </row>
-    <row r="104" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>371</v>
       </c>
@@ -22548,7 +22547,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>665</v>
       </c>
@@ -22707,7 +22706,7 @@
         <v>[40.57914,-105.07946],</v>
       </c>
     </row>
-    <row r="106" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>164</v>
       </c>
@@ -22879,7 +22878,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>613</v>
       </c>
@@ -23035,7 +23034,7 @@
         <v>[40.55511,-105.07836],</v>
       </c>
     </row>
-    <row r="108" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>559</v>
       </c>
@@ -23242,7 +23241,7 @@
         <v>[40.57291,-105.1154],</v>
       </c>
     </row>
-    <row r="109" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>62</v>
       </c>
@@ -23408,7 +23407,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>198</v>
       </c>
@@ -23574,7 +23573,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>394</v>
       </c>
@@ -23749,7 +23748,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="112" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>657</v>
       </c>
@@ -23957,7 +23956,7 @@
         <v>[40.57532,-105.10038],</v>
       </c>
     </row>
-    <row r="113" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>121</v>
       </c>
@@ -24171,7 +24170,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>166</v>
       </c>
@@ -24382,7 +24381,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>200</v>
       </c>
@@ -24554,7 +24553,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>168</v>
       </c>
@@ -24762,7 +24761,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="117" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>655</v>
       </c>
@@ -24921,7 +24920,7 @@
         <v>[40.58358,-105.04801],</v>
       </c>
     </row>
-    <row r="118" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>123</v>
       </c>
@@ -25087,7 +25086,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>653</v>
       </c>
@@ -25246,7 +25245,7 @@
         <v>[40.55065,-105.04275],</v>
       </c>
     </row>
-    <row r="120" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>202</v>
       </c>
@@ -25418,7 +25417,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>143</v>
       </c>
@@ -25584,7 +25583,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>449</v>
       </c>
@@ -25750,7 +25749,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="123" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>753</v>
       </c>
@@ -25901,7 +25900,7 @@
         <v>[40.527959,-105.077616],</v>
       </c>
     </row>
-    <row r="124" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>616</v>
       </c>
@@ -26105,7 +26104,7 @@
         <v>[40.52143,-105.05755],</v>
       </c>
     </row>
-    <row r="125" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>620</v>
       </c>
@@ -26306,7 +26305,7 @@
         <v>[40.56741,-105.08268],</v>
       </c>
     </row>
-    <row r="126" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>89</v>
       </c>
@@ -26520,7 +26519,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>574</v>
       </c>
@@ -26715,7 +26714,7 @@
         <v>[40.58998,-105.0731],</v>
       </c>
     </row>
-    <row r="128" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>204</v>
       </c>
@@ -26926,7 +26925,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>206</v>
       </c>
@@ -27122,7 +27121,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>450</v>
       </c>
@@ -27288,7 +27287,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="131" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>654</v>
       </c>
@@ -27447,7 +27446,7 @@
         <v>[40.57789,-105.0766],</v>
       </c>
     </row>
-    <row r="132" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>650</v>
       </c>
@@ -27613,7 +27612,7 @@
         <v>[40.57855,-105.07975],</v>
       </c>
     </row>
-    <row r="133" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>208</v>
       </c>
@@ -27812,7 +27811,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>743</v>
       </c>
@@ -28016,7 +28015,7 @@
         <v>[40.52369,-105.03435],</v>
       </c>
     </row>
-    <row r="135" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>662</v>
       </c>
@@ -28175,7 +28174,7 @@
         <v>[40.573785,-105.0833606],</v>
       </c>
     </row>
-    <row r="136" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>170</v>
       </c>
@@ -28380,7 +28379,7 @@
         <v/>
       </c>
     </row>
-    <row r="137" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>43</v>
       </c>
@@ -28579,7 +28578,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>210</v>
       </c>
@@ -28793,7 +28792,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>59</v>
       </c>
@@ -28959,7 +28958,7 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>451</v>
       </c>
@@ -29125,7 +29124,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="141" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>663</v>
       </c>
@@ -29281,7 +29280,7 @@
         <v>[40.55258,-105.09673],</v>
       </c>
     </row>
-    <row r="142" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>213</v>
       </c>
@@ -29447,7 +29446,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>478</v>
       </c>
@@ -29613,7 +29612,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="144" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>651</v>
       </c>
@@ -29817,7 +29816,7 @@
         <v>[40.55475,-105.09774],</v>
       </c>
     </row>
-    <row r="145" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>752</v>
       </c>
@@ -29971,7 +29970,7 @@
         <v>[40.563256,-105.077464],</v>
       </c>
     </row>
-    <row r="146" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>397</v>
       </c>
@@ -30137,7 +30136,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>378</v>
       </c>
@@ -30345,7 +30344,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>652</v>
       </c>
@@ -30534,7 +30533,7 @@
         <v>[40.5635177,-105.077318],</v>
       </c>
     </row>
-    <row r="149" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>216</v>
       </c>
@@ -30745,7 +30744,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>285</v>
       </c>
@@ -30956,7 +30955,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>103</v>
       </c>
@@ -31161,7 +31160,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>137</v>
       </c>
@@ -31333,7 +31332,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="153" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>118</v>
       </c>
@@ -31499,7 +31498,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>623</v>
       </c>
@@ -31655,7 +31654,7 @@
         <v>[40.58742,-105.0784],</v>
       </c>
     </row>
-    <row r="155" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>40</v>
       </c>
@@ -31830,7 +31829,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="156" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>37</v>
       </c>
@@ -32041,7 +32040,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>664</v>
       </c>
@@ -32194,7 +32193,7 @@
         <v>[40.58213,-105.02703],</v>
       </c>
     </row>
-    <row r="158" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>375</v>
       </c>
@@ -32360,7 +32359,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>536</v>
       </c>
@@ -32565,7 +32564,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>666</v>
       </c>
@@ -32724,7 +32723,7 @@
         <v>[40.62701,-105.13785],</v>
       </c>
     </row>
-    <row r="161" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>112</v>
       </c>
@@ -32920,7 +32919,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>542</v>
       </c>
@@ -33122,7 +33121,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>80</v>
       </c>
@@ -33295,7 +33294,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>667</v>
       </c>
@@ -33463,7 +33462,7 @@
         <v>[40.66018,-105.161719],</v>
       </c>
     </row>
-    <row r="165" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>452</v>
       </c>
@@ -33629,7 +33628,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="166" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>100</v>
       </c>
@@ -33795,7 +33794,7 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>626</v>
       </c>
@@ -33948,7 +33947,7 @@
         <v>[40.57906,-105.07656],</v>
       </c>
     </row>
-    <row r="168" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>83</v>
       </c>
@@ -34117,7 +34116,7 @@
         <v/>
       </c>
     </row>
-    <row r="169" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>218</v>
       </c>
@@ -34316,7 +34315,7 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>628</v>
       </c>
@@ -34496,7 +34495,7 @@
         <v>[40.56208,-105.03864],</v>
       </c>
     </row>
-    <row r="171" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>173</v>
       </c>
@@ -34695,7 +34694,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>571</v>
       </c>
@@ -34860,7 +34859,7 @@
         <v>[40.57891,-105.07843],</v>
       </c>
     </row>
-    <row r="173" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>754</v>
       </c>
@@ -35011,7 +35010,7 @@
         <v>[40.586451,-105.078568],</v>
       </c>
     </row>
-    <row r="174" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>699</v>
       </c>
@@ -35212,7 +35211,7 @@
         <v>[40.58815,-105.07761],</v>
       </c>
     </row>
-    <row r="175" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>631</v>
       </c>
@@ -35368,7 +35367,7 @@
         <v>[40.58899,-105.07637],</v>
       </c>
     </row>
-    <row r="176" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>564</v>
       </c>
@@ -35530,7 +35529,7 @@
         <v>[40.58487,-105.0765],</v>
       </c>
     </row>
-    <row r="177" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>634</v>
       </c>
@@ -35689,7 +35688,7 @@
         <v>[40.58758,-105.07636],</v>
       </c>
     </row>
-    <row r="178" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>453</v>
       </c>
@@ -35855,7 +35854,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="179" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>220</v>
       </c>
@@ -36069,7 +36068,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>380</v>
       </c>
@@ -36271,7 +36270,7 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>223</v>
       </c>
@@ -36437,7 +36436,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>553</v>
       </c>
@@ -36633,7 +36632,7 @@
         <v>[40.58741,-105.07661],</v>
       </c>
     </row>
-    <row r="183" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>636</v>
       </c>
@@ -36786,7 +36785,7 @@
         <v>[40.57844,-105.07856],</v>
       </c>
     </row>
-    <row r="184" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>287</v>
       </c>
@@ -36997,7 +36996,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>401</v>
       </c>
@@ -37166,7 +37165,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>750</v>
       </c>
@@ -37317,7 +37316,7 @@
         <v>[40.523973,-105.025125],</v>
       </c>
     </row>
-    <row r="187" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>748</v>
       </c>
@@ -37471,7 +37470,7 @@
         <v>[40.589425,-105.076553],</v>
       </c>
     </row>
-    <row r="188" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>638</v>
       </c>
@@ -37627,7 +37626,7 @@
         <v>[40.57429,-105.0971],</v>
       </c>
     </row>
-    <row r="189" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>660</v>
       </c>
@@ -37780,7 +37779,7 @@
         <v>[40.55258,-105.09673],</v>
       </c>
     </row>
-    <row r="190" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>128</v>
       </c>
@@ -37952,7 +37951,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>550</v>
       </c>
@@ -38117,7 +38116,7 @@
         <v>[40.55197,-105.03718],</v>
       </c>
     </row>
-    <row r="192" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>641</v>
       </c>
@@ -38286,7 +38285,7 @@
         <v>[40.57358,-105.05826],</v>
       </c>
     </row>
-    <row r="193" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>225</v>
       </c>
@@ -38444,7 +38443,7 @@
         <v/>
       </c>
     </row>
-    <row r="194" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>49</v>
       </c>
@@ -38602,7 +38601,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>645</v>
       </c>
@@ -38757,7 +38756,7 @@
         <v>[40.57488,-105.10039],</v>
       </c>
     </row>
-    <row r="196" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>227</v>
       </c>
@@ -38937,77 +38936,77 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C2:C191" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:BL197">
+  <autoFilter ref="C2:C191"/>
+  <sortState ref="B2:BL197">
     <sortCondition ref="B2:B197"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G136" r:id="rId1" display="https://www.google.com/maps/dir/Current+Location/101 S. College Avenue, Fort Collins, CO 80524" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="AR42" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="AR99" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="AR28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="AR115" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="AR20" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="AR8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="AR55" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="AR34" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="AR64" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="AR46" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="AR163" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="AR54" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="AR126" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="AR95" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="AR63" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="AR166" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="AR151" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="AR19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="AR10" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="AR161" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="AR91" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="AR153" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="AR113" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="AR190" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="AR93" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="AR15" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="AR86" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="AR5" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="AR7" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="AR43" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="AR45" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="AR57" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="AR82" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="AR106" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="AR114" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="AR116" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="AR136" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="AR16" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="AR24" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="AR62" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="AR80" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="AR85" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="AR110" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="AR128" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="AR138" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="AR142" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="AR149" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="AR169" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="AR181" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="AR196" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="AR23" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="AR58" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="AR66" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="AR67" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="AR77" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="AR101" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="AR150" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="AR184" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="AR59" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="AR79" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="AR48" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="AR9" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="AR174" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B11" r:id="rId65" display="https://www.yelp.com/biz/avuncular-bobs-beerhouse-fort-collins" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="AR172" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="G136" r:id="rId1" display="https://www.google.com/maps/dir/Current+Location/101 S. College Avenue, Fort Collins, CO 80524"/>
+    <hyperlink ref="AR42" r:id="rId2"/>
+    <hyperlink ref="AR99" r:id="rId3"/>
+    <hyperlink ref="AR28" r:id="rId4"/>
+    <hyperlink ref="AR115" r:id="rId5"/>
+    <hyperlink ref="AR20" r:id="rId6"/>
+    <hyperlink ref="AR8" r:id="rId7"/>
+    <hyperlink ref="AR55" r:id="rId8"/>
+    <hyperlink ref="AR34" r:id="rId9"/>
+    <hyperlink ref="AR64" r:id="rId10"/>
+    <hyperlink ref="AR46" r:id="rId11"/>
+    <hyperlink ref="AR163" r:id="rId12"/>
+    <hyperlink ref="AR54" r:id="rId13"/>
+    <hyperlink ref="AR126" r:id="rId14"/>
+    <hyperlink ref="AR95" r:id="rId15"/>
+    <hyperlink ref="AR63" r:id="rId16"/>
+    <hyperlink ref="AR166" r:id="rId17"/>
+    <hyperlink ref="AR151" r:id="rId18"/>
+    <hyperlink ref="AR19" r:id="rId19"/>
+    <hyperlink ref="AR10" r:id="rId20"/>
+    <hyperlink ref="AR161" r:id="rId21"/>
+    <hyperlink ref="AR91" r:id="rId22"/>
+    <hyperlink ref="AR153" r:id="rId23"/>
+    <hyperlink ref="AR113" r:id="rId24"/>
+    <hyperlink ref="AR190" r:id="rId25"/>
+    <hyperlink ref="AR93" r:id="rId26"/>
+    <hyperlink ref="AR15" r:id="rId27"/>
+    <hyperlink ref="AR86" r:id="rId28"/>
+    <hyperlink ref="AR5" r:id="rId29"/>
+    <hyperlink ref="AR7" r:id="rId30"/>
+    <hyperlink ref="AR43" r:id="rId31"/>
+    <hyperlink ref="AR45" r:id="rId32"/>
+    <hyperlink ref="AR57" r:id="rId33"/>
+    <hyperlink ref="AR82" r:id="rId34"/>
+    <hyperlink ref="AR106" r:id="rId35"/>
+    <hyperlink ref="AR114" r:id="rId36"/>
+    <hyperlink ref="AR116" r:id="rId37"/>
+    <hyperlink ref="AR136" r:id="rId38"/>
+    <hyperlink ref="AR16" r:id="rId39"/>
+    <hyperlink ref="AR24" r:id="rId40"/>
+    <hyperlink ref="AR62" r:id="rId41"/>
+    <hyperlink ref="AR80" r:id="rId42"/>
+    <hyperlink ref="AR85" r:id="rId43"/>
+    <hyperlink ref="AR110" r:id="rId44"/>
+    <hyperlink ref="AR128" r:id="rId45"/>
+    <hyperlink ref="AR138" r:id="rId46"/>
+    <hyperlink ref="AR142" r:id="rId47"/>
+    <hyperlink ref="AR149" r:id="rId48"/>
+    <hyperlink ref="AR169" r:id="rId49"/>
+    <hyperlink ref="AR181" r:id="rId50"/>
+    <hyperlink ref="AR196" r:id="rId51"/>
+    <hyperlink ref="AR23" r:id="rId52"/>
+    <hyperlink ref="AR58" r:id="rId53"/>
+    <hyperlink ref="AR66" r:id="rId54"/>
+    <hyperlink ref="AR67" r:id="rId55"/>
+    <hyperlink ref="AR77" r:id="rId56"/>
+    <hyperlink ref="AR101" r:id="rId57"/>
+    <hyperlink ref="AR150" r:id="rId58"/>
+    <hyperlink ref="AR184" r:id="rId59"/>
+    <hyperlink ref="AR59" r:id="rId60"/>
+    <hyperlink ref="AR79" r:id="rId61"/>
+    <hyperlink ref="AR48" r:id="rId62"/>
+    <hyperlink ref="AR9" r:id="rId63"/>
+    <hyperlink ref="AR174" r:id="rId64"/>
+    <hyperlink ref="B11" r:id="rId65" display="https://www.yelp.com/biz/avuncular-bobs-beerhouse-fort-collins"/>
+    <hyperlink ref="AR172" r:id="rId66"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId67"/>
@@ -39015,19 +39014,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>769</v>
       </c>
@@ -39044,7 +39043,7 @@
         <v>-105.076553</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>772</v>
       </c>
@@ -39061,7 +39060,7 @@
         <v>-105.076497</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>773</v>
       </c>
@@ -39078,7 +39077,7 @@
         <v>-105.025125</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>775</v>
       </c>
@@ -39095,7 +39094,7 @@
         <v>-105.05831000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>777</v>
       </c>
@@ -39112,7 +39111,7 @@
         <v>-105.07746400000001</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>778</v>
       </c>
@@ -39129,7 +39128,7 @@
         <v>-105.07761600000001</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>779</v>
       </c>
@@ -39155,14 +39154,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <customProperties>

</xml_diff>

<commit_message>
Added swing station deal
</commit_message>
<xml_diff>
--- a/database_working.xlsx
+++ b/database_working.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="800">
   <si>
     <t>Name</t>
   </si>
@@ -2431,6 +2431,9 @@
   </si>
   <si>
     <t>pet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ride Your Bike For $1 Off All Draft Beer&lt;br&gt;2 Live Music Stages - Indoor And Outdoor&lt;br&gt;Happy Hour 2-7pm - Monday - Friday&lt;br&gt;Open Mic Every Wednesday Night </t>
   </si>
 </sst>
 </file>
@@ -3392,10 +3395,10 @@
   <dimension ref="B1:BL196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AE74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AE140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="U86" sqref="U86"/>
-      <selection pane="bottomRight" activeCell="AU85" sqref="AU85"/>
+      <selection pane="bottomRight" activeCell="AV161" sqref="AV161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32577,6 +32580,39 @@
       <c r="G160" t="s">
         <v>694</v>
       </c>
+      <c r="J160">
+        <v>1400</v>
+      </c>
+      <c r="K160">
+        <v>1900</v>
+      </c>
+      <c r="L160">
+        <v>1400</v>
+      </c>
+      <c r="M160">
+        <v>1900</v>
+      </c>
+      <c r="N160">
+        <v>1400</v>
+      </c>
+      <c r="O160">
+        <v>1900</v>
+      </c>
+      <c r="P160">
+        <v>1400</v>
+      </c>
+      <c r="Q160">
+        <v>1900</v>
+      </c>
+      <c r="R160">
+        <v>1400</v>
+      </c>
+      <c r="S160">
+        <v>1900</v>
+      </c>
+      <c r="V160" s="4" t="s">
+        <v>799</v>
+      </c>
       <c r="W160" t="str">
         <f t="shared" si="232"/>
         <v/>
@@ -32585,45 +32621,45 @@
         <f t="shared" si="233"/>
         <v/>
       </c>
-      <c r="Y160" t="str">
+      <c r="Y160">
         <f t="shared" si="234"/>
-        <v/>
-      </c>
-      <c r="Z160" t="str">
+        <v>14</v>
+      </c>
+      <c r="Z160">
         <f t="shared" si="235"/>
-        <v/>
-      </c>
-      <c r="AA160" t="str">
+        <v>19</v>
+      </c>
+      <c r="AA160">
         <f t="shared" si="236"/>
-        <v/>
-      </c>
-      <c r="AB160" t="str">
+        <v>14</v>
+      </c>
+      <c r="AB160">
         <f t="shared" si="237"/>
-        <v/>
-      </c>
-      <c r="AC160" t="str">
+        <v>19</v>
+      </c>
+      <c r="AC160">
         <f t="shared" si="238"/>
-        <v/>
-      </c>
-      <c r="AD160" t="str">
+        <v>14</v>
+      </c>
+      <c r="AD160">
         <f t="shared" si="239"/>
-        <v/>
-      </c>
-      <c r="AE160" t="str">
+        <v>19</v>
+      </c>
+      <c r="AE160">
         <f t="shared" si="230"/>
-        <v/>
-      </c>
-      <c r="AF160" t="str">
+        <v>14</v>
+      </c>
+      <c r="AF160">
         <f t="shared" si="231"/>
-        <v/>
-      </c>
-      <c r="AG160" t="str">
+        <v>19</v>
+      </c>
+      <c r="AG160">
         <f t="shared" si="240"/>
-        <v/>
-      </c>
-      <c r="AH160" t="str">
+        <v>14</v>
+      </c>
+      <c r="AH160">
         <f t="shared" si="241"/>
-        <v/>
+        <v>19</v>
       </c>
       <c r="AI160" t="str">
         <f t="shared" si="242"/>
@@ -32639,23 +32675,23 @@
       </c>
       <c r="AL160" t="str">
         <f t="shared" si="223"/>
-        <v/>
+        <v>2pm-7pm</v>
       </c>
       <c r="AM160" t="str">
         <f t="shared" si="224"/>
-        <v/>
+        <v>2pm-7pm</v>
       </c>
       <c r="AN160" t="str">
         <f t="shared" si="225"/>
-        <v/>
+        <v>2pm-7pm</v>
       </c>
       <c r="AO160" t="str">
         <f t="shared" si="226"/>
-        <v/>
+        <v>2pm-7pm</v>
       </c>
       <c r="AP160" t="str">
         <f t="shared" si="227"/>
-        <v/>
+        <v>2pm-7pm</v>
       </c>
       <c r="AQ160" t="str">
         <f t="shared" si="228"/>
@@ -32668,7 +32704,7 @@
         <v>28</v>
       </c>
       <c r="AV160" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AW160" s="3" t="s">
         <v>307</v>
@@ -32678,7 +32714,7 @@
         <v>{
     'name': "Swing Station",
     'area': "nfoco",'hours': {
-      'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"", 'wednesday-end':"", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "", 'link':"", 'pricing':"low",   'phone-number': "", 'address': "3311 Co Road 54G Laporte CO", 'other-amenities': ['outdoor','','medium'], 'has-drink':false, 'has-food':false},</v>
+      'sunday-start':"", 'sunday-end':"", 'monday-start':"1400", 'monday-end':"1900", 'tuesday-start':"1400", 'tuesday-end':"1900", 'wednesday-start':"1400", 'wednesday-end':"1900", 'thursday-start':"1400", 'thursday-end':"1900", 'friday-start':"1400", 'friday-end':"1900", 'saturday-start':"", 'saturday-end':""},  'description': "Ride Your Bike For $1 Off All Draft Beer&lt;br&gt;2 Live Music Stages - Indoor And Outdoor&lt;br&gt;Happy Hour 2-7pm - Monday - Friday&lt;br&gt;Open Mic Every Wednesday Night ", 'link':"", 'pricing':"low",   'phone-number': "", 'address': "3311 Co Road 54G Laporte CO", 'other-amenities': ['outdoor','','medium'], 'has-drink':true, 'has-food':false},</v>
       </c>
       <c r="AY160" t="str">
         <f t="shared" si="213"/>
@@ -32694,7 +32730,7 @@
       </c>
       <c r="BB160" t="str">
         <f t="shared" si="216"/>
-        <v/>
+        <v>&lt;img src=@img/drinkicon.png@&gt;</v>
       </c>
       <c r="BC160" t="str">
         <f t="shared" si="217"/>
@@ -32702,11 +32738,11 @@
       </c>
       <c r="BD160" t="str">
         <f t="shared" si="218"/>
-        <v>&lt;img src=@img/outdoor.png@&gt;&lt;img src=@img/medium.png@&gt;</v>
+        <v>&lt;img src=@img/outdoor.png@&gt;&lt;img src=@img/medium.png@&gt;&lt;img src=@img/drinkicon.png@&gt;</v>
       </c>
       <c r="BE160" t="str">
         <f t="shared" si="219"/>
-        <v>outdoor medium low nfoco</v>
+        <v>outdoor drink medium low nfoco</v>
       </c>
       <c r="BF160" t="str">
         <f t="shared" si="220"/>

</xml_diff>

<commit_message>
Updated louie and muse
</commit_message>
<xml_diff>
--- a/database_working.xlsx
+++ b/database_working.xlsx
@@ -1498,9 +1498,6 @@
     <t>$4 drafts &lt;br&gt; $4.50 wells &lt;br&gt; $6 wine</t>
   </si>
   <si>
-    <t>Sundays: $2 off Bloody Mary’s &lt;br&gt; Wed-Thur: &lt;br&gt; $6 select cocktails including mules &lt;br&gt; $2 off select appetizers</t>
-  </si>
-  <si>
     <t>Premium Wells: $3.50 &lt;br&gt; Martini’s &amp; Manhattan's: $5.00  &lt;br&gt; Select Draft Beers: $3.50 &lt;br&gt; House Wines: $3.50 &lt;br&gt; A range of food specials</t>
   </si>
   <si>
@@ -2198,9 +2195,6 @@
     <t>347 E Foothills Pkwy #110, Fort Collins, CO 80525</t>
   </si>
   <si>
-    <t>$4 Green Chile Cheese Tots </t>
-  </si>
-  <si>
     <t>$4 Queso with chips </t>
   </si>
   <si>
@@ -2434,13 +2428,19 @@
   </si>
   <si>
     <t>Mondays: Happy Hour All Day! $5 pints - $4 12oz. Buy a Rally King T-shirt and get a free beer! FREE fresh-baked, chocolate chip cookies  5pm-8 pm &lt;br&gt;Tuesdays: Wear Rally King gear for BOGO beers!&lt;br&gt;Wednesdays:Happy Hour 2pm-4pm&lt;br&gt;Thursdays:Happy Hour 2pm-4pm&lt;br&gt;Fridays: Sour Fridays! Small batch sours released every Friday @2:00pm</t>
+  </si>
+  <si>
+    <t>Sundays: $2 off Bloody Mary’s &lt;br&gt; Wed-Thur: &lt;br&gt; $6 select cocktails including mules &lt;br&gt; Spinach Artichoke Dip $8&lt;br&gt;Bacon Wrapped Scallops $13&lt;br&gt;Meat and Cheese Board $13</t>
+  </si>
+  <si>
+    <t>$3.50 All 14 oz Drafts&lt;br&gt;$4.50 Wines by the Glass&lt;br&gt;$5.50 Signauture Martinis&lt;br&gt;Half Off Select Appetizers and Flatbreads</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2635,6 +2635,11 @@
       <u/>
       <sz val="6"/>
       <color rgb="FF4285F4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2981,7 +2986,7 @@
     <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -3008,6 +3013,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -3395,10 +3401,10 @@
   <dimension ref="B1:BL196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E115" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="U86" sqref="U86"/>
-      <selection pane="bottomRight" activeCell="AA128" sqref="AA128"/>
+      <selection pane="bottomRight" activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3797,7 +3803,7 @@
         <v>&lt;img src=@img/kidicon.png@&gt;</v>
       </c>
       <c r="BL2" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="3" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4010,7 +4016,7 @@
     </row>
     <row r="4" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C4" t="s">
         <v>426</v>
@@ -4019,7 +4025,7 @@
         <v>431</v>
       </c>
       <c r="G4" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="W4" t="str">
         <f t="shared" si="0"/>
@@ -4106,7 +4112,7 @@
         <v/>
       </c>
       <c r="AR4" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="AU4" t="s">
         <v>298</v>
@@ -4335,19 +4341,19 @@
     </row>
     <row r="6" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C6" t="s">
         <v>308</v>
       </c>
       <c r="D6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E6" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="W6" t="str">
         <f t="shared" si="0"/>
@@ -4728,7 +4734,7 @@
         <v>1800</v>
       </c>
       <c r="V8" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
@@ -4885,19 +4891,19 @@
     </row>
     <row r="9" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C9" t="s">
         <v>426</v>
       </c>
       <c r="D9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E9" t="s">
         <v>431</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H9">
         <v>1500</v>
@@ -4942,7 +4948,7 @@
         <v>1800</v>
       </c>
       <c r="V9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="W9">
         <f t="shared" si="0"/>
@@ -5313,19 +5319,19 @@
     </row>
     <row r="11" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C11" t="s">
         <v>308</v>
       </c>
       <c r="D11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E11" t="s">
         <v>431</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="W11" t="str">
         <f t="shared" si="0"/>
@@ -5412,7 +5418,7 @@
         <v/>
       </c>
       <c r="AR11" s="10" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="AU11" t="s">
         <v>28</v>
@@ -5475,19 +5481,19 @@
     </row>
     <row r="12" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C12" t="s">
         <v>427</v>
       </c>
       <c r="D12" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E12" t="s">
         <v>431</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="0"/>
@@ -5639,7 +5645,7 @@
     </row>
     <row r="13" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C13" t="s">
         <v>426</v>
@@ -5648,7 +5654,7 @@
         <v>431</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="0"/>
@@ -5800,7 +5806,7 @@
     </row>
     <row r="14" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C14" t="s">
         <v>309</v>
@@ -5809,7 +5815,7 @@
         <v>431</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="H14">
         <v>1500</v>
@@ -5854,7 +5860,7 @@
         <v>1800</v>
       </c>
       <c r="V14" s="14" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="W14">
         <f t="shared" si="0"/>
@@ -5941,7 +5947,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR14" s="2" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="AS14" t="s">
         <v>295</v>
@@ -5950,7 +5956,7 @@
         <v>299</v>
       </c>
       <c r="AV14" s="7" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="AW14" s="3" t="s">
         <v>306</v>
@@ -6218,8 +6224,8 @@
       <c r="S16">
         <v>1900</v>
       </c>
-      <c r="V16" s="14" t="s">
-        <v>721</v>
+      <c r="V16" s="16" t="s">
+        <v>799</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="0"/>
@@ -6325,7 +6331,7 @@
         <v>{
     'name': "Bar Louie",
     'area': "midtown",'hours': {
-      'sunday-start':"", 'sunday-end':"", 'monday-start':"1600", 'monday-end':"1900", 'tuesday-start':"1600", 'tuesday-end':"1900", 'wednesday-start':"1600", 'wednesday-end':"1900", 'thursday-start':"1600", 'thursday-end':"1900", 'friday-start':"1600", 'friday-end':"1900", 'saturday-start':"", 'saturday-end':""},  'description': "$4 Green Chile Cheese Tots ", 'link':"http://www.barlouie.com/locations/states/colorado/foothills-mall-fort-collins/", 'pricing':"med",   'phone-number': "", 'address': "321 E Foothills Pkwy, Fort Collins, CO 80525", 'other-amenities': ['outdoor','','easy'], 'has-drink':true, 'has-food':true},</v>
+      'sunday-start':"", 'sunday-end':"", 'monday-start':"1600", 'monday-end':"1900", 'tuesday-start':"1600", 'tuesday-end':"1900", 'wednesday-start':"1600", 'wednesday-end':"1900", 'thursday-start':"1600", 'thursday-end':"1900", 'friday-start':"1600", 'friday-end':"1900", 'saturday-start':"", 'saturday-end':""},  'description': "$3.50 All 14 oz Drafts&lt;br&gt;$4.50 Wines by the Glass&lt;br&gt;$5.50 Signauture Martinis&lt;br&gt;Half Off Select Appetizers and Flatbreads", 'link':"http://www.barlouie.com/locations/states/colorado/foothills-mall-fort-collins/", 'pricing':"med",   'phone-number': "", 'address': "321 E Foothills Pkwy, Fort Collins, CO 80525", 'other-amenities': ['outdoor','','easy'], 'has-drink':true, 'has-food':true},</v>
       </c>
       <c r="AY16" t="str">
         <f t="shared" si="16"/>
@@ -6376,16 +6382,16 @@
     </row>
     <row r="17" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C17" t="s">
         <v>308</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="V17" s="14" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="W17" t="str">
         <f t="shared" si="0"/>
@@ -6472,7 +6478,7 @@
         <v/>
       </c>
       <c r="AR17" s="12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="AS17" t="s">
         <v>295</v>
@@ -6595,7 +6601,7 @@
         <v>1800</v>
       </c>
       <c r="V18" s="14" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="W18">
         <f t="shared" si="0"/>
@@ -6815,7 +6821,7 @@
         <v>2400</v>
       </c>
       <c r="V19" s="14" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="W19">
         <f t="shared" si="0"/>
@@ -7391,7 +7397,7 @@
         <v>1800</v>
       </c>
       <c r="V22" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="W22">
         <f t="shared" si="0"/>
@@ -7967,7 +7973,7 @@
     </row>
     <row r="25" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C25" t="s">
         <v>426</v>
@@ -7976,7 +7982,7 @@
         <v>431</v>
       </c>
       <c r="G25" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="P25">
         <v>2000</v>
@@ -7997,7 +8003,7 @@
         <v>2000</v>
       </c>
       <c r="V25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="W25" t="str">
         <f t="shared" si="0"/>
@@ -8084,7 +8090,7 @@
         <v>6pm-8pm</v>
       </c>
       <c r="AR25" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="AU25" t="s">
         <v>298</v>
@@ -8331,19 +8337,19 @@
     </row>
     <row r="27" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C27" t="s">
         <v>309</v>
       </c>
       <c r="D27" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E27" t="s">
         <v>54</v>
       </c>
       <c r="G27" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="W27" t="str">
         <f t="shared" si="0"/>
@@ -8666,7 +8672,7 @@
     </row>
     <row r="29" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C29" t="s">
         <v>309</v>
@@ -8675,7 +8681,7 @@
         <v>431</v>
       </c>
       <c r="G29" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="W29" t="str">
         <f t="shared" si="0"/>
@@ -8822,7 +8828,7 @@
     </row>
     <row r="30" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C30" t="s">
         <v>428</v>
@@ -8831,7 +8837,7 @@
         <v>431</v>
       </c>
       <c r="G30" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="W30" t="str">
         <f t="shared" si="0"/>
@@ -8983,7 +8989,7 @@
     </row>
     <row r="31" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C31" t="s">
         <v>308</v>
@@ -8992,7 +8998,7 @@
         <v>431</v>
       </c>
       <c r="G31" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="W31" t="str">
         <f t="shared" si="0"/>
@@ -9144,13 +9150,13 @@
     </row>
     <row r="32" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C32" t="s">
         <v>429</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="W32" t="str">
         <f t="shared" si="0"/>
@@ -9237,7 +9243,7 @@
         <v/>
       </c>
       <c r="AR32" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="AU32" t="s">
         <v>299</v>
@@ -9300,13 +9306,13 @@
     </row>
     <row r="33" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C33" t="s">
         <v>309</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="W33" t="str">
         <f t="shared" si="0"/>
@@ -9393,7 +9399,7 @@
         <v/>
       </c>
       <c r="AR33" s="10" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="AU33" t="s">
         <v>299</v>
@@ -9511,7 +9517,7 @@
         <v>1800</v>
       </c>
       <c r="V34" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="W34" t="str">
         <f t="shared" ref="W34:W64" si="34">IF(H34&gt;0,H34/100,"")</f>
@@ -9672,13 +9678,13 @@
     </row>
     <row r="35" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C35" t="s">
         <v>426</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="W35" t="str">
         <f t="shared" si="34"/>
@@ -9765,7 +9771,7 @@
         <v/>
       </c>
       <c r="AR35" s="12" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="AU35" t="s">
         <v>28</v>
@@ -10254,7 +10260,7 @@
         <v>&lt;img src=@img/kidicon.png@&gt;</v>
       </c>
       <c r="BL37" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="38" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -10461,13 +10467,13 @@
     </row>
     <row r="39" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C39" t="s">
         <v>427</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="W39" t="str">
         <f t="shared" si="34"/>
@@ -10554,7 +10560,7 @@
         <v/>
       </c>
       <c r="AR39" s="12" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="AU39" t="s">
         <v>299</v>
@@ -10786,16 +10792,16 @@
     </row>
     <row r="41" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C41" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E41" t="s">
         <v>431</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="H41">
         <v>1600</v>
@@ -10840,7 +10846,7 @@
         <v>1800</v>
       </c>
       <c r="V41" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="W41">
         <f t="shared" si="34"/>
@@ -10927,7 +10933,7 @@
         <v>4pm-6pm</v>
       </c>
       <c r="AR41" s="6" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="AU41" t="s">
         <v>28</v>
@@ -11383,7 +11389,7 @@
         <v>1800</v>
       </c>
       <c r="V44" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="W44" t="str">
         <f t="shared" si="34"/>
@@ -11576,7 +11582,7 @@
         <v>2100</v>
       </c>
       <c r="V45" t="s">
-        <v>488</v>
+        <v>798</v>
       </c>
       <c r="W45">
         <f t="shared" si="34"/>
@@ -11682,7 +11688,7 @@
         <v>{
     'name': "CopperMuse Distillery",
     'area': "old",'hours': {
-      'sunday-start':"1200", 'sunday-end':"1900", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"1600", 'wednesday-end':"2100", 'thursday-start':"1600", 'thursday-end':"2100", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "Sundays: $2 off Bloody Mary’s &lt;br&gt; Wed-Thur: &lt;br&gt; $6 select cocktails including mules &lt;br&gt; $2 off select appetizers", 'link':"http://www.coppermuse.com/", 'pricing':"med",   'phone-number': "", 'address': "244 N. College Ave, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':true, 'has-food':true},</v>
+      'sunday-start':"1200", 'sunday-end':"1900", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"1600", 'wednesday-end':"2100", 'thursday-start':"1600", 'thursday-end':"2100", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "Sundays: $2 off Bloody Mary’s &lt;br&gt; Wed-Thur: &lt;br&gt; $6 select cocktails including mules &lt;br&gt; Spinach Artichoke Dip $8&lt;br&gt;Bacon Wrapped Scallops $13&lt;br&gt;Meat and Cheese Board $13", 'link':"http://www.coppermuse.com/", 'pricing':"med",   'phone-number': "", 'address': "244 N. College Ave, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':true, 'has-food':true},</v>
       </c>
       <c r="AY45" t="str">
         <f t="shared" si="49"/>
@@ -11790,7 +11796,7 @@
         <v>2400</v>
       </c>
       <c r="V46" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="W46">
         <f t="shared" si="34"/>
@@ -11947,7 +11953,7 @@
     </row>
     <row r="47" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C47" t="s">
         <v>426</v>
@@ -11956,7 +11962,7 @@
         <v>431</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="W47" t="str">
         <f t="shared" ref="W47" si="59">IF(H47&gt;0,H47/100,"")</f>
@@ -12047,7 +12053,7 @@
         <v>295</v>
       </c>
       <c r="AT47" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="AU47" t="s">
         <v>298</v>
@@ -12482,7 +12488,7 @@
     </row>
     <row r="50" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C50" t="s">
         <v>428</v>
@@ -12681,7 +12687,7 @@
     </row>
     <row r="51" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C51" t="s">
         <v>426</v>
@@ -12690,7 +12696,7 @@
         <v>54</v>
       </c>
       <c r="G51" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="W51" t="str">
         <f t="shared" si="34"/>
@@ -12777,7 +12783,7 @@
         <v/>
       </c>
       <c r="AR51" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="AU51" t="s">
         <v>298</v>
@@ -12840,7 +12846,7 @@
     </row>
     <row r="52" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C52" t="s">
         <v>426</v>
@@ -12849,7 +12855,7 @@
         <v>431</v>
       </c>
       <c r="G52" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="W52" t="str">
         <f t="shared" si="34"/>
@@ -12936,7 +12942,7 @@
         <v/>
       </c>
       <c r="AR52" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="AS52" t="s">
         <v>295</v>
@@ -13002,7 +13008,7 @@
     </row>
     <row r="53" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C53" t="s">
         <v>309</v>
@@ -13011,7 +13017,7 @@
         <v>431</v>
       </c>
       <c r="G53" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H53">
         <v>1600</v>
@@ -13044,7 +13050,7 @@
         <v>1900</v>
       </c>
       <c r="V53" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="W53">
         <f t="shared" si="34"/>
@@ -13131,7 +13137,7 @@
         <v/>
       </c>
       <c r="AR53" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="AU53" t="s">
         <v>299</v>
@@ -13526,7 +13532,7 @@
     </row>
     <row r="56" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C56" t="s">
         <v>427</v>
@@ -13535,7 +13541,7 @@
         <v>431</v>
       </c>
       <c r="G56" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="L56">
         <v>1600</v>
@@ -13568,7 +13574,7 @@
         <v>1800</v>
       </c>
       <c r="V56" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="W56" t="str">
         <f t="shared" si="34"/>
@@ -13655,7 +13661,7 @@
         <v>4pm-6pm</v>
       </c>
       <c r="AR56" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="AU56" t="s">
         <v>299</v>
@@ -13745,7 +13751,7 @@
         <v>1800</v>
       </c>
       <c r="V57" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="W57" t="str">
         <f t="shared" si="34"/>
@@ -13947,7 +13953,7 @@
         <v>1900</v>
       </c>
       <c r="V58" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="W58" t="str">
         <f t="shared" si="34"/>
@@ -14158,7 +14164,7 @@
         <v>1800</v>
       </c>
       <c r="V59" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="W59">
         <f t="shared" si="34"/>
@@ -14312,7 +14318,7 @@
     </row>
     <row r="60" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C60" t="s">
         <v>426</v>
@@ -14321,7 +14327,7 @@
         <v>54</v>
       </c>
       <c r="G60" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="W60" t="str">
         <f t="shared" si="34"/>
@@ -14408,7 +14414,7 @@
         <v/>
       </c>
       <c r="AR60" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="AU60" t="s">
         <v>298</v>
@@ -14860,7 +14866,7 @@
         <v>1800</v>
       </c>
       <c r="V63" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="W63">
         <f t="shared" si="34"/>
@@ -15180,7 +15186,7 @@
     </row>
     <row r="65" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C65" t="s">
         <v>426</v>
@@ -15189,7 +15195,7 @@
         <v>54</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="W65" t="str">
         <f t="shared" ref="W65:W91" si="89">IF(H65&gt;0,H65/100,"")</f>
@@ -15268,7 +15274,7 @@
         <v/>
       </c>
       <c r="AR65" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="AS65" t="s">
         <v>295</v>
@@ -15593,7 +15599,7 @@
         <v>1800</v>
       </c>
       <c r="V67" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="W67" t="str">
         <f t="shared" si="89"/>
@@ -15751,7 +15757,7 @@
     </row>
     <row r="68" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C68" t="s">
         <v>309</v>
@@ -15760,7 +15766,7 @@
         <v>431</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="W68" t="str">
         <f t="shared" si="89"/>
@@ -15839,7 +15845,7 @@
         <v/>
       </c>
       <c r="AR68" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="AU68" t="s">
         <v>299</v>
@@ -15902,13 +15908,13 @@
     </row>
     <row r="69" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C69" t="s">
         <v>426</v>
       </c>
       <c r="G69" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W69" t="str">
         <f t="shared" si="89"/>
@@ -16111,7 +16117,7 @@
         <v>2400</v>
       </c>
       <c r="V70" s="4" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="W70">
         <f t="shared" si="89"/>
@@ -16317,7 +16323,7 @@
         <v>2400</v>
       </c>
       <c r="V71" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="W71" t="str">
         <f t="shared" si="89"/>
@@ -16806,7 +16812,7 @@
     </row>
     <row r="74" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C74" t="s">
         <v>426</v>
@@ -16815,7 +16821,7 @@
         <v>431</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="H74">
         <v>1600</v>
@@ -16860,7 +16866,7 @@
         <v>1800</v>
       </c>
       <c r="V74" s="4" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="W74">
         <f t="shared" si="89"/>
@@ -16947,7 +16953,7 @@
         <v>4pm-6pm</v>
       </c>
       <c r="AR74" s="12" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="AS74" t="s">
         <v>295</v>
@@ -17013,16 +17019,16 @@
     </row>
     <row r="75" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C75" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E75" t="s">
         <v>431</v>
       </c>
       <c r="G75" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="W75" t="str">
         <f t="shared" si="89"/>
@@ -17174,16 +17180,16 @@
     </row>
     <row r="76" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C76" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E76" t="s">
         <v>431</v>
       </c>
       <c r="G76" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="H76">
         <v>1500</v>
@@ -17228,7 +17234,7 @@
         <v>1800</v>
       </c>
       <c r="V76" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="W76">
         <f t="shared" si="89"/>
@@ -17315,7 +17321,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR76" s="6" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="AU76" t="s">
         <v>299</v>
@@ -17429,7 +17435,7 @@
         <v>1900</v>
       </c>
       <c r="V77" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="W77" t="str">
         <f t="shared" si="89"/>
@@ -17583,7 +17589,7 @@
     </row>
     <row r="78" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C78" t="s">
         <v>426</v>
@@ -17592,7 +17598,7 @@
         <v>431</v>
       </c>
       <c r="G78" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="W78" t="str">
         <f t="shared" si="89"/>
@@ -17679,7 +17685,7 @@
         <v/>
       </c>
       <c r="AR78" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="AU78" t="s">
         <v>298</v>
@@ -17787,7 +17793,7 @@
         <v>1800</v>
       </c>
       <c r="V79" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="W79">
         <f t="shared" si="89"/>
@@ -17948,7 +17954,7 @@
         <v>&lt;img src=@img/kidicon.png@&gt;</v>
       </c>
       <c r="BL79" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="80" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -18348,7 +18354,7 @@
         <v>2000</v>
       </c>
       <c r="V82" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="W82">
         <f t="shared" si="89"/>
@@ -18671,7 +18677,7 @@
     </row>
     <row r="84" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C84" t="s">
         <v>426</v>
@@ -18680,7 +18686,7 @@
         <v>431</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="J84">
         <v>1600</v>
@@ -18713,7 +18719,7 @@
         <v>1800</v>
       </c>
       <c r="V84" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="X84" t="str">
         <f t="shared" ref="X84" si="121">IF(I84&gt;0,I84/100,"")</f>
@@ -19090,7 +19096,7 @@
         <v>1900</v>
       </c>
       <c r="V86" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="W86">
         <f t="shared" si="89"/>
@@ -19250,7 +19256,7 @@
     </row>
     <row r="87" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C87" t="s">
         <v>428</v>
@@ -19259,7 +19265,7 @@
         <v>431</v>
       </c>
       <c r="G87" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="W87" t="str">
         <f t="shared" si="89"/>
@@ -19406,13 +19412,13 @@
     </row>
     <row r="88" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C88" t="s">
         <v>429</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H88">
         <v>1100</v>
@@ -19457,7 +19463,7 @@
         <v>1300</v>
       </c>
       <c r="V88" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="W88">
         <f t="shared" si="89"/>
@@ -19544,7 +19550,7 @@
         <v>11am-1pm</v>
       </c>
       <c r="AR88" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="AS88" t="s">
         <v>295</v>
@@ -19881,7 +19887,7 @@
         <v>1800</v>
       </c>
       <c r="V90" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="W90">
         <f t="shared" si="89"/>
@@ -20053,7 +20059,7 @@
         <v>117</v>
       </c>
       <c r="V91" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="W91" t="str">
         <f t="shared" si="89"/>
@@ -20210,7 +20216,7 @@
     </row>
     <row r="92" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C92" t="s">
         <v>309</v>
@@ -20219,7 +20225,7 @@
         <v>431</v>
       </c>
       <c r="G92" s="7" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="AK92" t="str">
         <f t="shared" si="111"/>
@@ -20250,7 +20256,7 @@
         <v/>
       </c>
       <c r="AR92" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="AS92" t="s">
         <v>295</v>
@@ -20482,7 +20488,7 @@
     </row>
     <row r="94" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C94" t="s">
         <v>429</v>
@@ -20491,7 +20497,7 @@
         <v>54</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="J94">
         <v>1100</v>
@@ -20524,7 +20530,7 @@
         <v>1400</v>
       </c>
       <c r="V94" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="W94" t="str">
         <f t="shared" ref="W94" si="165">IF(H94&gt;0,H94/100,"")</f>
@@ -20842,7 +20848,7 @@
     </row>
     <row r="96" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C96" t="s">
         <v>428</v>
@@ -20854,7 +20860,7 @@
         <v>431</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="H96">
         <v>1600</v>
@@ -20899,7 +20905,7 @@
         <v>1800</v>
       </c>
       <c r="V96" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="W96">
         <f t="shared" si="151"/>
@@ -20986,7 +20992,7 @@
         <v>4pm-6pm</v>
       </c>
       <c r="AR96" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="AS96" t="s">
         <v>295</v>
@@ -21056,13 +21062,13 @@
     </row>
     <row r="97" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C97" t="s">
         <v>428</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="H97">
         <v>1100</v>
@@ -21107,7 +21113,7 @@
         <v>1800</v>
       </c>
       <c r="V97" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="W97">
         <f t="shared" si="151"/>
@@ -21194,7 +21200,7 @@
         <v>11am-6pm</v>
       </c>
       <c r="AR97" s="12" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AU97" t="s">
         <v>28</v>
@@ -21302,7 +21308,7 @@
         <v>1900</v>
       </c>
       <c r="V98" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="W98" t="str">
         <f t="shared" si="151"/>
@@ -21513,7 +21519,7 @@
         <v>1800</v>
       </c>
       <c r="V99" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="W99">
         <f t="shared" si="151"/>
@@ -21670,13 +21676,13 @@
     </row>
     <row r="100" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C100" t="s">
         <v>426</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="W100" t="str">
         <f t="shared" si="151"/>
@@ -21763,7 +21769,7 @@
         <v/>
       </c>
       <c r="AR100" s="12" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AU100" t="s">
         <v>28</v>
@@ -21883,7 +21889,7 @@
         <v>1900</v>
       </c>
       <c r="V101" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="W101">
         <f t="shared" si="151"/>
@@ -22041,13 +22047,13 @@
     </row>
     <row r="102" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C102" t="s">
         <v>426</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="W102" t="str">
         <f t="shared" si="151"/>
@@ -22134,7 +22140,7 @@
         <v/>
       </c>
       <c r="AR102" s="12" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AU102" t="s">
         <v>298</v>
@@ -22197,13 +22203,13 @@
     </row>
     <row r="103" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C103" t="s">
         <v>429</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="W103" t="str">
         <f t="shared" si="151"/>
@@ -22395,7 +22401,7 @@
         <v>1800</v>
       </c>
       <c r="V104" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="W104" t="str">
         <f t="shared" si="151"/>
@@ -22552,7 +22558,7 @@
     </row>
     <row r="105" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C105" t="s">
         <v>308</v>
@@ -22561,7 +22567,7 @@
         <v>431</v>
       </c>
       <c r="G105" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="W105" t="str">
         <f t="shared" si="151"/>
@@ -22648,7 +22654,7 @@
         <v/>
       </c>
       <c r="AR105" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="AU105" t="s">
         <v>28</v>
@@ -22883,13 +22889,13 @@
     </row>
     <row r="107" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C107" t="s">
         <v>309</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="W107" t="str">
         <f t="shared" si="151"/>
@@ -22976,7 +22982,7 @@
         <v/>
       </c>
       <c r="AR107" s="10" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="AU107" t="s">
         <v>299</v>
@@ -23039,19 +23045,19 @@
     </row>
     <row r="108" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C108" t="s">
         <v>309</v>
       </c>
       <c r="D108" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E108" t="s">
         <v>54</v>
       </c>
       <c r="G108" s="7" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H108">
         <v>1400</v>
@@ -23096,7 +23102,7 @@
         <v>1700</v>
       </c>
       <c r="V108" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="W108">
         <f t="shared" si="151"/>
@@ -23183,7 +23189,7 @@
         <v>2pm-5pm</v>
       </c>
       <c r="AR108" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AU108" t="s">
         <v>299</v>
@@ -23753,7 +23759,7 @@
     </row>
     <row r="112" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C112" t="s">
         <v>429</v>
@@ -23762,7 +23768,7 @@
         <v>431</v>
       </c>
       <c r="G112" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="H112">
         <v>1600</v>
@@ -23807,7 +23813,7 @@
         <v>1900</v>
       </c>
       <c r="V112" s="4" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="W112">
         <f t="shared" si="151"/>
@@ -23894,7 +23900,7 @@
         <v>4pm-7pm</v>
       </c>
       <c r="AR112" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="AS112" t="s">
         <v>295</v>
@@ -24018,7 +24024,7 @@
         <v>1800</v>
       </c>
       <c r="V113" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="W113">
         <f t="shared" si="151"/>
@@ -24232,7 +24238,7 @@
         <v>1900</v>
       </c>
       <c r="V114" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="W114">
         <f t="shared" si="151"/>
@@ -24603,7 +24609,7 @@
         <v>1800</v>
       </c>
       <c r="V116" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="W116" t="str">
         <f t="shared" si="151"/>
@@ -24766,7 +24772,7 @@
     </row>
     <row r="117" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C117" t="s">
         <v>427</v>
@@ -24775,7 +24781,7 @@
         <v>431</v>
       </c>
       <c r="G117" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="W117" t="str">
         <f t="shared" si="151"/>
@@ -24862,7 +24868,7 @@
         <v/>
       </c>
       <c r="AR117" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="AU117" t="s">
         <v>299</v>
@@ -25091,7 +25097,7 @@
     </row>
     <row r="119" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C119" t="s">
         <v>309</v>
@@ -25100,7 +25106,7 @@
         <v>54</v>
       </c>
       <c r="G119" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="W119" t="str">
         <f t="shared" si="151"/>
@@ -25754,7 +25760,7 @@
     </row>
     <row r="123" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C123" t="s">
         <v>309</v>
@@ -25763,7 +25769,7 @@
         <v>431</v>
       </c>
       <c r="G123" s="7" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="W123" t="str">
         <f t="shared" ref="W123:W153" si="198">IF(H123&gt;0,H123/100,"")</f>
@@ -25842,7 +25848,7 @@
         <v/>
       </c>
       <c r="AR123" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="AU123" t="s">
         <v>299</v>
@@ -25905,13 +25911,13 @@
     </row>
     <row r="124" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C124" t="s">
         <v>428</v>
       </c>
       <c r="G124" s="7" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H124">
         <v>1500</v>
@@ -25956,7 +25962,7 @@
         <v>1800</v>
       </c>
       <c r="V124" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="W124">
         <f t="shared" si="198"/>
@@ -26043,7 +26049,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR124" s="12" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AS124" t="s">
         <v>295</v>
@@ -26109,13 +26115,13 @@
     </row>
     <row r="125" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C125" t="s">
         <v>308</v>
       </c>
       <c r="G125" s="7" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="H125">
         <v>1500</v>
@@ -26247,7 +26253,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR125" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AU125" t="s">
         <v>28</v>
@@ -26524,19 +26530,19 @@
     </row>
     <row r="127" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C127" t="s">
         <v>426</v>
       </c>
       <c r="D127" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E127" t="s">
         <v>431</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="J127">
         <v>1700</v>
@@ -26569,7 +26575,7 @@
         <v>2400</v>
       </c>
       <c r="V127" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="W127" t="str">
         <f t="shared" si="198"/>
@@ -26656,7 +26662,7 @@
         <v/>
       </c>
       <c r="AR127" s="10" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="AU127" t="s">
         <v>298</v>
@@ -26776,7 +26782,7 @@
         <v>1800</v>
       </c>
       <c r="V128" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="W128">
         <f t="shared" si="198"/>
@@ -26969,7 +26975,7 @@
         <v>2400</v>
       </c>
       <c r="V129" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="W129" t="str">
         <f t="shared" si="198"/>
@@ -27292,7 +27298,7 @@
     </row>
     <row r="131" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C131" t="s">
         <v>308</v>
@@ -27301,7 +27307,7 @@
         <v>54</v>
       </c>
       <c r="G131" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="W131" t="str">
         <f t="shared" si="198"/>
@@ -27388,7 +27394,7 @@
         <v/>
       </c>
       <c r="AR131" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="AU131" t="s">
         <v>28</v>
@@ -27451,7 +27457,7 @@
     </row>
     <row r="132" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C132" t="s">
         <v>308</v>
@@ -27460,7 +27466,7 @@
         <v>431</v>
       </c>
       <c r="G132" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="W132" t="str">
         <f t="shared" si="198"/>
@@ -27547,7 +27553,7 @@
         <v/>
       </c>
       <c r="AR132" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="AS132" t="s">
         <v>295</v>
@@ -27656,7 +27662,7 @@
         <v>1600</v>
       </c>
       <c r="V133" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="W133" t="str">
         <f t="shared" si="198"/>
@@ -27816,7 +27822,7 @@
     </row>
     <row r="134" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C134" t="s">
         <v>309</v>
@@ -27825,7 +27831,7 @@
         <v>431</v>
       </c>
       <c r="G134" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="H134">
         <v>1500</v>
@@ -27870,7 +27876,7 @@
         <v>1800</v>
       </c>
       <c r="V134" s="4" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="W134">
         <f t="shared" si="198"/>
@@ -27957,7 +27963,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR134" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="AU134" t="s">
         <v>299</v>
@@ -28020,7 +28026,7 @@
     </row>
     <row r="135" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C135" t="s">
         <v>308</v>
@@ -28029,7 +28035,7 @@
         <v>54</v>
       </c>
       <c r="G135" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="W135" t="str">
         <f t="shared" si="198"/>
@@ -28116,7 +28122,7 @@
         <v/>
       </c>
       <c r="AR135" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="AU135" t="s">
         <v>28</v>
@@ -28640,7 +28646,7 @@
         <v>2000</v>
       </c>
       <c r="V138" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="W138">
         <f t="shared" si="198"/>
@@ -29129,7 +29135,7 @@
     </row>
     <row r="141" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C141" t="s">
         <v>309</v>
@@ -29138,7 +29144,7 @@
         <v>54</v>
       </c>
       <c r="G141" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="W141" t="str">
         <f t="shared" si="198"/>
@@ -29617,7 +29623,7 @@
     </row>
     <row r="144" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C144" t="s">
         <v>309</v>
@@ -29626,7 +29632,7 @@
         <v>431</v>
       </c>
       <c r="G144" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H144">
         <v>1500</v>
@@ -29671,7 +29677,7 @@
         <v>1800</v>
       </c>
       <c r="V144" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="W144">
         <f t="shared" si="198"/>
@@ -29758,7 +29764,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR144" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="AU144" t="s">
         <v>299</v>
@@ -29821,7 +29827,7 @@
     </row>
     <row r="145" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C145" t="s">
         <v>309</v>
@@ -29830,7 +29836,7 @@
         <v>431</v>
       </c>
       <c r="G145" s="7" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="W145" t="str">
         <f t="shared" si="198"/>
@@ -29909,7 +29915,7 @@
         <v/>
       </c>
       <c r="AR145" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="AS145" t="s">
         <v>295</v>
@@ -30349,7 +30355,7 @@
     </row>
     <row r="148" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C148" t="s">
         <v>308</v>
@@ -30358,7 +30364,7 @@
         <v>431</v>
       </c>
       <c r="G148" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J148">
         <v>1500</v>
@@ -30391,7 +30397,7 @@
         <v>1800</v>
       </c>
       <c r="V148" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="W148" t="str">
         <f t="shared" si="198"/>
@@ -30589,7 +30595,7 @@
         <v>2000</v>
       </c>
       <c r="V149" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="W149">
         <f t="shared" si="198"/>
@@ -31011,7 +31017,7 @@
         <v>1900</v>
       </c>
       <c r="V151" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="W151">
         <f t="shared" si="198"/>
@@ -31503,13 +31509,13 @@
     </row>
     <row r="154" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C154" t="s">
         <v>426</v>
       </c>
       <c r="G154" s="7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="W154" t="str">
         <f t="shared" ref="W154:W185" si="232">IF(H154&gt;0,H154/100,"")</f>
@@ -31596,7 +31602,7 @@
         <v/>
       </c>
       <c r="AR154" s="12" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="AU154" t="s">
         <v>298</v>
@@ -32045,13 +32051,13 @@
     </row>
     <row r="157" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E157" t="s">
         <v>431</v>
       </c>
       <c r="G157" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W157" t="str">
         <f t="shared" si="232"/>
@@ -32364,7 +32370,7 @@
     </row>
     <row r="159" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C159" t="s">
         <v>426</v>
@@ -32373,7 +32379,7 @@
         <v>431</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="H159">
         <v>1500</v>
@@ -32418,7 +32424,7 @@
         <v>2400</v>
       </c>
       <c r="V159" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="W159">
         <f t="shared" si="232"/>
@@ -32569,7 +32575,7 @@
     </row>
     <row r="160" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C160" t="s">
         <v>427</v>
@@ -32578,7 +32584,7 @@
         <v>54</v>
       </c>
       <c r="G160" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="J160">
         <v>1400</v>
@@ -32611,7 +32617,7 @@
         <v>1900</v>
       </c>
       <c r="V160" s="4" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="W160" t="str">
         <f t="shared" si="232"/>
@@ -32957,7 +32963,7 @@
     </row>
     <row r="162" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C162" t="s">
         <v>426</v>
@@ -32969,7 +32975,7 @@
         <v>431</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H162">
         <v>1130</v>
@@ -33002,7 +33008,7 @@
         <v>1800</v>
       </c>
       <c r="V162" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="W162">
         <f t="shared" si="232"/>
@@ -33089,7 +33095,7 @@
         <v/>
       </c>
       <c r="AR162" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="AS162" t="s">
         <v>295</v>
@@ -33332,7 +33338,7 @@
     </row>
     <row r="164" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C164" t="s">
         <v>427</v>
@@ -33341,7 +33347,7 @@
         <v>431</v>
       </c>
       <c r="G164" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="N164">
         <v>1200</v>
@@ -33350,7 +33356,7 @@
         <v>1700</v>
       </c>
       <c r="V164" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="W164" t="str">
         <f t="shared" si="232"/>
@@ -33437,7 +33443,7 @@
         <v/>
       </c>
       <c r="AS164" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="AU164" t="s">
         <v>299</v>
@@ -33832,13 +33838,13 @@
     </row>
     <row r="167" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C167" t="s">
         <v>429</v>
       </c>
       <c r="G167" s="7" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="W167" t="str">
         <f t="shared" si="232"/>
@@ -34199,7 +34205,7 @@
         <v>1800</v>
       </c>
       <c r="V169" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="W169" t="str">
         <f t="shared" si="232"/>
@@ -34353,13 +34359,13 @@
     </row>
     <row r="170" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C170" t="s">
         <v>309</v>
       </c>
       <c r="G170" s="7" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="L170">
         <v>1600</v>
@@ -34470,7 +34476,7 @@
         <v/>
       </c>
       <c r="AR170" s="12" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AU170" t="s">
         <v>299</v>
@@ -34578,7 +34584,7 @@
         <v>1800</v>
       </c>
       <c r="V171" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="W171" t="str">
         <f t="shared" si="232"/>
@@ -34732,19 +34738,19 @@
     </row>
     <row r="172" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C172" t="s">
         <v>426</v>
       </c>
       <c r="D172" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E172" t="s">
         <v>431</v>
       </c>
       <c r="G172" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="W172" t="str">
         <f t="shared" si="232"/>
@@ -34831,7 +34837,7 @@
         <v/>
       </c>
       <c r="AR172" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="AS172" t="s">
         <v>295</v>
@@ -34897,7 +34903,7 @@
     </row>
     <row r="173" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C173" t="s">
         <v>426</v>
@@ -34906,7 +34912,7 @@
         <v>431</v>
       </c>
       <c r="G173" s="7" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="W173" t="str">
         <f t="shared" si="232"/>
@@ -34985,7 +34991,7 @@
         <v/>
       </c>
       <c r="AR173" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="AU173" t="s">
         <v>298</v>
@@ -35048,19 +35054,19 @@
     </row>
     <row r="174" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C174" t="s">
         <v>426</v>
       </c>
       <c r="D174" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E174" t="s">
         <v>35</v>
       </c>
       <c r="G174" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="J174">
         <v>1100</v>
@@ -35099,7 +35105,7 @@
         <v>1700</v>
       </c>
       <c r="V174" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="W174" t="str">
         <f t="shared" si="232"/>
@@ -35186,7 +35192,7 @@
         <v>11am-5pm</v>
       </c>
       <c r="AR174" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AU174" t="s">
         <v>298</v>
@@ -35249,13 +35255,13 @@
     </row>
     <row r="175" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C175" t="s">
         <v>426</v>
       </c>
       <c r="G175" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="W175" t="str">
         <f t="shared" si="232"/>
@@ -35342,7 +35348,7 @@
         <v/>
       </c>
       <c r="AR175" s="12" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="AU175" t="s">
         <v>298</v>
@@ -35405,19 +35411,19 @@
     </row>
     <row r="176" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C176" t="s">
         <v>426</v>
       </c>
       <c r="D176" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E176" t="s">
         <v>35</v>
       </c>
       <c r="G176" s="7" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="W176" t="str">
         <f t="shared" si="232"/>
@@ -35504,7 +35510,7 @@
         <v/>
       </c>
       <c r="AR176" s="12" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="AU176" t="s">
         <v>298</v>
@@ -35567,13 +35573,13 @@
     </row>
     <row r="177" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C177" t="s">
         <v>426</v>
       </c>
       <c r="G177" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="W177" t="str">
         <f t="shared" si="232"/>
@@ -35660,7 +35666,7 @@
         <v/>
       </c>
       <c r="AR177" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="AS177" t="s">
         <v>295</v>
@@ -35949,7 +35955,7 @@
         <v>1900</v>
       </c>
       <c r="V179" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="W179">
         <f t="shared" si="232"/>
@@ -36151,7 +36157,7 @@
         <v>1900</v>
       </c>
       <c r="V180" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="W180" t="str">
         <f t="shared" si="232"/>
@@ -36474,7 +36480,7 @@
     </row>
     <row r="182" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C182" t="s">
         <v>426</v>
@@ -36486,7 +36492,7 @@
         <v>54</v>
       </c>
       <c r="G182" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J182">
         <v>1500</v>
@@ -36670,13 +36676,13 @@
     </row>
     <row r="183" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C183" t="s">
         <v>308</v>
       </c>
       <c r="G183" s="7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="W183" t="str">
         <f t="shared" si="232"/>
@@ -36880,7 +36886,7 @@
         <v>1900</v>
       </c>
       <c r="V184" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="W184">
         <f t="shared" si="232"/>
@@ -37203,7 +37209,7 @@
     </row>
     <row r="186" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C186" t="s">
         <v>426</v>
@@ -37212,7 +37218,7 @@
         <v>431</v>
       </c>
       <c r="G186" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="W186" t="str">
         <f t="shared" ref="W186:W196" si="256">IF(H186&gt;0,H186/100,"")</f>
@@ -37291,7 +37297,7 @@
         <v/>
       </c>
       <c r="AR186" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="AU186" t="s">
         <v>299</v>
@@ -37354,7 +37360,7 @@
     </row>
     <row r="187" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C187" t="s">
         <v>426</v>
@@ -37363,7 +37369,7 @@
         <v>54</v>
       </c>
       <c r="G187" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="W187" t="str">
         <f t="shared" si="256"/>
@@ -37442,7 +37448,7 @@
         <v/>
       </c>
       <c r="AR187" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="AS187" t="s">
         <v>295</v>
@@ -37508,13 +37514,13 @@
     </row>
     <row r="188" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C188" t="s">
         <v>429</v>
       </c>
       <c r="G188" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="W188" t="str">
         <f t="shared" si="256"/>
@@ -37601,7 +37607,7 @@
         <v/>
       </c>
       <c r="AR188" s="12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="AU188" t="s">
         <v>28</v>
@@ -37664,13 +37670,13 @@
     </row>
     <row r="189" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E189" t="s">
         <v>431</v>
       </c>
       <c r="G189" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="W189" t="str">
         <f t="shared" si="256"/>
@@ -37989,7 +37995,7 @@
     </row>
     <row r="191" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C191" t="s">
         <v>309</v>
@@ -38001,7 +38007,7 @@
         <v>431</v>
       </c>
       <c r="G191" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="W191" t="str">
         <f t="shared" si="256"/>
@@ -38088,7 +38094,7 @@
         <v/>
       </c>
       <c r="AR191" s="12" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="AS191" t="s">
         <v>295</v>
@@ -38154,13 +38160,13 @@
     </row>
     <row r="192" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C192" t="s">
         <v>309</v>
       </c>
       <c r="G192" s="7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J192">
         <v>1100</v>
@@ -38181,7 +38187,7 @@
         <v>2400</v>
       </c>
       <c r="V192" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="W192" t="str">
         <f t="shared" si="256"/>
@@ -38260,7 +38266,7 @@
         <v/>
       </c>
       <c r="AR192" s="12" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AU192" t="s">
         <v>299</v>
@@ -38639,13 +38645,13 @@
     </row>
     <row r="195" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C195" t="s">
         <v>429</v>
       </c>
       <c r="G195" s="7" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="W195" t="str">
         <f t="shared" si="256"/>
@@ -38724,7 +38730,7 @@
         <v/>
       </c>
       <c r="AR195" s="12" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AS195" t="s">
         <v>295</v>
@@ -38821,7 +38827,7 @@
         <v>1600</v>
       </c>
       <c r="V196" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="W196" t="str">
         <f t="shared" si="256"/>
@@ -39064,13 +39070,13 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>766</v>
+      </c>
+      <c r="C1" t="s">
+        <v>767</v>
+      </c>
+      <c r="D1" t="s">
         <v>768</v>
-      </c>
-      <c r="C1" t="s">
-        <v>769</v>
-      </c>
-      <c r="D1" t="s">
-        <v>770</v>
       </c>
       <c r="E1">
         <v>40.589424999999999</v>
@@ -39081,13 +39087,13 @@
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C2" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D2" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E2">
         <v>40.589759999999998</v>
@@ -39098,13 +39104,13 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C3" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D3" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="E3">
         <v>40.523972999999998</v>
@@ -39115,13 +39121,13 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C4" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D4" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="E4">
         <v>40.551048999999999</v>
@@ -39132,13 +39138,13 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C5" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D5" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="E5">
         <v>40.563256000000003</v>
@@ -39149,13 +39155,13 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C6" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D6" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="E6">
         <v>40.527959000000003</v>
@@ -39166,13 +39172,13 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C7" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D7" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E7">
         <v>40.586450999999997</v>

</xml_diff>

<commit_message>
Updated nicks, fixed taste and savor
</commit_message>
<xml_diff>
--- a/database_working.xlsx
+++ b/database_working.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Dropbox\CLD\Orange House\Happy Hour\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clorange\Dropbox\CLD\Orange House\Happy Hour\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52045C10-69CE-40FE-975A-D5570A130D33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$2:$C$192</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2398,9 +2397,6 @@
     <t>out</t>
   </si>
   <si>
-    <t>Draft beers $3.50 &lt;br&gt; Budwiser $2.00 &lt;br&gt; House Wine $4.25 &lt;br&gt;$2.50-$3.00 Pizza by the slice&lt;br&gt;$5.00 Fried Mozzarella&lt;br&gt;$4.00 Parmesan Fries&lt;br&gt;$5.00 Fried Calamari&lt;br&gt;$5.00 Chicken Wings</t>
-  </si>
-  <si>
     <t>Half off beverages in a can.</t>
   </si>
   <si>
@@ -2447,12 +2443,15 @@
   </si>
   <si>
     <t>Special pricing on a sparkling, white, rose and red by the glass. Discount prices on cheese board and cheese bread.</t>
+  </si>
+  <si>
+    <t>Draft beers $3.50 &lt;br&gt; Budwiser $2.00 &lt;br&gt; House Wine $4.25 &lt;br&gt;$2.50-$3.00 Pizza by the slice&lt;br&gt;$5.00 Fried Mozzarella&lt;br&gt;$4.00 Parmesan Fries&lt;br&gt;$5.00 Fried Calamari&lt;br&gt;$5.00 Chicken Wings&lt;br&gt;&lt;b&gt;Wine Mondays!&lt;/b&gt;Half off all bottles of wine from 5 to 9pm on Mondays</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3041,12 +3040,12 @@
     <cellStyle name="40% - Accent4" xfId="28" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent5" xfId="31" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent6" xfId="34" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="37" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2" xfId="38" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3" xfId="39" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4" xfId="40" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5" xfId="41" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6" xfId="42" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="60% - Accent1" xfId="37"/>
+    <cellStyle name="60% - Accent2" xfId="38"/>
+    <cellStyle name="60% - Accent3" xfId="39"/>
+    <cellStyle name="60% - Accent4" xfId="40"/>
+    <cellStyle name="60% - Accent5" xfId="41"/>
+    <cellStyle name="60% - Accent6" xfId="42"/>
     <cellStyle name="Accent1" xfId="17" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="23" builtinId="37" customBuiltin="1"/>
@@ -3065,11 +3064,11 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Input" xfId="8" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="11" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Neutral" xfId="36"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="14" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="9" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="35" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Title" xfId="35"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="13" builtinId="11" customBuiltin="1"/>
   </cellStyles>
@@ -3098,7 +3097,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -3410,33 +3409,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BL197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="BA151" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="U86" sqref="U86"/>
-      <selection pane="bottomRight" activeCell="BH163" sqref="BH163"/>
+      <selection pane="bottomRight" activeCell="V117" sqref="V117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="36" width="6" customWidth="1"/>
-    <col min="37" max="37" width="10.81640625" customWidth="1"/>
-    <col min="38" max="38" width="13.54296875" customWidth="1"/>
+    <col min="37" max="37" width="10.85546875" customWidth="1"/>
+    <col min="38" max="38" width="13.5703125" customWidth="1"/>
     <col min="39" max="39" width="13" customWidth="1"/>
-    <col min="40" max="42" width="10.26953125" customWidth="1"/>
-    <col min="43" max="43" width="15.81640625" customWidth="1"/>
-    <col min="50" max="50" width="90.54296875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.1796875" customWidth="1"/>
-    <col min="57" max="57" width="53.54296875" customWidth="1"/>
-    <col min="58" max="58" width="19.453125" customWidth="1"/>
+    <col min="40" max="42" width="10.28515625" customWidth="1"/>
+    <col min="43" max="43" width="15.85546875" customWidth="1"/>
+    <col min="50" max="50" width="90.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.140625" customWidth="1"/>
+    <col min="57" max="57" width="53.5703125" customWidth="1"/>
+    <col min="58" max="58" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3604,7 +3603,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="2" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>454</v>
       </c>
@@ -3819,7 +3818,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="3" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>140</v>
       </c>
@@ -4027,7 +4026,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>669</v>
       </c>
@@ -4186,7 +4185,7 @@
         <v>[40.58526,-105.07653],</v>
       </c>
     </row>
-    <row r="5" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>146</v>
       </c>
@@ -4352,7 +4351,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>508</v>
       </c>
@@ -4516,7 +4515,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>149</v>
       </c>
@@ -4688,7 +4687,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>65</v>
       </c>
@@ -4902,7 +4901,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>512</v>
       </c>
@@ -5116,7 +5115,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>109</v>
       </c>
@@ -5330,7 +5329,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>567</v>
       </c>
@@ -5492,7 +5491,7 @@
         <v>[40.57561,-105.07659],</v>
       </c>
     </row>
-    <row r="12" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>515</v>
       </c>
@@ -5656,7 +5655,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>517</v>
       </c>
@@ -5817,7 +5816,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>718</v>
       </c>
@@ -6024,7 +6023,7 @@
         <v>[40.543718,-105.074853],</v>
       </c>
     </row>
-    <row r="15" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>134</v>
       </c>
@@ -6191,7 +6190,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -6238,7 +6237,7 @@
         <v>1900</v>
       </c>
       <c r="V16" s="16" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="0"/>
@@ -6393,7 +6392,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>578</v>
       </c>
@@ -6555,7 +6554,7 @@
         <v>[40.56626,-105.07835],</v>
       </c>
     </row>
-    <row r="18" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>56</v>
       </c>
@@ -6775,7 +6774,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="19" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>246</v>
       </c>
@@ -6986,7 +6985,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>52</v>
       </c>
@@ -7152,7 +7151,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>301</v>
       </c>
@@ -7351,7 +7350,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>151</v>
       </c>
@@ -7571,7 +7570,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="23" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>266</v>
       </c>
@@ -7782,7 +7781,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="24" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>178</v>
       </c>
@@ -7984,7 +7983,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>657</v>
       </c>
@@ -8164,7 +8163,7 @@
         <v>[40.58814,-105.07477],</v>
       </c>
     </row>
-    <row r="26" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>267</v>
       </c>
@@ -8348,7 +8347,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>519</v>
       </c>
@@ -8511,7 +8510,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>180</v>
       </c>
@@ -8683,7 +8682,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="29" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>646</v>
       </c>
@@ -8839,7 +8838,7 @@
         <v>[40.562466,-105.037963],</v>
       </c>
     </row>
-    <row r="30" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>522</v>
       </c>
@@ -9000,7 +8999,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>524</v>
       </c>
@@ -9161,7 +9160,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>581</v>
       </c>
@@ -9317,7 +9316,7 @@
         <v>[40.57515,-105.09912],</v>
       </c>
     </row>
-    <row r="33" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>584</v>
       </c>
@@ -9483,7 +9482,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="34" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>366</v>
       </c>
@@ -9689,7 +9688,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>587</v>
       </c>
@@ -9845,7 +9844,7 @@
         <v>[40.57951,-105.07766],</v>
       </c>
     </row>
-    <row r="36" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>387</v>
       </c>
@@ -10059,7 +10058,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>275</v>
       </c>
@@ -10276,7 +10275,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="38" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>274</v>
       </c>
@@ -10478,7 +10477,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>590</v>
       </c>
@@ -10634,7 +10633,7 @@
         <v>[40.58152,-105.04595],</v>
       </c>
     </row>
-    <row r="40" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>126</v>
       </c>
@@ -10803,7 +10802,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>728</v>
       </c>
@@ -11011,7 +11010,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>30</v>
       </c>
@@ -11189,7 +11188,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>153</v>
       </c>
@@ -11248,7 +11247,7 @@
         <v>1700</v>
       </c>
       <c r="V43" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="W43">
         <f t="shared" si="34"/>
@@ -11400,7 +11399,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>26</v>
       </c>
@@ -11605,7 +11604,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>156</v>
       </c>
@@ -11640,7 +11639,7 @@
         <v>2100</v>
       </c>
       <c r="V45" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="W45">
         <f t="shared" si="34"/>
@@ -11795,7 +11794,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>77</v>
       </c>
@@ -12009,9 +12008,9 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C47" t="s">
         <v>426</v>
@@ -12020,7 +12019,7 @@
         <v>431</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="W47" t="str">
         <f t="shared" ref="W47" si="59">IF(H47&gt;0,H47/100,"")</f>
@@ -12111,7 +12110,7 @@
         <v>295</v>
       </c>
       <c r="AT47" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="AU47" t="s">
         <v>298</v>
@@ -12176,7 +12175,7 @@
         <v>[40.589825,-105.076497],</v>
       </c>
     </row>
-    <row r="48" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>444</v>
       </c>
@@ -12378,7 +12377,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="49" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>445</v>
       </c>
@@ -12544,7 +12543,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="50" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>539</v>
       </c>
@@ -12743,7 +12742,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>659</v>
       </c>
@@ -12902,7 +12901,7 @@
         <v>[40.58875,-105.07418],</v>
       </c>
     </row>
-    <row r="52" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>656</v>
       </c>
@@ -13064,7 +13063,7 @@
         <v>[40.58587,-105.07762],</v>
       </c>
     </row>
-    <row r="53" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>654</v>
       </c>
@@ -13256,7 +13255,7 @@
         <v>[40.5666,-105.05774],</v>
       </c>
     </row>
-    <row r="54" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>86</v>
       </c>
@@ -13422,7 +13421,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>68</v>
       </c>
@@ -13588,7 +13587,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>647</v>
       </c>
@@ -13780,7 +13779,7 @@
         <v>[40.60892,-105.0743],</v>
       </c>
     </row>
-    <row r="57" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>159</v>
       </c>
@@ -13964,7 +13963,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>269</v>
       </c>
@@ -14163,7 +14162,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B59" s="5" t="s">
         <v>367</v>
       </c>
@@ -14374,7 +14373,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>668</v>
       </c>
@@ -14533,7 +14532,7 @@
         <v>[40.58602,-105.07859],</v>
       </c>
     </row>
-    <row r="61" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>446</v>
       </c>
@@ -14699,7 +14698,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="62" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>257</v>
       </c>
@@ -14865,7 +14864,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>98</v>
       </c>
@@ -15076,7 +15075,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>73</v>
       </c>
@@ -15242,7 +15241,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>746</v>
       </c>
@@ -15396,7 +15395,7 @@
         <v>[40.58976,-105.076497],</v>
       </c>
     </row>
-    <row r="66" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>270</v>
       </c>
@@ -15610,7 +15609,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>278</v>
       </c>
@@ -15813,7 +15812,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>748</v>
       </c>
@@ -15964,7 +15963,7 @@
         <v>[40.551049,-105.05831],</v>
       </c>
     </row>
-    <row r="69" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>529</v>
       </c>
@@ -16122,7 +16121,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>187</v>
       </c>
@@ -16328,7 +16327,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>189</v>
       </c>
@@ -16533,7 +16532,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>447</v>
       </c>
@@ -16699,7 +16698,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="73" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>191</v>
       </c>
@@ -16868,7 +16867,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>593</v>
       </c>
@@ -17075,7 +17074,7 @@
         <v>[40.59003,-105.07363],</v>
       </c>
     </row>
-    <row r="75" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>531</v>
       </c>
@@ -17236,7 +17235,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>733</v>
       </c>
@@ -17440,7 +17439,7 @@
         <v>[40.47964,-104.90192],</v>
       </c>
     </row>
-    <row r="77" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>280</v>
       </c>
@@ -17645,7 +17644,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>666</v>
       </c>
@@ -17804,7 +17803,7 @@
         <v>[40.58839,-105.0776],</v>
       </c>
     </row>
-    <row r="79" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>379</v>
       </c>
@@ -18015,7 +18014,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="80" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>193</v>
       </c>
@@ -18187,7 +18186,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>46</v>
       </c>
@@ -18353,7 +18352,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>162</v>
       </c>
@@ -18567,7 +18566,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>448</v>
       </c>
@@ -18733,9 +18732,9 @@
         <v>465</v>
       </c>
     </row>
-    <row r="84" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C84" t="s">
         <v>426</v>
@@ -18744,7 +18743,7 @@
         <v>431</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="J84">
         <v>1600</v>
@@ -18777,7 +18776,7 @@
         <v>1800</v>
       </c>
       <c r="V84" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="X84" t="str">
         <f t="shared" ref="X84" si="121">IF(I84&gt;0,I84/100,"")</f>
@@ -18929,7 +18928,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>195</v>
       </c>
@@ -19095,7 +19094,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>24</v>
       </c>
@@ -19312,7 +19311,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="87" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>667</v>
       </c>
@@ -19468,7 +19467,7 @@
         <v>[40.5315,-105.11594],</v>
       </c>
     </row>
-    <row r="88" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>596</v>
       </c>
@@ -19672,7 +19671,7 @@
         <v>[40.57428,-105.09835],</v>
       </c>
     </row>
-    <row r="89" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>92</v>
       </c>
@@ -19886,7 +19885,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>33</v>
       </c>
@@ -20100,7 +20099,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>115</v>
       </c>
@@ -20272,7 +20271,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>715</v>
       </c>
@@ -20378,7 +20377,7 @@
         <v>[40.562046,-105.038001],</v>
       </c>
     </row>
-    <row r="93" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>131</v>
       </c>
@@ -20544,7 +20543,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>781</v>
       </c>
@@ -20738,7 +20737,7 @@
         <v>[40.5738693,-105.1169419],</v>
       </c>
     </row>
-    <row r="95" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>95</v>
       </c>
@@ -20904,7 +20903,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>545</v>
       </c>
@@ -21118,7 +21117,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>600</v>
       </c>
@@ -21171,7 +21170,7 @@
         <v>1800</v>
       </c>
       <c r="V97" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="W97">
         <f t="shared" si="151"/>
@@ -21319,7 +21318,7 @@
         <v>[40.52366,-105.03402],</v>
       </c>
     </row>
-    <row r="98" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>376</v>
       </c>
@@ -21518,7 +21517,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>197</v>
       </c>
@@ -21732,7 +21731,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>603</v>
       </c>
@@ -21888,7 +21887,7 @@
         <v>[40.5831,-105.08285],</v>
       </c>
     </row>
-    <row r="101" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>282</v>
       </c>
@@ -22103,7 +22102,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>606</v>
       </c>
@@ -22259,7 +22258,7 @@
         <v>[40.58653,-105.07751],</v>
       </c>
     </row>
-    <row r="103" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>609</v>
       </c>
@@ -22412,7 +22411,7 @@
         <v>[40.58231,-105.10714],</v>
       </c>
     </row>
-    <row r="104" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>371</v>
       </c>
@@ -22459,7 +22458,7 @@
         <v>1800</v>
       </c>
       <c r="V104" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="W104" t="str">
         <f t="shared" si="151"/>
@@ -22614,7 +22613,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>663</v>
       </c>
@@ -22773,7 +22772,7 @@
         <v>[40.57914,-105.07946],</v>
       </c>
     </row>
-    <row r="106" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>164</v>
       </c>
@@ -22945,7 +22944,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>611</v>
       </c>
@@ -23101,7 +23100,7 @@
         <v>[40.55511,-105.07836],</v>
       </c>
     </row>
-    <row r="108" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>558</v>
       </c>
@@ -23308,7 +23307,7 @@
         <v>[40.57291,-105.1154],</v>
       </c>
     </row>
-    <row r="109" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>62</v>
       </c>
@@ -23474,7 +23473,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>198</v>
       </c>
@@ -23640,7 +23639,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>394</v>
       </c>
@@ -23815,7 +23814,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="112" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>655</v>
       </c>
@@ -24023,7 +24022,7 @@
         <v>[40.57532,-105.10038],</v>
       </c>
     </row>
-    <row r="113" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>121</v>
       </c>
@@ -24237,7 +24236,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>166</v>
       </c>
@@ -24448,7 +24447,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>200</v>
       </c>
@@ -24620,7 +24619,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>168</v>
       </c>
@@ -24640,7 +24639,7 @@
         <v>1530</v>
       </c>
       <c r="K116">
-        <v>1800</v>
+        <v>2100</v>
       </c>
       <c r="L116">
         <v>1530</v>
@@ -24667,7 +24666,7 @@
         <v>1800</v>
       </c>
       <c r="V116" t="s">
-        <v>787</v>
+        <v>803</v>
       </c>
       <c r="W116" t="str">
         <f t="shared" si="151"/>
@@ -24683,7 +24682,7 @@
       </c>
       <c r="Z116">
         <f t="shared" si="154"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="AA116">
         <f t="shared" si="155"/>
@@ -24731,7 +24730,7 @@
       </c>
       <c r="AL116" t="str">
         <f t="shared" si="112"/>
-        <v>3.3pm-6pm</v>
+        <v>3.3pm-9pm</v>
       </c>
       <c r="AM116" t="str">
         <f t="shared" si="113"/>
@@ -24773,7 +24772,7 @@
         <v>{
     'name': "Nick's Italian",
     'area': "campus",'hours': {
-      'sunday-start':"", 'sunday-end':"", 'monday-start':"1530", 'monday-end':"1800", 'tuesday-start':"1530", 'tuesday-end':"1800", 'wednesday-start':"1530", 'wednesday-end':"1800", 'thursday-start':"1530", 'thursday-end':"1800", 'friday-start':"1530", 'friday-end':"1800", 'saturday-start':"", 'saturday-end':""},  'description': "Draft beers $3.50 &lt;br&gt; Budwiser $2.00 &lt;br&gt; House Wine $4.25 &lt;br&gt;$2.50-$3.00 Pizza by the slice&lt;br&gt;$5.00 Fried Mozzarella&lt;br&gt;$4.00 Parmesan Fries&lt;br&gt;$5.00 Fried Calamari&lt;br&gt;$5.00 Chicken Wings", 'link':"http://www.nicksfc.com/", 'pricing':"med",   'phone-number': "", 'address': "1100 S. College Avenue, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','easy'], 'has-drink':true, 'has-food':true},</v>
+      'sunday-start':"", 'sunday-end':"", 'monday-start':"1530", 'monday-end':"2100", 'tuesday-start':"1530", 'tuesday-end':"1800", 'wednesday-start':"1530", 'wednesday-end':"1800", 'thursday-start':"1530", 'thursday-end':"1800", 'friday-start':"1530", 'friday-end':"1800", 'saturday-start':"", 'saturday-end':""},  'description': "Draft beers $3.50 &lt;br&gt; Budwiser $2.00 &lt;br&gt; House Wine $4.25 &lt;br&gt;$2.50-$3.00 Pizza by the slice&lt;br&gt;$5.00 Fried Mozzarella&lt;br&gt;$4.00 Parmesan Fries&lt;br&gt;$5.00 Fried Calamari&lt;br&gt;$5.00 Chicken Wings&lt;br&gt;&lt;b&gt;Wine Mondays!&lt;/b&gt;Half off all bottles of wine from 5 to 9pm on Mondays", 'link':"http://www.nicksfc.com/", 'pricing':"med",   'phone-number': "", 'address': "1100 S. College Avenue, Fort Collins, CO 80524", 'other-amenities': ['outdoor','','easy'], 'has-drink':true, 'has-food':true},</v>
       </c>
       <c r="AY116" t="str">
         <f t="shared" si="189"/>
@@ -24828,7 +24827,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="117" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>653</v>
       </c>
@@ -24987,7 +24986,7 @@
         <v>[40.58358,-105.04801],</v>
       </c>
     </row>
-    <row r="118" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>123</v>
       </c>
@@ -25153,7 +25152,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>651</v>
       </c>
@@ -25312,7 +25311,7 @@
         <v>[40.55065,-105.04275],</v>
       </c>
     </row>
-    <row r="120" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>202</v>
       </c>
@@ -25484,7 +25483,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>143</v>
       </c>
@@ -25650,7 +25649,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>449</v>
       </c>
@@ -25816,7 +25815,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="123" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>750</v>
       </c>
@@ -25967,7 +25966,7 @@
         <v>[40.527959,-105.077616],</v>
       </c>
     </row>
-    <row r="124" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>614</v>
       </c>
@@ -26171,7 +26170,7 @@
         <v>[40.52143,-105.05755],</v>
       </c>
     </row>
-    <row r="125" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>618</v>
       </c>
@@ -26372,7 +26371,7 @@
         <v>[40.56741,-105.08268],</v>
       </c>
     </row>
-    <row r="126" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>89</v>
       </c>
@@ -26586,7 +26585,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>573</v>
       </c>
@@ -26781,7 +26780,7 @@
         <v>[40.58998,-105.0731],</v>
       </c>
     </row>
-    <row r="128" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>204</v>
       </c>
@@ -26992,7 +26991,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>206</v>
       </c>
@@ -27188,7 +27187,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>450</v>
       </c>
@@ -27354,7 +27353,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="131" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>652</v>
       </c>
@@ -27513,7 +27512,7 @@
         <v>[40.57789,-105.0766],</v>
       </c>
     </row>
-    <row r="132" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>648</v>
       </c>
@@ -27645,15 +27644,15 @@
         <v/>
       </c>
       <c r="BA132" t="str">
-        <f t="shared" ref="BA132:BA163" si="215">IF(AU132="hard","&lt;img src=@img/hard.png@&gt;",IF(AU132="medium","&lt;img src=@img/medium.png@&gt;",IF(AU132="easy","&lt;img src=@img/easy.png@&gt;","")))</f>
+        <f t="shared" ref="BA132:BA162" si="215">IF(AU132="hard","&lt;img src=@img/hard.png@&gt;",IF(AU132="medium","&lt;img src=@img/medium.png@&gt;",IF(AU132="easy","&lt;img src=@img/easy.png@&gt;","")))</f>
         <v>&lt;img src=@img/medium.png@&gt;</v>
       </c>
       <c r="BB132" t="str">
-        <f t="shared" ref="BB132:BB163" si="216">IF(AV132="true","&lt;img src=@img/drinkicon.png@&gt;","")</f>
+        <f t="shared" ref="BB132:BB162" si="216">IF(AV132="true","&lt;img src=@img/drinkicon.png@&gt;","")</f>
         <v/>
       </c>
       <c r="BC132" t="str">
-        <f t="shared" ref="BC132:BC163" si="217">IF(AW132="true","&lt;img src=@img/foodicon.png@&gt;","")</f>
+        <f t="shared" ref="BC132:BC162" si="217">IF(AW132="true","&lt;img src=@img/foodicon.png@&gt;","")</f>
         <v/>
       </c>
       <c r="BD132" t="str">
@@ -27665,7 +27664,7 @@
         <v>outdoor medium med campus</v>
       </c>
       <c r="BF132" t="str">
-        <f t="shared" ref="BF132:BF163" si="220">IF(C132="old","Old Town",IF(C132="campus","Near Campus",IF(C132="sfoco","South Foco",IF(C132="nfoco","North Foco",IF(C132="midtown","Midtown",IF(C132="cwest","Campus West",IF(C132="efoco","East FoCo",IF(C132="windsor","Windsor",""))))))))</f>
+        <f t="shared" ref="BF132:BF162" si="220">IF(C132="old","Old Town",IF(C132="campus","Near Campus",IF(C132="sfoco","South Foco",IF(C132="nfoco","North Foco",IF(C132="midtown","Midtown",IF(C132="cwest","Campus West",IF(C132="efoco","East FoCo",IF(C132="windsor","Windsor",""))))))))</f>
         <v>Near Campus</v>
       </c>
       <c r="BG132">
@@ -27679,7 +27678,7 @@
         <v>[40.57855,-105.07975],</v>
       </c>
     </row>
-    <row r="133" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>208</v>
       </c>
@@ -27720,7 +27719,7 @@
         <v>1600</v>
       </c>
       <c r="V133" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="W133" t="str">
         <f t="shared" si="198"/>
@@ -27878,7 +27877,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>740</v>
       </c>
@@ -28082,7 +28081,7 @@
         <v>[40.52369,-105.03435],</v>
       </c>
     </row>
-    <row r="135" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>660</v>
       </c>
@@ -28241,7 +28240,7 @@
         <v>[40.573785,-105.0833606],</v>
       </c>
     </row>
-    <row r="136" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>170</v>
       </c>
@@ -28446,7 +28445,7 @@
         <v/>
       </c>
     </row>
-    <row r="137" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>43</v>
       </c>
@@ -28645,7 +28644,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>210</v>
       </c>
@@ -28859,7 +28858,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>59</v>
       </c>
@@ -29025,7 +29024,7 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>451</v>
       </c>
@@ -29191,7 +29190,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="141" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>661</v>
       </c>
@@ -29347,7 +29346,7 @@
         <v>[40.55258,-105.09673],</v>
       </c>
     </row>
-    <row r="142" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>213</v>
       </c>
@@ -29513,7 +29512,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>478</v>
       </c>
@@ -29679,7 +29678,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="144" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>649</v>
       </c>
@@ -29883,7 +29882,7 @@
         <v>[40.55475,-105.09774],</v>
       </c>
     </row>
-    <row r="145" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>749</v>
       </c>
@@ -30037,7 +30036,7 @@
         <v>[40.563256,-105.077464],</v>
       </c>
     </row>
-    <row r="146" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>397</v>
       </c>
@@ -30203,7 +30202,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>378</v>
       </c>
@@ -30411,7 +30410,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>650</v>
       </c>
@@ -30600,7 +30599,7 @@
         <v>[40.5635177,-105.077318],</v>
       </c>
     </row>
-    <row r="149" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>216</v>
       </c>
@@ -30811,7 +30810,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>285</v>
       </c>
@@ -31022,7 +31021,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>103</v>
       </c>
@@ -31227,7 +31226,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>137</v>
       </c>
@@ -31399,7 +31398,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="153" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>118</v>
       </c>
@@ -31565,7 +31564,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>621</v>
       </c>
@@ -31721,7 +31720,7 @@
         <v>[40.58742,-105.0784],</v>
       </c>
     </row>
-    <row r="155" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>40</v>
       </c>
@@ -31896,7 +31895,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="156" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>37</v>
       </c>
@@ -32107,7 +32106,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>662</v>
       </c>
@@ -32260,7 +32259,7 @@
         <v>[40.58213,-105.02703],</v>
       </c>
     </row>
-    <row r="158" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>375</v>
       </c>
@@ -32426,7 +32425,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>535</v>
       </c>
@@ -32631,7 +32630,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>664</v>
       </c>
@@ -32675,7 +32674,7 @@
         <v>1900</v>
       </c>
       <c r="V160" s="4" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="W160" t="str">
         <f t="shared" si="232"/>
@@ -32823,7 +32822,7 @@
         <v>[40.62701,-105.13785],</v>
       </c>
     </row>
-    <row r="161" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>112</v>
       </c>
@@ -33019,7 +33018,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>541</v>
       </c>
@@ -33221,9 +33220,9 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="7" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C163" t="s">
         <v>428</v>
@@ -33232,7 +33231,7 @@
         <v>431</v>
       </c>
       <c r="G163" s="7" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H163">
         <v>1500</v>
@@ -33277,7 +33276,11 @@
         <v>1800</v>
       </c>
       <c r="V163" t="s">
-        <v>803</v>
+        <v>802</v>
+      </c>
+      <c r="W163">
+        <f t="shared" si="232"/>
+        <v>15</v>
       </c>
       <c r="X163">
         <f t="shared" ref="X163" si="244">IF(I163&gt;0,I163/100,"")</f>
@@ -33333,7 +33336,7 @@
       </c>
       <c r="AK163" t="str">
         <f t="shared" ref="AK163" si="257">IF(H163&gt;0,CONCATENATE(IF(W163&lt;=12,W163,W163-12),IF(OR(W163&lt;12,W163=24),"am","pm"),"-",IF(X163&lt;=12,X163,X163-12),IF(OR(X163&lt;12,X163=24),"am","pm")),"")</f>
-        <v>am-6pm</v>
+        <v>3pm-6pm</v>
       </c>
       <c r="AL163" t="str">
         <f t="shared" ref="AL163" si="258">IF(J163&gt;0,CONCATENATE(IF(Y163&lt;=12,Y163,Y163-12),IF(OR(Y163&lt;12,Y163=24),"am","pm"),"-",IF(Z163&lt;=12,Z163,Z163-12),IF(OR(Z163&lt;12,Z163=24),"am","pm")),"")</f>
@@ -33423,7 +33426,7 @@
         <v>[40.5228646,-105.0117552],</v>
       </c>
     </row>
-    <row r="164" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>80</v>
       </c>
@@ -33592,7 +33595,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>665</v>
       </c>
@@ -33711,7 +33714,7 @@
         <v>307</v>
       </c>
       <c r="AX165" s="4" t="str">
-        <f t="shared" ref="AX164:AX195" si="274">CONCATENATE("{
+        <f t="shared" ref="AX165:AX195" si="274">CONCATENATE("{
     'name': """,B165,""",
     'area': ","""",C165,""",",
 "'hours': {
@@ -33722,35 +33725,35 @@
       'sunday-start':"", 'sunday-end':"", 'monday-start':"", 'monday-end':"", 'tuesday-start':"", 'tuesday-end':"", 'wednesday-start':"1200", 'wednesday-end':"1700", 'thursday-start':"", 'thursday-end':"", 'friday-start':"", 'friday-end':"", 'saturday-start':"", 'saturday-end':""},  'description': "Wine Wednesdays - 10 percent off all purchases on Hump Day!", 'link':"", 'pricing':"med",   'phone-number': "", 'address': "5114 County Rd 23E Laporte CO", 'other-amenities': ['out','','easy'], 'has-drink':true, 'has-food':false},</v>
       </c>
       <c r="AY165" t="str">
-        <f t="shared" ref="AY164:AY197" si="275">IF(AS165&gt;0,"&lt;img src=@img/outdoor.png@&gt;","")</f>
+        <f t="shared" ref="AY165:AY197" si="275">IF(AS165&gt;0,"&lt;img src=@img/outdoor.png@&gt;","")</f>
         <v>&lt;img src=@img/outdoor.png@&gt;</v>
       </c>
       <c r="AZ165" t="str">
-        <f t="shared" ref="AZ164:AZ197" si="276">IF(AT165&gt;0,"&lt;img src=@img/pets.png@&gt;","")</f>
+        <f t="shared" ref="AZ165:AZ197" si="276">IF(AT165&gt;0,"&lt;img src=@img/pets.png@&gt;","")</f>
         <v/>
       </c>
       <c r="BA165" t="str">
-        <f t="shared" ref="BA164:BA197" si="277">IF(AU165="hard","&lt;img src=@img/hard.png@&gt;",IF(AU165="medium","&lt;img src=@img/medium.png@&gt;",IF(AU165="easy","&lt;img src=@img/easy.png@&gt;","")))</f>
+        <f t="shared" ref="BA165:BA197" si="277">IF(AU165="hard","&lt;img src=@img/hard.png@&gt;",IF(AU165="medium","&lt;img src=@img/medium.png@&gt;",IF(AU165="easy","&lt;img src=@img/easy.png@&gt;","")))</f>
         <v>&lt;img src=@img/easy.png@&gt;</v>
       </c>
       <c r="BB165" t="str">
-        <f t="shared" ref="BB164:BB197" si="278">IF(AV165="true","&lt;img src=@img/drinkicon.png@&gt;","")</f>
+        <f t="shared" ref="BB165:BB197" si="278">IF(AV165="true","&lt;img src=@img/drinkicon.png@&gt;","")</f>
         <v>&lt;img src=@img/drinkicon.png@&gt;</v>
       </c>
       <c r="BC165" t="str">
-        <f t="shared" ref="BC164:BC197" si="279">IF(AW165="true","&lt;img src=@img/foodicon.png@&gt;","")</f>
+        <f t="shared" ref="BC165:BC197" si="279">IF(AW165="true","&lt;img src=@img/foodicon.png@&gt;","")</f>
         <v/>
       </c>
       <c r="BD165" t="str">
-        <f t="shared" ref="BD164:BD195" si="280">CONCATENATE(AY165,AZ165,BA165,BB165,BC165,BK165)</f>
+        <f t="shared" ref="BD165:BD195" si="280">CONCATENATE(AY165,AZ165,BA165,BB165,BC165,BK165)</f>
         <v>&lt;img src=@img/outdoor.png@&gt;&lt;img src=@img/easy.png@&gt;&lt;img src=@img/drinkicon.png@&gt;</v>
       </c>
       <c r="BE165" t="str">
-        <f t="shared" ref="BE164:BE197" si="281">CONCATENATE(IF(AS165&gt;0,"outdoor ",""),IF(AT165&gt;0,"pet ",""),IF(AV165="true","drink ",""),IF(AW165="true","food ",""),AU165," ",E165," ",C165,IF(BJ165=TRUE," kid",""))</f>
+        <f t="shared" ref="BE165:BE197" si="281">CONCATENATE(IF(AS165&gt;0,"outdoor ",""),IF(AT165&gt;0,"pet ",""),IF(AV165="true","drink ",""),IF(AW165="true","food ",""),AU165," ",E165," ",C165,IF(BJ165=TRUE," kid",""))</f>
         <v>outdoor drink easy med nfoco</v>
       </c>
       <c r="BF165" t="str">
-        <f t="shared" ref="BF164:BF197" si="282">IF(C165="old","Old Town",IF(C165="campus","Near Campus",IF(C165="sfoco","South Foco",IF(C165="nfoco","North Foco",IF(C165="midtown","Midtown",IF(C165="cwest","Campus West",IF(C165="efoco","East FoCo",IF(C165="windsor","Windsor",""))))))))</f>
+        <f t="shared" ref="BF165:BF197" si="282">IF(C165="old","Old Town",IF(C165="campus","Near Campus",IF(C165="sfoco","South Foco",IF(C165="nfoco","North Foco",IF(C165="midtown","Midtown",IF(C165="cwest","Campus West",IF(C165="efoco","East FoCo",IF(C165="windsor","Windsor",""))))))))</f>
         <v>North Foco</v>
       </c>
       <c r="BG165">
@@ -33764,7 +33767,7 @@
         <v>[40.66018,-105.161719],</v>
       </c>
     </row>
-    <row r="166" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>452</v>
       </c>
@@ -33930,7 +33933,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="167" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>100</v>
       </c>
@@ -34096,7 +34099,7 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>624</v>
       </c>
@@ -34249,7 +34252,7 @@
         <v>[40.57906,-105.07656],</v>
       </c>
     </row>
-    <row r="169" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>83</v>
       </c>
@@ -34418,7 +34421,7 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>218</v>
       </c>
@@ -34617,7 +34620,7 @@
         <v/>
       </c>
     </row>
-    <row r="171" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>626</v>
       </c>
@@ -34797,7 +34800,7 @@
         <v>[40.56208,-105.03864],</v>
       </c>
     </row>
-    <row r="172" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>173</v>
       </c>
@@ -34996,7 +34999,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>570</v>
       </c>
@@ -35161,7 +35164,7 @@
         <v>[40.57891,-105.07843],</v>
       </c>
     </row>
-    <row r="174" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>751</v>
       </c>
@@ -35312,7 +35315,7 @@
         <v>[40.586451,-105.078568],</v>
       </c>
     </row>
-    <row r="175" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>697</v>
       </c>
@@ -35513,7 +35516,7 @@
         <v>[40.58815,-105.07761],</v>
       </c>
     </row>
-    <row r="176" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>629</v>
       </c>
@@ -35669,7 +35672,7 @@
         <v>[40.58899,-105.07637],</v>
       </c>
     </row>
-    <row r="177" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>563</v>
       </c>
@@ -35831,7 +35834,7 @@
         <v>[40.58487,-105.0765],</v>
       </c>
     </row>
-    <row r="178" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>632</v>
       </c>
@@ -35990,7 +35993,7 @@
         <v>[40.58758,-105.07636],</v>
       </c>
     </row>
-    <row r="179" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>453</v>
       </c>
@@ -36156,7 +36159,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="180" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>220</v>
       </c>
@@ -36370,7 +36373,7 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>380</v>
       </c>
@@ -36572,7 +36575,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>223</v>
       </c>
@@ -36738,7 +36741,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>552</v>
       </c>
@@ -36934,7 +36937,7 @@
         <v>[40.58741,-105.07661],</v>
       </c>
     </row>
-    <row r="184" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>634</v>
       </c>
@@ -37087,7 +37090,7 @@
         <v>[40.57844,-105.07856],</v>
       </c>
     </row>
-    <row r="185" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>287</v>
       </c>
@@ -37298,7 +37301,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>401</v>
       </c>
@@ -37467,7 +37470,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>747</v>
       </c>
@@ -37618,7 +37621,7 @@
         <v>[40.523973,-105.025125],</v>
       </c>
     </row>
-    <row r="188" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>745</v>
       </c>
@@ -37772,7 +37775,7 @@
         <v>[40.589425,-105.076553],</v>
       </c>
     </row>
-    <row r="189" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>636</v>
       </c>
@@ -37928,7 +37931,7 @@
         <v>[40.57429,-105.0971],</v>
       </c>
     </row>
-    <row r="190" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>658</v>
       </c>
@@ -38081,7 +38084,7 @@
         <v>[40.55258,-105.09673],</v>
       </c>
     </row>
-    <row r="191" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>128</v>
       </c>
@@ -38253,7 +38256,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>549</v>
       </c>
@@ -38418,7 +38421,7 @@
         <v>[40.55197,-105.03718],</v>
       </c>
     </row>
-    <row r="193" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>639</v>
       </c>
@@ -38587,7 +38590,7 @@
         <v>[40.57358,-105.05826],</v>
       </c>
     </row>
-    <row r="194" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>225</v>
       </c>
@@ -38745,7 +38748,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>49</v>
       </c>
@@ -38903,7 +38906,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>643</v>
       </c>
@@ -39058,7 +39061,7 @@
         <v>[40.57488,-105.10039],</v>
       </c>
     </row>
-    <row r="197" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>227</v>
       </c>
@@ -39238,77 +39241,77 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C2:C192" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:BL198">
+  <autoFilter ref="C2:C192"/>
+  <sortState ref="B2:BL198">
     <sortCondition ref="B2:B198"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G136" r:id="rId1" display="https://www.google.com/maps/dir/Current+Location/101 S. College Avenue, Fort Collins, CO 80524" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="AR42" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="AR99" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="AR28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="AR115" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="AR20" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="AR8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="AR55" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="AR34" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="AR64" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="AR46" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="AR164" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="AR54" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="AR126" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="AR95" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="AR63" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="AR167" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="AR151" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="AR19" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="AR10" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="AR161" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="AR91" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="AR153" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="AR113" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="AR191" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="AR93" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="AR15" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="AR86" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="AR5" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="AR7" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="AR43" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="AR45" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="AR57" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="AR82" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="AR106" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="AR114" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="AR116" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="AR136" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="AR16" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="AR24" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="AR62" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="AR80" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="AR85" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="AR110" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="AR128" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="AR138" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="AR142" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="AR149" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="AR170" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="AR182" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="AR197" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="AR23" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="AR58" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="AR66" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="AR67" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="AR77" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="AR101" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="AR150" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="AR185" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="AR59" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="AR79" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="AR48" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="AR9" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="AR175" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B11" r:id="rId65" display="https://www.yelp.com/biz/avuncular-bobs-beerhouse-fort-collins" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="AR173" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="G136" r:id="rId1" display="https://www.google.com/maps/dir/Current+Location/101 S. College Avenue, Fort Collins, CO 80524"/>
+    <hyperlink ref="AR42" r:id="rId2"/>
+    <hyperlink ref="AR99" r:id="rId3"/>
+    <hyperlink ref="AR28" r:id="rId4"/>
+    <hyperlink ref="AR115" r:id="rId5"/>
+    <hyperlink ref="AR20" r:id="rId6"/>
+    <hyperlink ref="AR8" r:id="rId7"/>
+    <hyperlink ref="AR55" r:id="rId8"/>
+    <hyperlink ref="AR34" r:id="rId9"/>
+    <hyperlink ref="AR64" r:id="rId10"/>
+    <hyperlink ref="AR46" r:id="rId11"/>
+    <hyperlink ref="AR164" r:id="rId12"/>
+    <hyperlink ref="AR54" r:id="rId13"/>
+    <hyperlink ref="AR126" r:id="rId14"/>
+    <hyperlink ref="AR95" r:id="rId15"/>
+    <hyperlink ref="AR63" r:id="rId16"/>
+    <hyperlink ref="AR167" r:id="rId17"/>
+    <hyperlink ref="AR151" r:id="rId18"/>
+    <hyperlink ref="AR19" r:id="rId19"/>
+    <hyperlink ref="AR10" r:id="rId20"/>
+    <hyperlink ref="AR161" r:id="rId21"/>
+    <hyperlink ref="AR91" r:id="rId22"/>
+    <hyperlink ref="AR153" r:id="rId23"/>
+    <hyperlink ref="AR113" r:id="rId24"/>
+    <hyperlink ref="AR191" r:id="rId25"/>
+    <hyperlink ref="AR93" r:id="rId26"/>
+    <hyperlink ref="AR15" r:id="rId27"/>
+    <hyperlink ref="AR86" r:id="rId28"/>
+    <hyperlink ref="AR5" r:id="rId29"/>
+    <hyperlink ref="AR7" r:id="rId30"/>
+    <hyperlink ref="AR43" r:id="rId31"/>
+    <hyperlink ref="AR45" r:id="rId32"/>
+    <hyperlink ref="AR57" r:id="rId33"/>
+    <hyperlink ref="AR82" r:id="rId34"/>
+    <hyperlink ref="AR106" r:id="rId35"/>
+    <hyperlink ref="AR114" r:id="rId36"/>
+    <hyperlink ref="AR116" r:id="rId37"/>
+    <hyperlink ref="AR136" r:id="rId38"/>
+    <hyperlink ref="AR16" r:id="rId39"/>
+    <hyperlink ref="AR24" r:id="rId40"/>
+    <hyperlink ref="AR62" r:id="rId41"/>
+    <hyperlink ref="AR80" r:id="rId42"/>
+    <hyperlink ref="AR85" r:id="rId43"/>
+    <hyperlink ref="AR110" r:id="rId44"/>
+    <hyperlink ref="AR128" r:id="rId45"/>
+    <hyperlink ref="AR138" r:id="rId46"/>
+    <hyperlink ref="AR142" r:id="rId47"/>
+    <hyperlink ref="AR149" r:id="rId48"/>
+    <hyperlink ref="AR170" r:id="rId49"/>
+    <hyperlink ref="AR182" r:id="rId50"/>
+    <hyperlink ref="AR197" r:id="rId51"/>
+    <hyperlink ref="AR23" r:id="rId52"/>
+    <hyperlink ref="AR58" r:id="rId53"/>
+    <hyperlink ref="AR66" r:id="rId54"/>
+    <hyperlink ref="AR67" r:id="rId55"/>
+    <hyperlink ref="AR77" r:id="rId56"/>
+    <hyperlink ref="AR101" r:id="rId57"/>
+    <hyperlink ref="AR150" r:id="rId58"/>
+    <hyperlink ref="AR185" r:id="rId59"/>
+    <hyperlink ref="AR59" r:id="rId60"/>
+    <hyperlink ref="AR79" r:id="rId61"/>
+    <hyperlink ref="AR48" r:id="rId62"/>
+    <hyperlink ref="AR9" r:id="rId63"/>
+    <hyperlink ref="AR175" r:id="rId64"/>
+    <hyperlink ref="B11" r:id="rId65" display="https://www.yelp.com/biz/avuncular-bobs-beerhouse-fort-collins"/>
+    <hyperlink ref="AR173" r:id="rId66"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId67"/>
@@ -39316,19 +39319,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>766</v>
       </c>
@@ -39345,7 +39348,7 @@
         <v>-105.076553</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>769</v>
       </c>
@@ -39362,7 +39365,7 @@
         <v>-105.076497</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>770</v>
       </c>
@@ -39379,7 +39382,7 @@
         <v>-105.025125</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>772</v>
       </c>
@@ -39396,7 +39399,7 @@
         <v>-105.05831000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>774</v>
       </c>
@@ -39413,7 +39416,7 @@
         <v>-105.07746400000001</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>775</v>
       </c>
@@ -39430,7 +39433,7 @@
         <v>-105.07761600000001</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>776</v>
       </c>
@@ -39456,14 +39459,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <customProperties>

</xml_diff>

<commit_message>
Updated cafe vino content
</commit_message>
<xml_diff>
--- a/database_working.xlsx
+++ b/database_working.xlsx
@@ -1609,9 +1609,6 @@
     <t>524 W. Laurel Street, Fort Collins, CO 80521</t>
   </si>
   <si>
-    <t>Monday-Friday&lt;br&gt;3-6pm and 9pm-close&lt;br&gt;$6 White Wine&lt;br&gt;$6 Red Wine &lt;br&gt;$2.5 select beers&lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;$3 Toasted nuts&lt;br&gt;$4 Hummus naan&lt;br&gt;$4 Olives and peppadews&lt;br&gt;$5 Lunchable</t>
-  </si>
-  <si>
     <t>Monday-Sunday&lt;br&gt;3-6 pm:&lt;br&gt;$2.50 mugs&lt;br&gt;$3.50 20-oz pints&lt;br&gt;$10 pitchers&lt;br&gt;&lt;br&gt;Monday&lt;br&gt;$10 14-inch pizza&lt;br&gt;&lt;br&gt;Tuesday&lt;br&gt;1 hour free pool with a pitcher of beer or large pizza&lt;br&gt;&lt;br&gt;Wednesday&lt;br&gt;$2 Pints of Beer after 10 pm&lt;br&gt;&lt;br&gt;Thursday&lt;br&gt;1 hour free pool with a pitcher</t>
   </si>
   <si>
@@ -2449,6 +2446,9 @@
   </si>
   <si>
     <t>&lt;b&gt;Drink Specials&lt;/b&gt;&lt;br&gt;$1 off 8oz pours&lt;br&gt;$2 off 12oz pours&lt;br&gt;$3 off 16oz pours  &lt;br&gt;$5 glasses of wine&lt;br&gt;&lt;b&gt;Food Specials&lt;/b&gt;&lt;br&gt;$1 wings (up to 24)&lt;br&gt;$3 chips &amp; salsa (no refill)&lt;br&gt;$4 fire &amp; ice&lt;br&gt;$5 artisan flatbreads&lt;br&gt;$5 nachos&lt;br&gt;&lt;b&gt;Daily Food Specials&lt;/b&gt;&lt;br&gt;Slider Mondays&lt;br&gt;Taco Tuesdays ($2 Tacos) and Beer 2, 12, and 22 on the board are only $2&lt;br&gt;Wing Wednesdays&lt;br&gt;Satay Thursdays&lt;br&gt;Friday Night Flights - 4oz beers paired with 4oz bites</t>
+  </si>
+  <si>
+    <t>Monday-Friday&lt;br&gt;3-6pm and 9pm-close at the bar&lt;br&gt;A range of drink specials&lt;br&gt;Toum (Lebanese Garlic Spread) $4&lt;br&gt;Crispy Chickpeas $4&lt;br&gt;Patatas Bravas $5&lt;br&gt;Hummus Naan $6&lt;br&gt;Potted Salmon $6&lt;br&gt;Cacio E Pepe $7</t>
   </si>
 </sst>
 </file>
@@ -3416,10 +3416,10 @@
   <dimension ref="B1:BL197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AL45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="I33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="U86" sqref="U86"/>
-      <selection pane="bottomRight" activeCell="AT45" sqref="AT45"/>
+      <selection pane="bottomRight" activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4031,7 +4031,7 @@
     </row>
     <row r="4" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C4" t="s">
         <v>426</v>
@@ -4040,7 +4040,7 @@
         <v>431</v>
       </c>
       <c r="G4" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="W4" t="str">
         <f t="shared" si="0"/>
@@ -4127,7 +4127,7 @@
         <v/>
       </c>
       <c r="AR4" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="AU4" t="s">
         <v>298</v>
@@ -5334,19 +5334,19 @@
     </row>
     <row r="11" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C11" t="s">
         <v>308</v>
       </c>
       <c r="D11" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E11" t="s">
         <v>431</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="W11" t="str">
         <f t="shared" si="0"/>
@@ -5433,7 +5433,7 @@
         <v/>
       </c>
       <c r="AR11" s="10" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="AU11" t="s">
         <v>28</v>
@@ -5821,7 +5821,7 @@
     </row>
     <row r="14" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C14" t="s">
         <v>309</v>
@@ -5830,7 +5830,7 @@
         <v>431</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H14">
         <v>1500</v>
@@ -5875,7 +5875,7 @@
         <v>1800</v>
       </c>
       <c r="V14" s="14" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="W14">
         <f t="shared" si="0"/>
@@ -5962,7 +5962,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR14" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="AS14" t="s">
         <v>295</v>
@@ -5971,7 +5971,7 @@
         <v>299</v>
       </c>
       <c r="AV14" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="AW14" s="3" t="s">
         <v>306</v>
@@ -6240,7 +6240,7 @@
         <v>1900</v>
       </c>
       <c r="V16" s="16" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="0"/>
@@ -6397,16 +6397,16 @@
     </row>
     <row r="17" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C17" t="s">
         <v>308</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="V17" s="14" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="W17" t="str">
         <f t="shared" si="0"/>
@@ -6493,7 +6493,7 @@
         <v/>
       </c>
       <c r="AR17" s="12" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="AS17" t="s">
         <v>295</v>
@@ -6616,7 +6616,7 @@
         <v>1800</v>
       </c>
       <c r="V18" s="14" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="W18">
         <f t="shared" si="0"/>
@@ -6836,7 +6836,7 @@
         <v>2400</v>
       </c>
       <c r="V19" s="14" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="W19">
         <f t="shared" si="0"/>
@@ -7412,7 +7412,7 @@
         <v>1800</v>
       </c>
       <c r="V22" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="W22">
         <f t="shared" si="0"/>
@@ -7988,7 +7988,7 @@
     </row>
     <row r="25" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C25" t="s">
         <v>426</v>
@@ -7997,7 +7997,7 @@
         <v>431</v>
       </c>
       <c r="G25" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="P25">
         <v>2000</v>
@@ -8018,7 +8018,7 @@
         <v>2000</v>
       </c>
       <c r="V25" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="W25" t="str">
         <f t="shared" si="0"/>
@@ -8105,7 +8105,7 @@
         <v>6pm-8pm</v>
       </c>
       <c r="AR25" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="AU25" t="s">
         <v>298</v>
@@ -8687,7 +8687,7 @@
     </row>
     <row r="29" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C29" t="s">
         <v>309</v>
@@ -8696,7 +8696,7 @@
         <v>431</v>
       </c>
       <c r="G29" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="W29" t="str">
         <f t="shared" si="0"/>
@@ -9165,13 +9165,13 @@
     </row>
     <row r="32" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C32" t="s">
         <v>429</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="W32" t="str">
         <f t="shared" si="0"/>
@@ -9258,7 +9258,7 @@
         <v/>
       </c>
       <c r="AR32" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AU32" t="s">
         <v>299</v>
@@ -9321,13 +9321,13 @@
     </row>
     <row r="33" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C33" t="s">
         <v>309</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="W33" t="str">
         <f t="shared" si="0"/>
@@ -9414,7 +9414,7 @@
         <v/>
       </c>
       <c r="AR33" s="10" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="AU33" t="s">
         <v>299</v>
@@ -9532,7 +9532,7 @@
         <v>1800</v>
       </c>
       <c r="V34" t="s">
-        <v>525</v>
+        <v>804</v>
       </c>
       <c r="W34" t="str">
         <f t="shared" ref="W34:W64" si="34">IF(H34&gt;0,H34/100,"")</f>
@@ -9642,7 +9642,7 @@
         <v>{
     'name': "Cafe Vino",
     'area': "campus",'hours': {
-      'sunday-start':"", 'sunday-end':"", 'monday-start':"1500", 'monday-end':"1800", 'tuesday-start':"1500", 'tuesday-end':"1800", 'wednesday-start':"1500", 'wednesday-end':"1800", 'thursday-start':"1500", 'thursday-end':"1800", 'friday-start':"1500", 'friday-end':"1800", 'saturday-start':"", 'saturday-end':""},  'description': "Monday-Friday&lt;br&gt;3-6pm and 9pm-close&lt;br&gt;$6 White Wine&lt;br&gt;$6 Red Wine &lt;br&gt;$2.5 select beers&lt;br&gt;&lt;br&gt; &lt;br&gt;&lt;br&gt;$3 Toasted nuts&lt;br&gt;$4 Hummus naan&lt;br&gt;$4 Olives and peppadews&lt;br&gt;$5 Lunchable", 'link':"http://www.cafevino.com/", 'pricing':"med",   'phone-number': "", 'address': "1200 S College Ave., Fort Collins 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':true, 'has-food':true},</v>
+      'sunday-start':"", 'sunday-end':"", 'monday-start':"1500", 'monday-end':"1800", 'tuesday-start':"1500", 'tuesday-end':"1800", 'wednesday-start':"1500", 'wednesday-end':"1800", 'thursday-start':"1500", 'thursday-end':"1800", 'friday-start':"1500", 'friday-end':"1800", 'saturday-start':"", 'saturday-end':""},  'description': "Monday-Friday&lt;br&gt;3-6pm and 9pm-close at the bar&lt;br&gt;A range of drink specials&lt;br&gt;Toum (Lebanese Garlic Spread) $4&lt;br&gt;Crispy Chickpeas $4&lt;br&gt;Patatas Bravas $5&lt;br&gt;Hummus Naan $6&lt;br&gt;Potted Salmon $6&lt;br&gt;Cacio E Pepe $7", 'link':"http://www.cafevino.com/", 'pricing':"med",   'phone-number': "", 'address': "1200 S College Ave., Fort Collins 80524", 'other-amenities': ['outdoor','','medium'], 'has-drink':true, 'has-food':true},</v>
       </c>
       <c r="AY34" t="str">
         <f t="shared" ref="AY34:AY66" si="49">IF(AS34&gt;0,"&lt;img src=@img/outdoor.png@&gt;","")</f>
@@ -9693,13 +9693,13 @@
     </row>
     <row r="35" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C35" t="s">
         <v>426</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="W35" t="str">
         <f t="shared" si="34"/>
@@ -9786,7 +9786,7 @@
         <v/>
       </c>
       <c r="AR35" s="12" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="AU35" t="s">
         <v>28</v>
@@ -10275,7 +10275,7 @@
         <v>&lt;img src=@img/kidicon.png@&gt;</v>
       </c>
       <c r="BL37" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="38" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -10482,13 +10482,13 @@
     </row>
     <row r="39" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C39" t="s">
         <v>427</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="W39" t="str">
         <f t="shared" si="34"/>
@@ -10575,7 +10575,7 @@
         <v/>
       </c>
       <c r="AR39" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="AU39" t="s">
         <v>299</v>
@@ -10807,16 +10807,16 @@
     </row>
     <row r="41" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>725</v>
+      </c>
+      <c r="C41" t="s">
         <v>726</v>
-      </c>
-      <c r="C41" t="s">
-        <v>727</v>
       </c>
       <c r="E41" t="s">
         <v>431</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="H41">
         <v>1600</v>
@@ -10861,7 +10861,7 @@
         <v>1800</v>
       </c>
       <c r="V41" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="W41">
         <f t="shared" si="34"/>
@@ -10948,7 +10948,7 @@
         <v>4pm-6pm</v>
       </c>
       <c r="AR41" s="6" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="AU41" t="s">
         <v>28</v>
@@ -11250,7 +11250,7 @@
         <v>1700</v>
       </c>
       <c r="V43" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="W43">
         <f t="shared" si="34"/>
@@ -11449,7 +11449,7 @@
         <v>1800</v>
       </c>
       <c r="V44" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="W44" t="str">
         <f t="shared" si="34"/>
@@ -11642,7 +11642,7 @@
         <v>2100</v>
       </c>
       <c r="V45" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="W45">
         <f t="shared" si="34"/>
@@ -12013,7 +12013,7 @@
     </row>
     <row r="47" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C47" t="s">
         <v>426</v>
@@ -12022,7 +12022,7 @@
         <v>431</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="W47" t="str">
         <f t="shared" ref="W47" si="59">IF(H47&gt;0,H47/100,"")</f>
@@ -12113,7 +12113,7 @@
         <v>295</v>
       </c>
       <c r="AT47" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="AU47" t="s">
         <v>298</v>
@@ -12548,7 +12548,7 @@
     </row>
     <row r="50" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C50" t="s">
         <v>428</v>
@@ -12747,7 +12747,7 @@
     </row>
     <row r="51" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C51" t="s">
         <v>426</v>
@@ -12756,7 +12756,7 @@
         <v>54</v>
       </c>
       <c r="G51" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="W51" t="str">
         <f t="shared" si="34"/>
@@ -12843,7 +12843,7 @@
         <v/>
       </c>
       <c r="AR51" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="AU51" t="s">
         <v>298</v>
@@ -12906,7 +12906,7 @@
     </row>
     <row r="52" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C52" t="s">
         <v>426</v>
@@ -12915,7 +12915,7 @@
         <v>431</v>
       </c>
       <c r="G52" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="W52" t="str">
         <f t="shared" si="34"/>
@@ -13002,7 +13002,7 @@
         <v/>
       </c>
       <c r="AR52" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="AS52" t="s">
         <v>295</v>
@@ -13068,7 +13068,7 @@
     </row>
     <row r="53" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C53" t="s">
         <v>309</v>
@@ -13077,7 +13077,7 @@
         <v>431</v>
       </c>
       <c r="G53" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H53">
         <v>1600</v>
@@ -13110,7 +13110,7 @@
         <v>1900</v>
       </c>
       <c r="V53" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="W53">
         <f t="shared" si="34"/>
@@ -13197,7 +13197,7 @@
         <v/>
       </c>
       <c r="AR53" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="AU53" t="s">
         <v>299</v>
@@ -13592,7 +13592,7 @@
     </row>
     <row r="56" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C56" t="s">
         <v>427</v>
@@ -13601,7 +13601,7 @@
         <v>431</v>
       </c>
       <c r="G56" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="H56">
         <v>1600</v>
@@ -13640,7 +13640,7 @@
         <v>1800</v>
       </c>
       <c r="V56" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="W56">
         <f t="shared" si="34"/>
@@ -13727,7 +13727,7 @@
         <v>4pm-6pm</v>
       </c>
       <c r="AR56" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="AS56" t="s">
         <v>295</v>
@@ -13820,7 +13820,7 @@
         <v>1800</v>
       </c>
       <c r="V57" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="W57" t="str">
         <f t="shared" si="34"/>
@@ -13913,7 +13913,7 @@
         <v>295</v>
       </c>
       <c r="AT57" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="AU57" t="s">
         <v>299</v>
@@ -14390,7 +14390,7 @@
     </row>
     <row r="60" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C60" t="s">
         <v>426</v>
@@ -14399,7 +14399,7 @@
         <v>54</v>
       </c>
       <c r="G60" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="W60" t="str">
         <f t="shared" si="34"/>
@@ -14486,7 +14486,7 @@
         <v/>
       </c>
       <c r="AR60" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="AU60" t="s">
         <v>298</v>
@@ -14938,7 +14938,7 @@
         <v>1800</v>
       </c>
       <c r="V63" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="W63">
         <f t="shared" si="34"/>
@@ -15258,7 +15258,7 @@
     </row>
     <row r="65" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C65" t="s">
         <v>426</v>
@@ -15267,7 +15267,7 @@
         <v>54</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="W65" t="str">
         <f t="shared" ref="W65:W91" si="89">IF(H65&gt;0,H65/100,"")</f>
@@ -15346,7 +15346,7 @@
         <v/>
       </c>
       <c r="AR65" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="AS65" t="s">
         <v>295</v>
@@ -15671,7 +15671,7 @@
         <v>1800</v>
       </c>
       <c r="V67" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="W67" t="str">
         <f t="shared" si="89"/>
@@ -15832,7 +15832,7 @@
     </row>
     <row r="68" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C68" t="s">
         <v>309</v>
@@ -15841,7 +15841,7 @@
         <v>431</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="W68" t="str">
         <f t="shared" si="89"/>
@@ -15920,7 +15920,7 @@
         <v/>
       </c>
       <c r="AR68" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="AU68" t="s">
         <v>299</v>
@@ -15983,13 +15983,13 @@
     </row>
     <row r="69" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C69" t="s">
         <v>426</v>
       </c>
       <c r="G69" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="W69" t="str">
         <f t="shared" si="89"/>
@@ -16192,7 +16192,7 @@
         <v>2400</v>
       </c>
       <c r="V70" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="W70">
         <f t="shared" si="89"/>
@@ -16398,7 +16398,7 @@
         <v>2400</v>
       </c>
       <c r="V71" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="W71" t="str">
         <f t="shared" si="89"/>
@@ -16887,7 +16887,7 @@
     </row>
     <row r="74" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C74" t="s">
         <v>426</v>
@@ -16896,7 +16896,7 @@
         <v>431</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="H74">
         <v>1600</v>
@@ -16941,7 +16941,7 @@
         <v>1800</v>
       </c>
       <c r="V74" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="W74">
         <f t="shared" si="89"/>
@@ -17028,7 +17028,7 @@
         <v>4pm-6pm</v>
       </c>
       <c r="AR74" s="12" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="AS74" t="s">
         <v>295</v>
@@ -17094,16 +17094,16 @@
     </row>
     <row r="75" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C75" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E75" t="s">
         <v>431</v>
       </c>
       <c r="G75" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="W75" t="str">
         <f t="shared" si="89"/>
@@ -17255,16 +17255,16 @@
     </row>
     <row r="76" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C76" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E76" t="s">
         <v>431</v>
       </c>
       <c r="G76" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="H76">
         <v>1500</v>
@@ -17309,7 +17309,7 @@
         <v>1800</v>
       </c>
       <c r="V76" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="W76">
         <f t="shared" si="89"/>
@@ -17396,7 +17396,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR76" s="6" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AU76" t="s">
         <v>299</v>
@@ -17516,7 +17516,7 @@
         <v>1900</v>
       </c>
       <c r="V77" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="W77">
         <f t="shared" si="89"/>
@@ -17670,7 +17670,7 @@
     </row>
     <row r="78" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C78" t="s">
         <v>426</v>
@@ -17679,7 +17679,7 @@
         <v>431</v>
       </c>
       <c r="G78" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W78" t="str">
         <f t="shared" si="89"/>
@@ -17766,7 +17766,7 @@
         <v/>
       </c>
       <c r="AR78" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="AU78" t="s">
         <v>298</v>
@@ -17880,7 +17880,7 @@
         <v>2300</v>
       </c>
       <c r="V79" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="W79">
         <f t="shared" si="89"/>
@@ -18041,7 +18041,7 @@
         <v>&lt;img src=@img/kidicon.png@&gt;</v>
       </c>
       <c r="BL79" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="80" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -18764,7 +18764,7 @@
     </row>
     <row r="84" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C84" t="s">
         <v>426</v>
@@ -18773,7 +18773,7 @@
         <v>431</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="J84">
         <v>1600</v>
@@ -18806,7 +18806,7 @@
         <v>1800</v>
       </c>
       <c r="V84" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="X84" t="str">
         <f t="shared" ref="X84" si="121">IF(I84&gt;0,I84/100,"")</f>
@@ -19343,7 +19343,7 @@
     </row>
     <row r="87" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C87" t="s">
         <v>428</v>
@@ -19352,7 +19352,7 @@
         <v>431</v>
       </c>
       <c r="G87" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="W87" t="str">
         <f t="shared" si="89"/>
@@ -19499,13 +19499,13 @@
     </row>
     <row r="88" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C88" t="s">
         <v>429</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H88">
         <v>1100</v>
@@ -19550,7 +19550,7 @@
         <v>1300</v>
       </c>
       <c r="V88" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="W88">
         <f t="shared" si="89"/>
@@ -19637,7 +19637,7 @@
         <v>11am-1pm</v>
       </c>
       <c r="AR88" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="AS88" t="s">
         <v>295</v>
@@ -20303,7 +20303,7 @@
     </row>
     <row r="92" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C92" t="s">
         <v>309</v>
@@ -20312,7 +20312,7 @@
         <v>431</v>
       </c>
       <c r="G92" s="7" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="AK92" t="str">
         <f t="shared" si="111"/>
@@ -20343,7 +20343,7 @@
         <v/>
       </c>
       <c r="AR92" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="AS92" t="s">
         <v>295</v>
@@ -20575,7 +20575,7 @@
     </row>
     <row r="94" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C94" t="s">
         <v>429</v>
@@ -20584,7 +20584,7 @@
         <v>54</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="J94">
         <v>1100</v>
@@ -20617,7 +20617,7 @@
         <v>1400</v>
       </c>
       <c r="V94" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="W94" t="str">
         <f t="shared" ref="W94" si="165">IF(H94&gt;0,H94/100,"")</f>
@@ -20935,7 +20935,7 @@
     </row>
     <row r="96" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C96" t="s">
         <v>428</v>
@@ -20947,7 +20947,7 @@
         <v>431</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H96">
         <v>1600</v>
@@ -20992,7 +20992,7 @@
         <v>1800</v>
       </c>
       <c r="V96" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="W96">
         <f t="shared" si="151"/>
@@ -21079,7 +21079,7 @@
         <v>4pm-6pm</v>
       </c>
       <c r="AR96" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AS96" t="s">
         <v>295</v>
@@ -21149,13 +21149,13 @@
     </row>
     <row r="97" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C97" t="s">
         <v>428</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H97">
         <v>1100</v>
@@ -21200,7 +21200,7 @@
         <v>1800</v>
       </c>
       <c r="V97" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="W97">
         <f t="shared" si="151"/>
@@ -21287,7 +21287,7 @@
         <v>11am-6pm</v>
       </c>
       <c r="AR97" s="12" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="AU97" t="s">
         <v>28</v>
@@ -21763,13 +21763,13 @@
     </row>
     <row r="100" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C100" t="s">
         <v>426</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="W100" t="str">
         <f t="shared" si="151"/>
@@ -21856,7 +21856,7 @@
         <v/>
       </c>
       <c r="AR100" s="12" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AU100" t="s">
         <v>28</v>
@@ -22134,13 +22134,13 @@
     </row>
     <row r="102" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C102" t="s">
         <v>426</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="W102" t="str">
         <f t="shared" si="151"/>
@@ -22227,7 +22227,7 @@
         <v/>
       </c>
       <c r="AR102" s="12" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="AU102" t="s">
         <v>298</v>
@@ -22290,13 +22290,13 @@
     </row>
     <row r="103" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C103" t="s">
         <v>429</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W103" t="str">
         <f t="shared" si="151"/>
@@ -22488,7 +22488,7 @@
         <v>1800</v>
       </c>
       <c r="V104" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="W104" t="str">
         <f t="shared" si="151"/>
@@ -22645,7 +22645,7 @@
     </row>
     <row r="105" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C105" t="s">
         <v>308</v>
@@ -22654,7 +22654,7 @@
         <v>431</v>
       </c>
       <c r="G105" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="W105" t="str">
         <f t="shared" si="151"/>
@@ -22741,7 +22741,7 @@
         <v/>
       </c>
       <c r="AR105" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="AU105" t="s">
         <v>28</v>
@@ -22976,13 +22976,13 @@
     </row>
     <row r="107" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C107" t="s">
         <v>309</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="W107" t="str">
         <f t="shared" si="151"/>
@@ -23069,7 +23069,7 @@
         <v/>
       </c>
       <c r="AR107" s="10" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="AU107" t="s">
         <v>299</v>
@@ -23132,19 +23132,19 @@
     </row>
     <row r="108" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C108" t="s">
         <v>309</v>
       </c>
       <c r="D108" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E108" t="s">
         <v>54</v>
       </c>
       <c r="G108" s="7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H108">
         <v>1400</v>
@@ -23189,7 +23189,7 @@
         <v>1700</v>
       </c>
       <c r="V108" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="W108">
         <f t="shared" si="151"/>
@@ -23276,7 +23276,7 @@
         <v>2pm-5pm</v>
       </c>
       <c r="AR108" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="AU108" t="s">
         <v>299</v>
@@ -23846,7 +23846,7 @@
     </row>
     <row r="112" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C112" t="s">
         <v>429</v>
@@ -23855,7 +23855,7 @@
         <v>431</v>
       </c>
       <c r="G112" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H112">
         <v>1600</v>
@@ -23900,7 +23900,7 @@
         <v>1900</v>
       </c>
       <c r="V112" s="4" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="W112">
         <f t="shared" si="151"/>
@@ -23987,7 +23987,7 @@
         <v>4pm-7pm</v>
       </c>
       <c r="AR112" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="AS112" t="s">
         <v>295</v>
@@ -24696,7 +24696,7 @@
         <v>1800</v>
       </c>
       <c r="V116" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="W116" t="str">
         <f t="shared" si="151"/>
@@ -24859,7 +24859,7 @@
     </row>
     <row r="117" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C117" t="s">
         <v>427</v>
@@ -24868,7 +24868,7 @@
         <v>431</v>
       </c>
       <c r="G117" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="W117" t="str">
         <f t="shared" si="151"/>
@@ -24955,7 +24955,7 @@
         <v/>
       </c>
       <c r="AR117" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="AU117" t="s">
         <v>299</v>
@@ -25184,7 +25184,7 @@
     </row>
     <row r="119" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C119" t="s">
         <v>309</v>
@@ -25193,7 +25193,7 @@
         <v>54</v>
       </c>
       <c r="G119" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="W119" t="str">
         <f t="shared" si="151"/>
@@ -25847,7 +25847,7 @@
     </row>
     <row r="123" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C123" t="s">
         <v>309</v>
@@ -25856,7 +25856,7 @@
         <v>431</v>
       </c>
       <c r="G123" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="W123" t="str">
         <f t="shared" ref="W123:W153" si="198">IF(H123&gt;0,H123/100,"")</f>
@@ -25935,7 +25935,7 @@
         <v/>
       </c>
       <c r="AR123" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="AU123" t="s">
         <v>299</v>
@@ -25998,13 +25998,13 @@
     </row>
     <row r="124" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C124" t="s">
         <v>428</v>
       </c>
       <c r="G124" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="H124">
         <v>1500</v>
@@ -26049,7 +26049,7 @@
         <v>1800</v>
       </c>
       <c r="V124" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="W124">
         <f t="shared" si="198"/>
@@ -26136,7 +26136,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR124" s="12" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="AS124" t="s">
         <v>295</v>
@@ -26202,13 +26202,13 @@
     </row>
     <row r="125" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C125" t="s">
         <v>308</v>
       </c>
       <c r="G125" s="7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="H125">
         <v>1500</v>
@@ -26340,7 +26340,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR125" s="12" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AU125" t="s">
         <v>28</v>
@@ -26617,19 +26617,19 @@
     </row>
     <row r="127" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C127" t="s">
         <v>426</v>
       </c>
       <c r="D127" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E127" t="s">
         <v>431</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="J127">
         <v>1700</v>
@@ -26662,7 +26662,7 @@
         <v>2400</v>
       </c>
       <c r="V127" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="W127" t="str">
         <f t="shared" si="198"/>
@@ -26749,7 +26749,7 @@
         <v/>
       </c>
       <c r="AR127" s="10" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="AU127" t="s">
         <v>298</v>
@@ -27062,7 +27062,7 @@
         <v>2400</v>
       </c>
       <c r="V129" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="W129" t="str">
         <f t="shared" si="198"/>
@@ -27385,7 +27385,7 @@
     </row>
     <row r="131" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C131" t="s">
         <v>308</v>
@@ -27394,7 +27394,7 @@
         <v>54</v>
       </c>
       <c r="G131" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="W131" t="str">
         <f t="shared" si="198"/>
@@ -27481,7 +27481,7 @@
         <v/>
       </c>
       <c r="AR131" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="AU131" t="s">
         <v>28</v>
@@ -27544,7 +27544,7 @@
     </row>
     <row r="132" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C132" t="s">
         <v>308</v>
@@ -27553,7 +27553,7 @@
         <v>431</v>
       </c>
       <c r="G132" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="W132" t="str">
         <f t="shared" si="198"/>
@@ -27640,7 +27640,7 @@
         <v/>
       </c>
       <c r="AR132" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="AS132" t="s">
         <v>295</v>
@@ -27749,7 +27749,7 @@
         <v>1600</v>
       </c>
       <c r="V133" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="W133" t="str">
         <f t="shared" si="198"/>
@@ -27909,7 +27909,7 @@
     </row>
     <row r="134" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C134" t="s">
         <v>309</v>
@@ -27918,7 +27918,7 @@
         <v>431</v>
       </c>
       <c r="G134" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="H134">
         <v>1500</v>
@@ -27963,7 +27963,7 @@
         <v>1800</v>
       </c>
       <c r="V134" s="4" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="W134">
         <f t="shared" si="198"/>
@@ -28050,7 +28050,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR134" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="AU134" t="s">
         <v>299</v>
@@ -28113,7 +28113,7 @@
     </row>
     <row r="135" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C135" t="s">
         <v>308</v>
@@ -28122,7 +28122,7 @@
         <v>54</v>
       </c>
       <c r="G135" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="W135" t="str">
         <f t="shared" si="198"/>
@@ -28209,7 +28209,7 @@
         <v/>
       </c>
       <c r="AR135" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="AU135" t="s">
         <v>28</v>
@@ -28733,7 +28733,7 @@
         <v>2000</v>
       </c>
       <c r="V138" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="W138">
         <f t="shared" si="198"/>
@@ -29222,7 +29222,7 @@
     </row>
     <row r="141" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C141" t="s">
         <v>309</v>
@@ -29231,7 +29231,7 @@
         <v>54</v>
       </c>
       <c r="G141" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="W141" t="str">
         <f t="shared" si="198"/>
@@ -29710,7 +29710,7 @@
     </row>
     <row r="144" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C144" t="s">
         <v>309</v>
@@ -29719,7 +29719,7 @@
         <v>431</v>
       </c>
       <c r="G144" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="H144">
         <v>1500</v>
@@ -29764,7 +29764,7 @@
         <v>1800</v>
       </c>
       <c r="V144" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="W144">
         <f t="shared" si="198"/>
@@ -29851,7 +29851,7 @@
         <v>3pm-6pm</v>
       </c>
       <c r="AR144" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="AU144" t="s">
         <v>299</v>
@@ -29914,7 +29914,7 @@
     </row>
     <row r="145" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C145" t="s">
         <v>309</v>
@@ -29923,7 +29923,7 @@
         <v>431</v>
       </c>
       <c r="G145" s="7" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="W145" t="str">
         <f t="shared" si="198"/>
@@ -30002,7 +30002,7 @@
         <v/>
       </c>
       <c r="AR145" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="AS145" t="s">
         <v>295</v>
@@ -30442,7 +30442,7 @@
     </row>
     <row r="148" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C148" t="s">
         <v>308</v>
@@ -30451,7 +30451,7 @@
         <v>431</v>
       </c>
       <c r="G148" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J148">
         <v>1500</v>
@@ -30484,7 +30484,7 @@
         <v>1800</v>
       </c>
       <c r="V148" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="W148" t="str">
         <f t="shared" si="198"/>
@@ -30682,7 +30682,7 @@
         <v>2000</v>
       </c>
       <c r="V149" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="W149">
         <f t="shared" si="198"/>
@@ -31104,7 +31104,7 @@
         <v>1900</v>
       </c>
       <c r="V151" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="W151">
         <f t="shared" si="198"/>
@@ -31596,13 +31596,13 @@
     </row>
     <row r="154" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C154" t="s">
         <v>426</v>
       </c>
       <c r="G154" s="7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="W154" t="str">
         <f t="shared" ref="W154:W186" si="232">IF(H154&gt;0,H154/100,"")</f>
@@ -31689,7 +31689,7 @@
         <v/>
       </c>
       <c r="AR154" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="AU154" t="s">
         <v>298</v>
@@ -32138,13 +32138,13 @@
     </row>
     <row r="157" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E157" t="s">
         <v>431</v>
       </c>
       <c r="G157" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="W157" t="str">
         <f t="shared" si="232"/>
@@ -32457,7 +32457,7 @@
     </row>
     <row r="159" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C159" t="s">
         <v>426</v>
@@ -32466,7 +32466,7 @@
         <v>431</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H159">
         <v>1500</v>
@@ -32511,7 +32511,7 @@
         <v>2400</v>
       </c>
       <c r="V159" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="W159">
         <f t="shared" si="232"/>
@@ -32662,7 +32662,7 @@
     </row>
     <row r="160" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C160" t="s">
         <v>427</v>
@@ -32671,7 +32671,7 @@
         <v>54</v>
       </c>
       <c r="G160" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="J160">
         <v>1400</v>
@@ -32704,7 +32704,7 @@
         <v>1900</v>
       </c>
       <c r="V160" s="4" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="W160" t="str">
         <f t="shared" si="232"/>
@@ -33050,7 +33050,7 @@
     </row>
     <row r="162" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C162" t="s">
         <v>426</v>
@@ -33062,7 +33062,7 @@
         <v>431</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H162">
         <v>1130</v>
@@ -33095,7 +33095,7 @@
         <v>1800</v>
       </c>
       <c r="V162" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="W162">
         <f t="shared" si="232"/>
@@ -33182,7 +33182,7 @@
         <v/>
       </c>
       <c r="AR162" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AS162" t="s">
         <v>295</v>
@@ -33252,7 +33252,7 @@
     </row>
     <row r="163" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="7" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C163" t="s">
         <v>428</v>
@@ -33261,7 +33261,7 @@
         <v>431</v>
       </c>
       <c r="G163" s="7" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H163">
         <v>1500</v>
@@ -33306,7 +33306,7 @@
         <v>1800</v>
       </c>
       <c r="V163" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="W163">
         <f t="shared" si="232"/>
@@ -33627,7 +33627,7 @@
     </row>
     <row r="165" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C165" t="s">
         <v>427</v>
@@ -33636,7 +33636,7 @@
         <v>431</v>
       </c>
       <c r="G165" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N165">
         <v>1200</v>
@@ -33645,7 +33645,7 @@
         <v>1700</v>
       </c>
       <c r="V165" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="W165" t="str">
         <f t="shared" si="232"/>
@@ -33732,7 +33732,7 @@
         <v/>
       </c>
       <c r="AS165" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="AU165" t="s">
         <v>299</v>
@@ -34131,13 +34131,13 @@
     </row>
     <row r="168" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C168" t="s">
         <v>429</v>
       </c>
       <c r="G168" s="7" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W168" t="str">
         <f t="shared" si="232"/>
@@ -34652,13 +34652,13 @@
     </row>
     <row r="171" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C171" t="s">
         <v>309</v>
       </c>
       <c r="G171" s="7" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="L171">
         <v>1600</v>
@@ -34769,7 +34769,7 @@
         <v/>
       </c>
       <c r="AR171" s="12" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="AU171" t="s">
         <v>299</v>
@@ -35031,19 +35031,19 @@
     </row>
     <row r="173" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C173" t="s">
         <v>426</v>
       </c>
       <c r="D173" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E173" t="s">
         <v>431</v>
       </c>
       <c r="G173" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="W173" t="str">
         <f t="shared" si="232"/>
@@ -35130,7 +35130,7 @@
         <v/>
       </c>
       <c r="AR173" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="AS173" t="s">
         <v>295</v>
@@ -35196,7 +35196,7 @@
     </row>
     <row r="174" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C174" t="s">
         <v>426</v>
@@ -35205,7 +35205,7 @@
         <v>431</v>
       </c>
       <c r="G174" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="H174">
         <v>1600</v>
@@ -35250,7 +35250,7 @@
         <v>1800</v>
       </c>
       <c r="V174" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W174">
         <f t="shared" si="232"/>
@@ -35329,7 +35329,7 @@
         <v>4pm-6pm</v>
       </c>
       <c r="AR174" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="AU174" t="s">
         <v>298</v>
@@ -35392,19 +35392,19 @@
     </row>
     <row r="175" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C175" t="s">
         <v>426</v>
       </c>
       <c r="D175" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E175" t="s">
         <v>35</v>
       </c>
       <c r="G175" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J175">
         <v>1100</v>
@@ -35443,7 +35443,7 @@
         <v>1700</v>
       </c>
       <c r="V175" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="W175" t="str">
         <f t="shared" si="232"/>
@@ -35530,7 +35530,7 @@
         <v>11am-5pm</v>
       </c>
       <c r="AR175" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AU175" t="s">
         <v>298</v>
@@ -35593,13 +35593,13 @@
     </row>
     <row r="176" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C176" t="s">
         <v>426</v>
       </c>
       <c r="G176" s="7" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="W176" t="str">
         <f t="shared" si="232"/>
@@ -35686,7 +35686,7 @@
         <v/>
       </c>
       <c r="AR176" s="12" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="AU176" t="s">
         <v>298</v>
@@ -35749,19 +35749,19 @@
     </row>
     <row r="177" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C177" t="s">
         <v>426</v>
       </c>
       <c r="D177" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E177" t="s">
         <v>35</v>
       </c>
       <c r="G177" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="W177" t="str">
         <f t="shared" si="232"/>
@@ -35848,7 +35848,7 @@
         <v/>
       </c>
       <c r="AR177" s="12" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="AU177" t="s">
         <v>298</v>
@@ -35911,13 +35911,13 @@
     </row>
     <row r="178" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C178" t="s">
         <v>426</v>
       </c>
       <c r="G178" s="7" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="W178" t="str">
         <f t="shared" si="232"/>
@@ -36004,7 +36004,7 @@
         <v/>
       </c>
       <c r="AR178" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="AS178" t="s">
         <v>295</v>
@@ -36818,7 +36818,7 @@
     </row>
     <row r="183" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C183" t="s">
         <v>426</v>
@@ -36830,7 +36830,7 @@
         <v>54</v>
       </c>
       <c r="G183" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="J183">
         <v>1500</v>
@@ -37014,13 +37014,13 @@
     </row>
     <row r="184" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C184" t="s">
         <v>308</v>
       </c>
       <c r="G184" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="W184" t="str">
         <f t="shared" si="232"/>
@@ -37547,7 +37547,7 @@
     </row>
     <row r="187" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C187" t="s">
         <v>426</v>
@@ -37556,7 +37556,7 @@
         <v>431</v>
       </c>
       <c r="G187" s="7" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="W187" t="str">
         <f t="shared" ref="W187:W197" si="285">IF(H187&gt;0,H187/100,"")</f>
@@ -37635,7 +37635,7 @@
         <v/>
       </c>
       <c r="AR187" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AU187" t="s">
         <v>299</v>
@@ -37698,7 +37698,7 @@
     </row>
     <row r="188" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C188" t="s">
         <v>426</v>
@@ -37707,7 +37707,7 @@
         <v>54</v>
       </c>
       <c r="G188" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="W188" t="str">
         <f t="shared" si="285"/>
@@ -37786,7 +37786,7 @@
         <v/>
       </c>
       <c r="AR188" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="AS188" t="s">
         <v>295</v>
@@ -37852,13 +37852,13 @@
     </row>
     <row r="189" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C189" t="s">
         <v>429</v>
       </c>
       <c r="G189" s="7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="W189" t="str">
         <f t="shared" si="285"/>
@@ -37945,7 +37945,7 @@
         <v/>
       </c>
       <c r="AR189" s="12" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="AU189" t="s">
         <v>28</v>
@@ -38008,13 +38008,13 @@
     </row>
     <row r="190" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E190" t="s">
         <v>431</v>
       </c>
       <c r="G190" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="W190" t="str">
         <f t="shared" si="285"/>
@@ -38333,7 +38333,7 @@
     </row>
     <row r="192" spans="2:64" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C192" t="s">
         <v>309</v>
@@ -38345,7 +38345,7 @@
         <v>431</v>
       </c>
       <c r="G192" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="W192" t="str">
         <f t="shared" si="285"/>
@@ -38432,7 +38432,7 @@
         <v/>
       </c>
       <c r="AR192" s="12" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AS192" t="s">
         <v>295</v>
@@ -38498,13 +38498,13 @@
     </row>
     <row r="193" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C193" t="s">
         <v>309</v>
       </c>
       <c r="G193" s="7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J193">
         <v>1100</v>
@@ -38525,7 +38525,7 @@
         <v>2400</v>
       </c>
       <c r="V193" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="W193" t="str">
         <f t="shared" si="285"/>
@@ -38604,7 +38604,7 @@
         <v/>
       </c>
       <c r="AR193" s="12" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="AU193" t="s">
         <v>299</v>
@@ -38983,13 +38983,13 @@
     </row>
     <row r="196" spans="2:63" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C196" t="s">
         <v>429</v>
       </c>
       <c r="G196" s="7" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="W196" t="str">
         <f t="shared" si="285"/>
@@ -39068,7 +39068,7 @@
         <v/>
       </c>
       <c r="AR196" s="12" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AS196" t="s">
         <v>295</v>
@@ -39165,7 +39165,7 @@
         <v>1600</v>
       </c>
       <c r="V197" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="W197" t="str">
         <f t="shared" si="285"/>
@@ -39408,13 +39408,13 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>762</v>
+      </c>
+      <c r="C1" t="s">
         <v>763</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>764</v>
-      </c>
-      <c r="D1" t="s">
-        <v>765</v>
       </c>
       <c r="E1">
         <v>40.589424999999999</v>
@@ -39425,13 +39425,13 @@
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C2" t="s">
+        <v>763</v>
+      </c>
+      <c r="D2" t="s">
         <v>764</v>
-      </c>
-      <c r="D2" t="s">
-        <v>765</v>
       </c>
       <c r="E2">
         <v>40.589759999999998</v>
@@ -39442,13 +39442,13 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>766</v>
+      </c>
+      <c r="C3" t="s">
+        <v>763</v>
+      </c>
+      <c r="D3" t="s">
         <v>767</v>
-      </c>
-      <c r="C3" t="s">
-        <v>764</v>
-      </c>
-      <c r="D3" t="s">
-        <v>768</v>
       </c>
       <c r="E3">
         <v>40.523972999999998</v>
@@ -39459,13 +39459,13 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>768</v>
+      </c>
+      <c r="C4" t="s">
+        <v>763</v>
+      </c>
+      <c r="D4" t="s">
         <v>769</v>
-      </c>
-      <c r="C4" t="s">
-        <v>764</v>
-      </c>
-      <c r="D4" t="s">
-        <v>770</v>
       </c>
       <c r="E4">
         <v>40.551048999999999</v>
@@ -39476,13 +39476,13 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C5" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D5" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E5">
         <v>40.563256000000003</v>
@@ -39493,13 +39493,13 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C6" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D6" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E6">
         <v>40.527959000000003</v>
@@ -39510,13 +39510,13 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C7" t="s">
+        <v>763</v>
+      </c>
+      <c r="D7" t="s">
         <v>764</v>
-      </c>
-      <c r="D7" t="s">
-        <v>765</v>
       </c>
       <c r="E7">
         <v>40.586450999999997</v>

</xml_diff>